<commit_message>
Add skeleton for the \"Legend Plus\" panel
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/py/A_Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97D8583-3A1F-C943-AF86-DD355835AB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBD52FB-80A1-B745-985C-0E37E76B6EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23020" yWindow="-1820" windowWidth="20920" windowHeight="19100" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-34580" yWindow="940" windowWidth="18800" windowHeight="15940" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
-    <sheet name="Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Routes" sheetId="3" r:id="rId2"/>
+    <sheet name="Analysis" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cities!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cities!$A$1:$F$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="285">
   <si>
     <t>Num</t>
   </si>
@@ -675,6 +676,225 @@
   </si>
   <si>
     <t>States</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Autotrain</t>
+  </si>
+  <si>
+    <t>CO, ID, MT, UT, WY</t>
+  </si>
+  <si>
+    <t>MN, ND, SD, CAN</t>
+  </si>
+  <si>
+    <t>AL, GA, NC, SC, TN</t>
+  </si>
+  <si>
+    <t>AR, LA, MS, TN, TX</t>
+  </si>
+  <si>
+    <t>IL, IN, KY, MI, OH, PA, WI, WV</t>
+  </si>
+  <si>
+    <t>AR, IA, IL, KS, MO, NE, OK</t>
+  </si>
+  <si>
+    <t>AZ, NM, NV, TX, UT</t>
+  </si>
+  <si>
+    <t>CA, OR, WA, CAN</t>
+  </si>
+  <si>
+    <t>CA, NV</t>
+  </si>
+  <si>
+    <t>Hawaii State</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>MSP</t>
+  </si>
+  <si>
+    <t>DFW</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>LAX</t>
+  </si>
+  <si>
+    <t>LAS</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>YYZ</t>
+  </si>
+  <si>
+    <t>SJU</t>
+  </si>
+  <si>
+    <t>drive_mileage</t>
+  </si>
+  <si>
+    <t>trip_days</t>
+  </si>
+  <si>
+    <t>route</t>
+  </si>
+  <si>
+    <t>pre_travel</t>
+  </si>
+  <si>
+    <t>extra_days</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>best_temp_1</t>
+  </si>
+  <si>
+    <t>best_temp_2</t>
+  </si>
+  <si>
+    <t>Aug-Sep</t>
+  </si>
+  <si>
+    <t>Oct-Nov</t>
+  </si>
+  <si>
+    <t>Nov-Dec</t>
+  </si>
+  <si>
+    <t>Jul-Aug</t>
+  </si>
+  <si>
+    <t>May-Jun</t>
+  </si>
+  <si>
+    <t>Apr-May</t>
+  </si>
+  <si>
+    <t>Mar-Apr</t>
+  </si>
+  <si>
+    <t>Jan-Mar</t>
+  </si>
+  <si>
+    <t>Jan-Feb</t>
+  </si>
+  <si>
+    <t>bt1</t>
+  </si>
+  <si>
+    <t>bt2</t>
+  </si>
+  <si>
+    <t>Northeastern US + MD, DE, VA</t>
+  </si>
+  <si>
+    <t>states_etc</t>
+  </si>
+  <si>
+    <t>url1</t>
+  </si>
+  <si>
+    <t>url2</t>
+  </si>
+  <si>
+    <t>url3</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Toronto,+ON,+Canada/Ottawa,+ON,+Canada/Montreal,+QC,+Canada/Qu%C3%A9bec,+QC,+Canada/Montr%C3%A9al,+QC,+Canada/Toronto,+ON,+Canada/@45.1540678,-79.7807285,6z/data=!3m1!4b1!4m41!4m40!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!1m5!1m1!1s0x4cce05b25f5113af:0x8a6a51e131dd15ed!2m2!1d-75.6971931!2d45.4215296!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x4cb8968a05db8893:0x8fc52d63f0e83a03!2m2!1d-71.2079809!2d46.8138783!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Anchorage,+AK/Fairbanks,+AK/Anchorage,+AK/@63.8441792,-152.4627417,6.14z/data=!4m22!4m21!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!1m5!1m1!1s0x5132454f67fd65a9:0xb3d805e009fef73a!2m2!1d-147.7163888!2d64.8377778!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!2m1!2b1!3e0</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Denver,+CO/Grand+Junction,+CO/Salt+Lake+City,+UT/Boise,+ID/Idaho+Falls,+ID/Helena,+MT/Billings,+MT/Casper,+WY/Cheyenne,+WY/Denver,+Colorado/@42.4201276,-119.4822548,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!1m5!1m1!1s0x8746d6e322e77057:0xcc63f451cebf7c56!2m2!1d-108.5506486!2d39.0638705!1m5!1m1!1s0x87523d9488d131ed:0x5b53b7a0484d31ca!2m2!1d-111.8910474!2d40.7607793!1m5!1m1!1s0x54aef172e947b49d:0x9a5b989b36679d9b!2m2!1d-116.2023137!2d43.6150186!1m5!1m1!1s0x5354594e739512b5:0x2311c9fc094c49c9!2m2!1d-112.0407584!2d43.4926607!1m5!1m1!1s0x5343510fedc7db4d:0x214c1d71e3fdf714!2m2!1d-112.0391057!2d46.5891452!1m5!1m1!1s0x53486f8888fa9d97:0x373556d4f179b550!2m2!1d-108.5006904!2d45.7832856!1m5!1m1!1s0x87609365c85e7a63:0x69cefc3917343e53!2m2!1d-106.2980824!2d42.848709!1m5!1m1!1s0x876f38762e73ef93:0xb10a30418f972d2b!2m2!1d-104.8202462!2d41.1399814!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Minneapolis,+MN/Sioux+Falls,+SD/Pierre,+SD/Bismarck,+ND/Fargo,+ND/Winnipeg,+MB,+Canada/Duluth,+MN/Minneapolis,+MN/@46.6404497,-100.928197,6z/data=!3m1!4b1!4m53!4m52!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!1m5!1m1!1s0x878eb498e0bdacd7:0xde95ff3aa8b2fccf!2m2!1d-96.731265!2d43.5460223!1m5!1m1!1s0x52d54a64b288f891:0x9e9950165931af92!2m2!1d-100.3537522!2d44.3667876!1m5!1m1!1s0x52d7831257d8e963:0xccaabd12f9bbca93!2m2!1d-100.7837392!2d46.8083268!1m5!1m1!1s0x52c8cb8d84677145:0x81aa30a52791aaca!2m2!1d-96.7898034!2d46.8771863!1m5!1m1!1s0x52ea73fbf91a2b11:0x2b2a1afac6b9ca64!2m2!1d-97.1383744!2d49.895136!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Seattle,+WA/Vancouver,+BC,+Canada/Leavenworth,+WA/Spokane,+WA/Redding,+CA/Gold+Beach,+OR/Salem,+OR/Portland,+OR/Olympia,+WA/Seattle,+WA/@44.8374018,-125.1438928,6.26z/data=!4m65!4m64!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!1m5!1m1!1s0x548673f143a94fb3:0xbb9196ea9b81f38b!2m2!1d-123.1207375!2d49.2827291!1m5!1m1!1s0x549a4d92a4f8f98d:0xa14f95fb0abfef7e!2m2!1d-120.6614765!2d47.5962326!1m5!1m1!1s0x549e185c30bbe7e5:0xddfcc9d60b84d9b1!2m2!1d-117.4260465!2d47.6587802!1m5!1m1!1s0x54d291d63b4a202f:0x1f3358ec7b360f57!2m2!1d-122.3916754!2d40.5865396!1m5!1m1!1s0x54dace49bf9ae73d:0x121195079f68806d!2m2!1d-124.4217741!2d42.4073334!1m5!1m1!1s0x54bffefcbc4b9c63:0xf93429e08f0357c2!2m2!1d-123.0350963!2d44.9428975!1m5!1m1!1s0x54950b0b7da97427:0x1c36b9e6f6d18591!2m2!1d-122.6783853!2d45.515232!1m5!1m1!1s0x5491c9c1ae285569:0x4f146197e2881b83!2m2!1d-122.9006951!2d47.0378741!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Albany,+NY/Burlington,+VT/Montpelier,+VT/Concord,+NH/Augusta,+ME/Portland,+ME/Boston,+MA/Barnstable,+MA/Providence,+RI/Hartford,+CT/@41.8793352,-74.5474305,7z/data=!4m65!4m64!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!1m5!1m1!1s0x4cca7a55b69b55e5:0xc35fe519720e498e!2m2!1d-73.212072!2d44.4758825!1m5!1m1!1s0x4cb5a78cc44dea05:0x4891e094ceb5836!2m2!1d-72.5753869!2d44.2600593!1m5!1m1!1s0x89e26a96154a8917:0x5a871a0a62528f1!2m2!1d-71.5375718!2d43.2081366!1m5!1m1!1s0x4cb200fdafacc49d:0x79a3488d64220b2d!2m2!1d-69.7794897!2d44.3106241!1m5!1m1!1s0x4cb29c72aab0ee2d:0x7e9db6b53372fa29!2m2!1d-70.2568189!2d43.6590993!1m5!1m1!1s0x89e3652d0d3d311b:0x787cbf240162e8a0!2m2!1d-71.0588801!2d42.3600825!1m5!1m1!1s0x89fb33b67f8ec5e5:0xea7648efbb136d73!2m2!1d-70.3002024!2d41.7003208!1m5!1m1!1s0x89e444e0437e735d:0x69df7c4d48b3b627!2m2!1d-71.4128343!2d41.8239891!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Hartford,+CT/New+York,+NY/Trenton,+NJ/Philadelphia,+PA/Dover,+DE/Annapolis,+MD/Baltimore,+MD/Washington+D.C.,+DC/Richmond,+VA/Williamsburg,+VA/@39.5003974,-77.3244192,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!1m5!1m1!1s0x89c24fa5d33f083b:0xc80b8f06e177fe62!2m2!1d-74.0059728!2d40.7127753!1m5!1m1!1s0x89c143482d3dbbb9:0xcf16567f895cd7bc!2m2!1d-74.759717!2d40.2205824!1m5!1m1!1s0x89c6b7d8d4b54beb:0x89f514d88c3e58c1!2m2!1d-75.1652215!2d39.9525839!1m5!1m1!1s0x89c7633375685ead:0xa9e2e447fb006cf0!2m2!1d-75.5243682!2d39.158168!1m5!1m1!1s0x89b7f66570672fd5:0x43f854fdd3a8274b!2m2!1d-76.4921829!2d38.9784453!1m5!1m1!1s0x89c803aed6f483b7:0x44896a84223e758!2m2!1d-76.6121893!2d39.2903848!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x89b111095799c9ed:0xbfd83e6de2423cc5!2m2!1d-77.4360481!2d37.5407246!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Williamsburg,+VA/Norfolk,+VA/Charlottesville,+VA/Harrisburg,+PA/Buffalo,+NY/Rochester,+NY/Albany,+NY/@40.2169587,-81.2677638,5.7z/data=!4m47!4m46!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!1m5!1m1!1s0x89ba973a5322ca45:0xab99107fce7a1e0a!2m2!1d-76.2858726!2d36.8507689!1m5!1m1!1s0x89b3862dea50a48f:0x9086f096c38b74fc!2m2!1d-78.4766781!2d38.0293059!1m5!1m1!1s0x89c8c116b8079e97:0xbb6e42c8128d46d5!2m2!1d-76.8867008!2d40.2731911!1m5!1m1!1s0x89d3126152dfe5a1:0x982304a5181f8171!2m2!1d-78.8783689!2d42.8864468!1m5!1m1!1s0x89d6b3059614b353:0x5a001ffc4125e61e!2m2!1d-77.6088465!2d43.1565779!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Pittsburgh,+PA/Charleston,+WV/Columbus,+OH/Cincinnati,+OH/Frankfort,+KY/Louisville,+KY/Indianapolis,+IN/Chicago,+IL/Milwaukee,+WI/Madison,+WI/@40.5504662,-89.1782838,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!1m5!1m1!1s0x884f2cce88145d39:0x7661a84704c91b0b!2m2!1d-81.6326234!2d38.3498195!1m5!1m1!1s0x883889c1b990de71:0xe43266f8cfb1b533!2m2!1d-82.9987942!2d39.9611755!1m5!1m1!1s0x884051b1de3821f9:0x69fb7e8be4c09317!2m2!1d-84.5120196!2d39.1031182!1m5!1m1!1s0x8842734c8b1953c9:0x536418a08867425c!2m2!1d-84.8732835!2d38.2009055!1m5!1m1!1s0x88690b1ab35bd511:0xd4d3b4282071fd32!2m2!1d-85.7584557!2d38.2526647!1m5!1m1!1s0x886b50ffa7796a03:0xd68e9df640b9ea7c!2m2!1d-86.158068!2d39.768403!1m5!1m1!1s0x880e2c3cd0f4cbed:0xafe0a6ad09c0c000!2m2!1d-87.6297982!2d41.8781136!1m5!1m1!1s0x880502d7578b47e7:0x445f1922b5417b84!2m2!1d-87.9064736!2d43.0389025!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Madison,+Wisconsin/Green+Bay,+WI/Mackinaw+City,+MI/Grand+Rapids,+MI/Lansing,+MI/Frankenmuth,+MI/Detroit,+MI/Cleveland,+OH/Pittsburgh,+PA/@43.1918863,-89.1853954,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!1m5!1m1!1s0x8802e2e809b380f3:0x6370045214dcf571!2m2!1d-88.0132958!2d44.5133188!1m5!1m1!1s0x4d358b3940a9ad83:0xeac771ab20cc7a7a!2m2!1d-84.7271465!2d45.7774987!1m5!1m1!1s0x88185460bb502815:0xa593aacb1bd3a8d0!2m2!1d-85.6680863!2d42.9633599!1m5!1m1!1s0x8822c01c7f318c37:0x4378b62389029d9e!2m2!1d-84.5555347!2d42.732535!1m5!1m1!1s0x8823f287285df793:0x8050516199bcb01f!2m2!1d-83.7380194!2d43.331691!1m5!1m1!1s0x8824ca0110cb1d75:0x5776864e35b9c4d2!2m2!1d-83.0457538!2d42.331427!1m5!1m1!1s0x8830ef2ee3686b2d:0xed04cb55f7621842!2m2!1d-81.6943605!2d41.49932!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/San+Juan,+Puerto+Rico/@28.406847,-80.5870322,5z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x8c03686fe268196f:0xad6b7f0f5c935adc!2m2!1d-66.1057355!2d18.4655394!3e4</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/Honolulu,+HI/@24.8112769,-154.8564566,3z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x7c00183b8cc3464d:0x4b28f55ff3a7976c!2m2!1d-157.8583333!2d21.3069444!3e4</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Orlando,+FL/Miami,+FL/Key+West,+FL/Everglades+City,+FL/Tampa,+FL/Tarpon+Springs,+FL/Tallahassee,+FL/Jacksonville,+FL/St.+Augustine,+FL/Orlando,+FL/@27.5091232,-84.4177219,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!1m5!1m1!1s0x88d9b0a20ec8c111:0xff96f271ddad4f65!2m2!1d-80.1917902!2d25.7616798!1m5!1m1!1s0x88d1b134ad952377:0x3fcee92f77463b5e!2m2!1d-81.7799871!2d24.5550593!1m5!1m1!1s0x88da5c605ba45fb1:0x92bcf49fb504533a!2m2!1d-81.3850695!2d25.8582443!1m5!1m1!1s0x88c2b782b3b9d1e1:0xa75f1389af96b463!2m2!1d-82.4571776!2d27.950575!1m5!1m1!1s0x88c28cfd6f0942df:0xf4297f0ce0bf24b7!2m2!1d-82.7567679!2d28.1461248!1m5!1m1!1s0x88ec8a5187124b53:0xebee077ad4fdb1f8!2m2!1d-84.2807329!2d30.4382559!1m5!1m1!1s0x88e5b716f1ceafeb:0xc4cd7d3896fcc7e2!2m2!1d-81.655651!2d30.3321838!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Los+Angeles,+CA/Santa+Barbara,+CA/Solvang,+CA/San+Jose,+CA/San+Francisco,+CA/Sacramento,+CA/Reno,+NV/Virginia+City,+NV/Carson+City,+NV/Fresno,+CA/@36.7777641,-122.6363689,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!1m5!1m1!1s0x80e914c76f2d83d5:0xc8d13a64d7ba7648!2m2!1d-119.6981901!2d34.4208305!1m5!1m1!1s0x80e954a0fc922285:0x2d0e281b060bc156!2m2!1d-120.1376481!2d34.5958201!1m5!1m1!1s0x808fcae48af93ff5:0xb99d8c0aca9f717b!2m2!1d-121.8863286!2d37.3382082!1m5!1m1!1s0x80859a6d00690021:0x4a501367f076adff!2m2!1d-122.4194155!2d37.7749295!1m5!1m1!1s0x809ac672b28397f9:0x921f6aaa74197fdb!2m2!1d-121.4943996!2d38.5815719!1m5!1m1!1s0x809940ae9292a09d:0x40c5c5ce7438f787!2m2!1d-119.8138027!2d39.5296329!1m5!1m1!1s0x80990faad3daafd1:0x29dad257dc576fa9!2m2!1d-119.6499793!2d39.3095135!1m5!1m1!1s0x80990aa1f8deb471:0xf79c6c82bde23828!2m2!1d-119.7674034!2d39.1637984!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Fresno,+CA/Riverside,+CA/San+Diego,+CA/Los+Angeles,+CA/@34.7127545,-120.6716835,7z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!1m5!1m1!1s0x80dca6df7ff47dbb:0xf7a1d705135e0ae8!2m2!1d-117.3754942!2d33.9806005!1m5!1m1!1s0x80d9530fad921e4b:0xd3a21fdfd15df79!2m2!1d-117.1610838!2d32.715738!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Phoenix,+AZ/Sedona,+AZ/Las+Vegas,+NV/St.+George,+UT/Taos,+NM/Santa+Fe,+NM/Albuquerque,+NM/Lubbock,+TX/El+Paso,+TX/Tucson,+AZ/@34.1501088,-117.508012,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!1m5!1m1!1s0x872da132f942b00d:0x5548c523fa6c8efd!2m2!1d-111.7609896!2d34.8697395!1m5!1m1!1s0x80beb782a4f57dd1:0x3accd5e6d5b379a3!2m2!1d-115.1398296!2d36.1699412!1m5!1m1!1s0x80ca44d0984939e5:0x531707f2f8a11c1e!2m2!1d-113.5684164!2d37.0965278!1m5!1m1!1s0x871764da7f11fcb1:0x90ea918361a9b782!2m2!1d-105.5733788!2d36.4072134!1m5!1m1!1s0x87185043e79852a9:0x8c902373fd88df40!2m2!1d-105.937799!2d35.6869752!1m5!1m1!1s0x87220addd309837b:0xc0d3f8ceb8d9f6fd!2m2!1d-106.650422!2d35.0843859!1m5!1m1!1s0x86fe12add37ddd39:0x1af0042922e84287!2m2!1d-101.8551665!2d33.5778631!1m5!1m1!1s0x86e73f8bc5fe3b69:0xe39184e3ab9d0222!2m2!1d-106.4850217!2d31.7618778!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Tucson,+AZ/Phoenix,+AZ/@32.6659365,-112.3105217,7.68z/data=!4m17!4m16!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Dallas,+TX/Austin,+TX/San+Antonio,+TX/McAllen,+TX/Houston,+TX/Baton+Rouge,+LA/New+Orleans,+LA/Gulfport,+MS/Jackson,+MS/@29.4197283,-98.2903561,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!1m5!1m1!1s0x8644b599a0cc032f:0x5d9b464bd469d57a!2m2!1d-97.7430608!2d30.267153!1m5!1m1!1s0x865c58af04d00eaf:0x856e13b10a016bc!2m2!1d-98.4936282!2d29.4241219!1m5!1m1!1s0x866576324d9637df:0x2f1d39a9b52c0eb8!2m2!1d-98.2300124!2d26.2034071!1m5!1m1!1s0x8640b8b4488d8501:0xca0d02def365053b!2m2!1d-95.3698028!2d29.7604267!1m5!1m1!1s0x86243867325f74cb:0x2123f1db91579a1d!2m2!1d-91.1871466!2d30.4514677!1m5!1m1!1s0x8620a454b2118265:0xdb065be85e22d3b4!2m2!1d-90.0715323!2d29.9510658!1m5!1m1!1s0x889c166ee80114e5:0xc2614d446e819544!2m2!1d-89.0928155!2d30.3674198!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Jackson,+MS/Little+Rock,+AR/Fayetteville,+AR/Dallas,+TX/@32.5477822,-99.0081422,5.75z/data=!4m29!4m28!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!1m5!1m1!1s0x87d2a134a11f569b:0x3405f5100df35b17!2m2!1d-92.2895948!2d34.7464809!1m5!1m1!1s0x87c96f7b2fb53e9d:0x4519f069fcb4c8cf!2m2!1d-94.157853!2d36.0662419!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>SEA &gt; ANC</t>
+  </si>
+  <si>
+    <t>SFO &gt; HNL</t>
   </si>
 </sst>
 </file>
@@ -813,7 +1033,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,13 +1073,173 @@
     <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="28">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -926,7 +1306,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="44599.859887384257" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="129" xr:uid="{EA2F0253-6C76-7441-B1BF-F3AA56816A8F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="44609.611265740743" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="129" xr:uid="{EA2F0253-6C76-7441-B1BF-F3AA56816A8F}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G1048576" sheet="Cities"/>
   </cacheSource>
@@ -1015,26 +1395,13 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Visit" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1" count="3">
-        <n v="0"/>
-        <n v="1"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="Photo" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1" count="3">
-        <n v="0"/>
-        <n v="1"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="Score" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="2" count="4">
-        <n v="2"/>
-        <n v="1"/>
-        <n v="0"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="2"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1052,1167 +1419,1341 @@
     <s v="Anchorage AK"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="2"/>
     <s v="Fairbanks AK"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="3"/>
     <s v="Birmingham AL"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="4"/>
     <s v="Montgomery AL"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="5"/>
     <s v="Montreal CAN"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="6"/>
     <s v="Ottawa CAN"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="7"/>
     <s v="Quebec City CAN"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="8"/>
     <s v="Toronto CAN"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="9"/>
     <s v="Vancouver CAN"/>
     <x v="2"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="10"/>
     <s v="Winnipeg CAN"/>
     <x v="2"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="11"/>
     <s v="Fayetteville AR"/>
     <x v="3"/>
     <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="12"/>
     <s v="Little Rock AR"/>
     <x v="3"/>
     <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="13"/>
     <s v="Phoenix AZ"/>
     <x v="4"/>
     <x v="6"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="14"/>
     <s v="Tucson AZ"/>
     <x v="4"/>
     <x v="6"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="15"/>
     <s v="Fresno CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="16"/>
     <s v="Los Angeles CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="17"/>
     <s v="Riverside CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="18"/>
     <s v="Sacramento CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="19"/>
     <s v="San Diego CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="20"/>
     <s v="San Francisco CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="21"/>
     <s v="San Jose CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="22"/>
     <s v="Santa Barbara CA"/>
     <x v="5"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="23"/>
     <s v="Denver CO"/>
     <x v="6"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="24"/>
     <s v="Grand Junction CO"/>
     <x v="6"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="25"/>
     <s v="Hartford CT"/>
     <x v="7"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="26"/>
     <s v="Washington DC"/>
     <x v="8"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="27"/>
     <s v="Dover DE"/>
     <x v="9"/>
     <x v="9"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="28"/>
     <s v="Jacksonville FL"/>
     <x v="10"/>
     <x v="10"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="29"/>
     <s v="Key West FL"/>
     <x v="10"/>
     <x v="10"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="30"/>
     <s v="Miami FL"/>
     <x v="10"/>
     <x v="10"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="31"/>
     <s v="Orlando FL"/>
     <x v="10"/>
     <x v="10"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="32"/>
     <s v="Tallahassee FL"/>
     <x v="10"/>
     <x v="10"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="33"/>
     <s v="Tampa FL"/>
     <x v="10"/>
     <x v="10"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="34"/>
     <s v="Atlanta GA"/>
     <x v="11"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="35"/>
     <s v="Helen GA"/>
     <x v="11"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="36"/>
     <s v="Savannah GA"/>
     <x v="11"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="37"/>
     <s v="Honolulu HI"/>
     <x v="12"/>
     <x v="11"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="38"/>
     <s v="Davenport IA"/>
     <x v="13"/>
     <x v="12"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="39"/>
     <s v="Des Moines IA"/>
     <x v="13"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="40"/>
     <s v="Boise ID"/>
     <x v="14"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="41"/>
     <s v="Idaho Falls ID"/>
     <x v="14"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="42"/>
     <s v="Chicago IL"/>
     <x v="15"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="43"/>
     <s v="Springfield IL"/>
     <x v="15"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="44"/>
     <s v="Indianapolis IN"/>
     <x v="16"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="45"/>
     <s v="Topeka KS"/>
     <x v="17"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="46"/>
     <s v="Wichita KS"/>
     <x v="17"/>
     <x v="12"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="47"/>
     <s v="Frankfort KY"/>
     <x v="18"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="48"/>
     <s v="Louisville KY"/>
     <x v="18"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="49"/>
     <s v="Baton Rouge LA"/>
     <x v="19"/>
     <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="50"/>
     <s v="New Orleans LA"/>
     <x v="19"/>
     <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="51"/>
     <s v="Barnstable MA"/>
     <x v="20"/>
     <x v="9"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="52"/>
     <s v="Boston MA"/>
     <x v="20"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="53"/>
     <s v="Annapolis MD"/>
     <x v="21"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="54"/>
     <s v="Baltimore MD"/>
     <x v="21"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="55"/>
     <s v="Augusta ME"/>
     <x v="22"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="56"/>
     <s v="Portland ME"/>
     <x v="22"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="57"/>
     <s v="Detroit MI"/>
     <x v="23"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="58"/>
     <s v="Grand Rapids MI"/>
     <x v="23"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="59"/>
     <s v="Lansing MI"/>
     <x v="23"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="60"/>
     <s v="Duluth MN"/>
     <x v="24"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="61"/>
     <s v="Minneapolis MN"/>
     <x v="24"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="62"/>
     <s v="Jefferson City MO"/>
     <x v="25"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="63"/>
     <s v="Kansas City MO"/>
     <x v="25"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="64"/>
     <s v="St Louis MO"/>
     <x v="25"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="65"/>
     <s v="Gulfport MS"/>
     <x v="26"/>
     <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="66"/>
     <s v="Jackson MS"/>
     <x v="26"/>
     <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="67"/>
     <s v="Billings MT"/>
     <x v="27"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="68"/>
     <s v="Helena MT"/>
     <x v="27"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="69"/>
     <s v="Charlotte NC"/>
     <x v="28"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="70"/>
     <s v="Greensboro NC"/>
     <x v="28"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="71"/>
     <s v="Raleigh NC"/>
     <x v="28"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="72"/>
     <s v="Bismarck ND"/>
     <x v="29"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="73"/>
     <s v="Fargo ND"/>
     <x v="29"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="74"/>
     <s v="Lincoln NE"/>
     <x v="30"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="75"/>
     <s v="Omaha NE"/>
     <x v="30"/>
     <x v="12"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="76"/>
     <s v="Concord NH"/>
     <x v="31"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="77"/>
     <s v="Trenton NJ"/>
     <x v="32"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="78"/>
     <s v="Albuquerque NM"/>
     <x v="33"/>
     <x v="6"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="79"/>
     <s v="Santa Fe NM"/>
     <x v="33"/>
     <x v="6"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="80"/>
     <s v="Taos NM"/>
     <x v="33"/>
     <x v="6"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="81"/>
     <s v="Carson City NV"/>
     <x v="34"/>
     <x v="7"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="82"/>
     <s v="Las Vegas NV"/>
     <x v="34"/>
     <x v="6"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="83"/>
     <s v="Albany NY"/>
     <x v="35"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="84"/>
     <s v="Buffalo NY"/>
     <x v="35"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="85"/>
     <s v="New York NY"/>
     <x v="35"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="86"/>
     <s v="Rochester NY"/>
     <x v="35"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="87"/>
     <s v="Cincinnati OH"/>
     <x v="36"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="88"/>
     <s v="Cleveland OH"/>
     <x v="36"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="89"/>
     <s v="Columbus OH"/>
     <x v="36"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="90"/>
     <s v="Oklahoma City OK"/>
     <x v="37"/>
     <x v="12"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="91"/>
     <s v="Tulsa OK"/>
     <x v="37"/>
     <x v="12"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="92"/>
     <s v="Portland OR"/>
     <x v="38"/>
     <x v="3"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="93"/>
     <s v="Salem OR"/>
     <x v="38"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="94"/>
     <s v="Harrisburg PA"/>
     <x v="39"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="95"/>
     <s v="Philadelphia PA"/>
     <x v="39"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="96"/>
     <s v="Pittsburgh PA"/>
     <x v="39"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="97"/>
     <s v="San Juan PR"/>
     <x v="40"/>
     <x v="11"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="98"/>
     <s v="Providence RI"/>
     <x v="41"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="99"/>
     <s v="Charleston SC"/>
     <x v="42"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="100"/>
     <s v="Columbia SC"/>
     <x v="42"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="101"/>
     <s v="Pierre SD"/>
     <x v="43"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="102"/>
     <s v="Sioux Falls SD"/>
     <x v="43"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="103"/>
     <s v="Knoxville TN"/>
     <x v="44"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="104"/>
     <s v="Memphis TN"/>
     <x v="44"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="105"/>
     <s v="Nashville TN"/>
     <x v="44"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="106"/>
     <s v="Austin TX"/>
     <x v="45"/>
     <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="107"/>
     <s v="Dallas TX"/>
     <x v="45"/>
     <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="108"/>
     <s v="El Paso TX"/>
     <x v="45"/>
     <x v="6"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="109"/>
     <s v="Houston TX"/>
     <x v="45"/>
     <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="110"/>
     <s v="Lubbock TX"/>
     <x v="45"/>
     <x v="6"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="111"/>
     <s v="McAllen TX"/>
     <x v="45"/>
     <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="112"/>
     <s v="San Antonio TX"/>
     <x v="45"/>
     <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="113"/>
     <s v="Salt Lake City UT"/>
     <x v="46"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="114"/>
     <s v="St George UT"/>
     <x v="46"/>
     <x v="6"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="115"/>
     <s v="Charlottesville VA"/>
     <x v="47"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="116"/>
     <s v="Norfolk VA"/>
     <x v="47"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="117"/>
     <s v="Richmond VA"/>
     <x v="47"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="118"/>
     <s v="Burlington VT"/>
     <x v="48"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="119"/>
     <s v="Montpelier VT"/>
     <x v="48"/>
     <x v="9"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="120"/>
     <s v="Olympia WA"/>
     <x v="49"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="121"/>
     <s v="Seattle WA"/>
     <x v="49"/>
     <x v="3"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="122"/>
     <s v="Spokane WA"/>
     <x v="49"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="123"/>
     <s v="Green Bay WI"/>
     <x v="50"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="124"/>
     <s v="Madison WI"/>
     <x v="50"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="125"/>
     <s v="Milwaukee WI"/>
     <x v="50"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="126"/>
     <s v="Charleston WV"/>
     <x v="51"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <n v="127"/>
     <s v="Casper WY"/>
     <x v="52"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="128"/>
     <s v="Cheyenne WY"/>
     <x v="52"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <m/>
     <m/>
     <x v="53"/>
     <x v="14"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="3"/>
+    <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="0"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="13"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Sum of Visit" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Photo" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Score" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="7">
+    <format dxfId="27">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2277,31 +2818,9 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="2"/>
@@ -2488,245 +3007,6 @@
     <dataField name="Max of Visit" fld="4" subtotal="max" baseField="0" baseItem="0"/>
     <dataField name="Max of Photo" fld="5" subtotal="max" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="55">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="16">
-        <item x="0"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="10"/>
-        <item x="1"/>
-        <item x="13"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item x="6"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="11"/>
-        <item x="8"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Sum of Visit" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Photo" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Score" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="7">
-    <format dxfId="6">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3039,8 +3319,8 @@
   <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6273,7 +6553,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
+  <autoFilter ref="A1:F129" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F129">
       <sortCondition ref="A1:A129"/>
     </sortState>
@@ -6286,11 +6566,705 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1056</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D16" si="0">IF(B2="Drive",0,2)+_xlfn.CEILING.MATH(C2/200,1)+K2</f>
+        <v>10</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K2" s="1">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="1">
+        <v>719</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" s="1">
+        <f>(3*2)+3-2</f>
+        <v>7</v>
+      </c>
+      <c r="L3" s="1">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2211</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>6</v>
+      </c>
+      <c r="M4" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1610</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>6</v>
+      </c>
+      <c r="M5" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1955</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>6</v>
+      </c>
+      <c r="M6" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2403</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="M7" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="1">
+        <f>1097+1202+(234*2)</f>
+        <v>2767</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>4</v>
+      </c>
+      <c r="M8" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1963</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>5</v>
+      </c>
+      <c r="M9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="1">
+        <f>971+490</f>
+        <v>1461</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>5</v>
+      </c>
+      <c r="M10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="1">
+        <f>2228+113</f>
+        <v>2341</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="M11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="1">
+        <f>1947+(270*2)</f>
+        <v>2487</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>4</v>
+      </c>
+      <c r="M12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="1">
+        <f>1448+783</f>
+        <v>2231</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="M13" s="1">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1384</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2</v>
+      </c>
+      <c r="M14" s="1">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="1">
+        <f>(3*2)+3-2</f>
+        <v>7</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M15" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="1">
+        <f>(1*2)+3-2</f>
+        <v>3</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L16">
+    <sortCondition ref="L2:L16"/>
+    <sortCondition descending="1" ref="K2:K16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01B0898-0BB8-CE48-8A78-B23E3CEFACCF}">
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Make the route paths on the routes and travels panels; begin work on the opportunity panel
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBD52FB-80A1-B745-985C-0E37E76B6EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA0E59C-0811-4943-94FA-D76E9F3884AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34580" yWindow="940" windowWidth="18800" windowHeight="15940" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-24320" yWindow="-1240" windowWidth="18800" windowHeight="20520" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="287">
   <si>
     <t>Num</t>
   </si>
@@ -895,6 +895,12 @@
   </si>
   <si>
     <t>SFO &gt; HNL</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>lat</t>
   </si>
 </sst>
 </file>
@@ -1083,163 +1089,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -2579,7 +2429,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2682,10 +2532,10 @@
     <dataField name="Sum of Score" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="27">
+    <format dxfId="6">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2694,7 +2544,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2703,7 +2553,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2712,7 +2562,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2721,7 +2571,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2730,7 +2580,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2753,7 +2603,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3316,11 +3166,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3335,7 +3185,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3357,8 +3207,14 @@
       <c r="G1" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3382,8 +3238,14 @@
         <f>((1-E2)-(1-F2))+((1-F2)*2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>-149.9002778</v>
+      </c>
+      <c r="I2" s="1">
+        <v>61.2180556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3407,8 +3269,14 @@
         <f t="shared" ref="G3:G66" si="0">((1-E3)-(1-F3))+((1-F3)*2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>-147.7163889</v>
+      </c>
+      <c r="I3" s="1">
+        <v>64.837777799999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3432,8 +3300,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>-86.8103567</v>
+      </c>
+      <c r="I4" s="1">
+        <v>33.518589200000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3457,8 +3331,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>-86.307736800000001</v>
+      </c>
+      <c r="I5" s="1">
+        <v>32.3792233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3481,8 +3361,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>-73.554167000000007</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45.508889000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3505,8 +3391,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>-75.697193100000007</v>
+      </c>
+      <c r="I7" s="1">
+        <v>45.4215296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3529,8 +3421,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>-71.207980899999995</v>
+      </c>
+      <c r="I8" s="1">
+        <v>46.813878299999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3553,8 +3451,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>-79.383184299999996</v>
+      </c>
+      <c r="I9" s="1">
+        <v>43.653225999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3577,8 +3481,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <v>-123.1207375</v>
+      </c>
+      <c r="I10" s="1">
+        <v>49.282729099999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3601,8 +3511,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <v>-97.138374400000004</v>
+      </c>
+      <c r="I11" s="1">
+        <v>49.895136000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3626,8 +3542,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="1">
+        <v>-94.157853000000003</v>
+      </c>
+      <c r="I12" s="1">
+        <v>36.066241900000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3651,8 +3573,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="1">
+        <v>-92.289594800000003</v>
+      </c>
+      <c r="I13" s="1">
+        <v>34.746480900000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3676,8 +3604,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="1">
+        <v>-112.0740373</v>
+      </c>
+      <c r="I14" s="1">
+        <v>33.448377100000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3701,8 +3635,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="1">
+        <v>-110.9747108</v>
+      </c>
+      <c r="I15" s="1">
+        <v>32.222606599999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3726,8 +3666,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="1">
+        <v>-119.78712470000001</v>
+      </c>
+      <c r="I16" s="1">
+        <v>36.737798099999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3751,8 +3697,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="1">
+        <v>-118.24368490000001</v>
+      </c>
+      <c r="I17" s="1">
+        <v>34.052234200000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3776,8 +3728,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="1">
+        <v>-117.37549420000001</v>
+      </c>
+      <c r="I18" s="1">
+        <v>33.980600500000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3801,8 +3759,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="1">
+        <v>-121.49439959999999</v>
+      </c>
+      <c r="I19" s="1">
+        <v>38.5815719</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3826,8 +3790,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="1">
+        <v>-117.1610838</v>
+      </c>
+      <c r="I20" s="1">
+        <v>32.715738000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3851,8 +3821,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="1">
+        <v>-122.4194155</v>
+      </c>
+      <c r="I21" s="1">
+        <v>37.774929499999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3876,8 +3852,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="1">
+        <v>-121.8863286</v>
+      </c>
+      <c r="I22" s="1">
+        <v>37.338208199999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3901,8 +3883,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="1">
+        <v>-119.69819010000001</v>
+      </c>
+      <c r="I23" s="1">
+        <v>34.420830500000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3926,8 +3914,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="1">
+        <v>-104.990251</v>
+      </c>
+      <c r="I24" s="1">
+        <v>39.739235800000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3951,8 +3945,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="1">
+        <v>-108.5506486</v>
+      </c>
+      <c r="I25" s="1">
+        <v>39.0638705</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3976,8 +3976,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="1">
+        <v>-72.673372299999997</v>
+      </c>
+      <c r="I26" s="1">
+        <v>41.765804299999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -4001,8 +4007,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="1">
+        <v>-77.036870699999994</v>
+      </c>
+      <c r="I27" s="1">
+        <v>38.907192299999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -4026,8 +4038,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="1">
+        <v>-75.524368199999998</v>
+      </c>
+      <c r="I28" s="1">
+        <v>39.158168000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -4051,8 +4069,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="1">
+        <v>-81.655651000000006</v>
+      </c>
+      <c r="I29" s="1">
+        <v>30.332183799999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -4076,8 +4100,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="1">
+        <v>-81.7841722</v>
+      </c>
+      <c r="I30" s="1">
+        <v>24.555418299999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -4101,8 +4131,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="1">
+        <v>-80.1917902</v>
+      </c>
+      <c r="I31" s="1">
+        <v>25.7616798</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -4126,8 +4162,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="1">
+        <v>-81.378926899999996</v>
+      </c>
+      <c r="I32" s="1">
+        <v>28.538383199999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -4151,8 +4193,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="1">
+        <v>-84.280732900000004</v>
+      </c>
+      <c r="I33" s="1">
+        <v>30.438255900000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -4176,8 +4224,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" s="1">
+        <v>-82.457177599999994</v>
+      </c>
+      <c r="I34" s="1">
+        <v>27.950575000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -4201,8 +4255,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="1">
+        <v>-84.387982399999999</v>
+      </c>
+      <c r="I35" s="1">
+        <v>33.748995399999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -4226,8 +4286,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="1">
+        <v>-83.731567499999997</v>
+      </c>
+      <c r="I36" s="1">
+        <v>34.701483899999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -4251,8 +4317,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="1">
+        <v>-81.091202999999993</v>
+      </c>
+      <c r="I37" s="1">
+        <v>32.080898900000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -4276,8 +4348,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="1">
+        <v>-157.8583333</v>
+      </c>
+      <c r="I38" s="1">
+        <v>21.306944399999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -4301,8 +4379,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="1">
+        <v>-90.577636699999999</v>
+      </c>
+      <c r="I39" s="1">
+        <v>41.523643700000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -4326,8 +4410,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="1">
+        <v>-93.6249593</v>
+      </c>
+      <c r="I40" s="1">
+        <v>41.586835299999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -4351,8 +4441,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="1">
+        <v>-116.2023137</v>
+      </c>
+      <c r="I41" s="1">
+        <v>43.615018599999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -4376,8 +4472,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" s="1">
+        <v>-112.0407584</v>
+      </c>
+      <c r="I42" s="1">
+        <v>43.492660700000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -4401,8 +4503,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" s="1">
+        <v>-87.629798199999996</v>
+      </c>
+      <c r="I43" s="1">
+        <v>41.878113599999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -4426,8 +4534,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" s="1">
+        <v>-89.650148099999996</v>
+      </c>
+      <c r="I44" s="1">
+        <v>39.781721300000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -4451,8 +4565,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" s="1">
+        <v>-86.158068</v>
+      </c>
+      <c r="I45" s="1">
+        <v>39.768402999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -4476,8 +4596,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" s="1">
+        <v>-95.675157600000006</v>
+      </c>
+      <c r="I46" s="1">
+        <v>39.047345100000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -4501,8 +4627,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" s="1">
+        <v>-97.330053000000007</v>
+      </c>
+      <c r="I47" s="1">
+        <v>37.687176100000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -4526,8 +4658,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="1">
+        <v>-84.873283499999999</v>
+      </c>
+      <c r="I48" s="1">
+        <v>38.200905499999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -4551,8 +4689,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" s="1">
+        <v>-85.758455699999999</v>
+      </c>
+      <c r="I49" s="1">
+        <v>38.252664699999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -4576,8 +4720,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="1">
+        <v>-91.187146600000005</v>
+      </c>
+      <c r="I50" s="1">
+        <v>30.451467699999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -4601,8 +4751,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="1">
+        <v>-90.071532300000001</v>
+      </c>
+      <c r="I51" s="1">
+        <v>29.951065799999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -4626,8 +4782,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="1">
+        <v>-70.300202400000003</v>
+      </c>
+      <c r="I52" s="1">
+        <v>41.7003208</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4651,8 +4813,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="1">
+        <v>-71.058880099999996</v>
+      </c>
+      <c r="I53" s="1">
+        <v>42.360082499999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4676,8 +4844,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="1">
+        <v>-76.492182900000003</v>
+      </c>
+      <c r="I54" s="1">
+        <v>38.978445299999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -4701,8 +4875,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="1">
+        <v>-76.612189299999997</v>
+      </c>
+      <c r="I55" s="1">
+        <v>39.290384799999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4726,8 +4906,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="1">
+        <v>-69.779489699999999</v>
+      </c>
+      <c r="I56" s="1">
+        <v>44.310624099999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4751,8 +4937,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="1">
+        <v>-70.256818899999999</v>
+      </c>
+      <c r="I57" s="1">
+        <v>43.659099300000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4776,8 +4968,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="1">
+        <v>-83.0457538</v>
+      </c>
+      <c r="I58" s="1">
+        <v>42.331426999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4801,8 +4999,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="1">
+        <v>-85.668086299999999</v>
+      </c>
+      <c r="I59" s="1">
+        <v>42.9633599</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4826,8 +5030,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="1">
+        <v>-84.555534699999995</v>
+      </c>
+      <c r="I60" s="1">
+        <v>42.732534999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4851,8 +5061,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="1">
+        <v>-92.100485199999994</v>
+      </c>
+      <c r="I61" s="1">
+        <v>46.786671900000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4876,8 +5092,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="1">
+        <v>-93.265010799999999</v>
+      </c>
+      <c r="I62" s="1">
+        <v>44.977753</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4901,8 +5123,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="1">
+        <v>-92.173516399999997</v>
+      </c>
+      <c r="I63" s="1">
+        <v>38.576701700000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4926,8 +5154,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64" s="1">
+        <v>-94.578566699999996</v>
+      </c>
+      <c r="I64" s="1">
+        <v>39.099726500000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4951,8 +5185,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65" s="1">
+        <v>-90.199404200000004</v>
+      </c>
+      <c r="I65" s="1">
+        <v>38.627002500000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4976,8 +5216,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" s="1">
+        <v>-89.0928155</v>
+      </c>
+      <c r="I66" s="1">
+        <v>30.3674198</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
         <v>66</v>
       </c>
@@ -5001,8 +5247,14 @@
         <f t="shared" ref="G67:G129" si="3">((1-E67)-(1-F67))+((1-F67)*2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67" s="1">
+        <v>-90.184810299999995</v>
+      </c>
+      <c r="I67" s="1">
+        <v>32.298757299999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -5026,8 +5278,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68" s="1">
+        <v>-108.5006904</v>
+      </c>
+      <c r="I68" s="1">
+        <v>45.783285599999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -5051,8 +5309,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69" s="1">
+        <v>-112.03910569999999</v>
+      </c>
+      <c r="I69" s="1">
+        <v>46.589145199999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -5076,8 +5340,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70" s="1">
+        <v>-80.843126699999999</v>
+      </c>
+      <c r="I70" s="1">
+        <v>35.227086900000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -5101,8 +5371,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71" s="1">
+        <v>-79.791975399999998</v>
+      </c>
+      <c r="I71" s="1">
+        <v>36.072635400000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -5126,8 +5402,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72" s="1">
+        <v>-78.638178699999997</v>
+      </c>
+      <c r="I72" s="1">
+        <v>35.779589700000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -5151,8 +5433,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73" s="1">
+        <v>-100.7837392</v>
+      </c>
+      <c r="I73" s="1">
+        <v>46.808326800000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -5176,8 +5464,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74" s="1">
+        <v>-96.789803399999997</v>
+      </c>
+      <c r="I74" s="1">
+        <v>46.877186299999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -5201,8 +5495,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75" s="1">
+        <v>-96.702595500000001</v>
+      </c>
+      <c r="I75" s="1">
+        <v>40.813616000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -5226,8 +5526,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H76" s="1">
+        <v>-95.934503399999997</v>
+      </c>
+      <c r="I76" s="1">
+        <v>41.2565369</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -5251,8 +5557,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77" s="1">
+        <v>-71.537571799999995</v>
+      </c>
+      <c r="I77" s="1">
+        <v>43.208136600000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -5276,8 +5588,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78" s="1">
+        <v>-74.759716999999995</v>
+      </c>
+      <c r="I78" s="1">
+        <v>40.220582399999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -5301,8 +5619,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79" s="1">
+        <v>-106.65042200000001</v>
+      </c>
+      <c r="I79" s="1">
+        <v>35.084385900000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -5326,8 +5650,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" s="1">
+        <v>-105.937799</v>
+      </c>
+      <c r="I80" s="1">
+        <v>35.686975199999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -5351,8 +5681,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81" s="1">
+        <v>-105.5733788</v>
+      </c>
+      <c r="I81" s="1">
+        <v>36.407213400000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -5376,8 +5712,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82" s="1">
+        <v>-119.76740340000001</v>
+      </c>
+      <c r="I82" s="1">
+        <v>39.163798399999997</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -5401,8 +5743,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" s="1">
+        <v>-115.1398296</v>
+      </c>
+      <c r="I83" s="1">
+        <v>36.169941199999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -5426,8 +5774,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84" s="1">
+        <v>-73.756231700000001</v>
+      </c>
+      <c r="I84" s="1">
+        <v>42.652579299999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -5451,8 +5805,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" s="1">
+        <v>-78.878368899999998</v>
+      </c>
+      <c r="I85" s="1">
+        <v>42.886446800000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -5476,8 +5836,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86" s="1">
+        <v>-74.005972799999995</v>
+      </c>
+      <c r="I86" s="1">
+        <v>40.712775299999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -5501,8 +5867,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87" s="1">
+        <v>-77.608846499999999</v>
+      </c>
+      <c r="I87" s="1">
+        <v>43.156577900000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -5526,8 +5898,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88" s="1">
+        <v>-84.512019600000002</v>
+      </c>
+      <c r="I88" s="1">
+        <v>39.103118199999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -5551,8 +5929,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89" s="1">
+        <v>-81.694360500000002</v>
+      </c>
+      <c r="I89" s="1">
+        <v>41.499319999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -5576,8 +5960,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90" s="1">
+        <v>-82.998794200000006</v>
+      </c>
+      <c r="I90" s="1">
+        <v>39.961175500000003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -5601,8 +5991,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91" s="1">
+        <v>-97.5164276</v>
+      </c>
+      <c r="I91" s="1">
+        <v>35.467560200000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -5626,8 +6022,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" s="1">
+        <v>-95.992774999999995</v>
+      </c>
+      <c r="I92" s="1">
+        <v>36.153981600000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -5651,8 +6053,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" s="1">
+        <v>-122.6783853</v>
+      </c>
+      <c r="I93" s="1">
+        <v>45.515231999999997</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -5676,8 +6084,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" s="1">
+        <v>-123.03509630000001</v>
+      </c>
+      <c r="I94" s="1">
+        <v>44.942897500000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -5701,8 +6115,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95" s="1">
+        <v>-76.8867008</v>
+      </c>
+      <c r="I95" s="1">
+        <v>40.273191099999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -5726,8 +6146,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96" s="1">
+        <v>-75.165221500000001</v>
+      </c>
+      <c r="I96" s="1">
+        <v>39.9525839</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -5751,8 +6177,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97" s="1">
+        <v>-79.995886400000003</v>
+      </c>
+      <c r="I97" s="1">
+        <v>40.440624800000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -5776,8 +6208,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98" s="1">
+        <v>-66.105735499999994</v>
+      </c>
+      <c r="I98" s="1">
+        <v>18.465539400000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -5801,8 +6239,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" s="1">
+        <v>-71.4128343</v>
+      </c>
+      <c r="I99" s="1">
+        <v>41.823989099999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -5826,8 +6270,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" s="1">
+        <v>-79.931051199999999</v>
+      </c>
+      <c r="I100" s="1">
+        <v>32.776474899999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5851,8 +6301,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" s="1">
+        <v>-81.034814400000002</v>
+      </c>
+      <c r="I101" s="1">
+        <v>34.000710400000003</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -5876,8 +6332,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="1">
+        <v>-100.3537522</v>
+      </c>
+      <c r="I102" s="1">
+        <v>44.366787600000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -5901,8 +6363,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" s="1">
+        <v>-96.731264999999993</v>
+      </c>
+      <c r="I103" s="1">
+        <v>43.546022299999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -5926,8 +6394,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" s="1">
+        <v>-83.9207392</v>
+      </c>
+      <c r="I104" s="1">
+        <v>35.960638400000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -5951,8 +6425,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105" s="1">
+        <v>-90.048980099999994</v>
+      </c>
+      <c r="I105" s="1">
+        <v>35.149534299999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -5976,8 +6456,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106" s="1">
+        <v>-86.781601600000002</v>
+      </c>
+      <c r="I106" s="1">
+        <v>36.162663799999997</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -6001,8 +6487,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" s="1">
+        <v>-97.743060799999995</v>
+      </c>
+      <c r="I107" s="1">
+        <v>30.267153</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -6026,8 +6518,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108" s="1">
+        <v>-96.796987900000005</v>
+      </c>
+      <c r="I108" s="1">
+        <v>32.776664199999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -6051,8 +6549,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H109" s="1">
+        <v>-106.4850217</v>
+      </c>
+      <c r="I109" s="1">
+        <v>31.761877800000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -6076,8 +6580,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110" s="1">
+        <v>-95.369802800000002</v>
+      </c>
+      <c r="I110" s="1">
+        <v>29.7604267</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -6101,8 +6611,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111" s="1">
+        <v>-101.8551665</v>
+      </c>
+      <c r="I111" s="1">
+        <v>33.577863100000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -6126,8 +6642,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" s="1">
+        <v>-98.230012400000007</v>
+      </c>
+      <c r="I112" s="1">
+        <v>26.2034071</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -6151,8 +6673,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" s="1">
+        <v>-98.493628200000003</v>
+      </c>
+      <c r="I113" s="1">
+        <v>29.424121899999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -6176,8 +6704,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" s="1">
+        <v>-111.89104740000001</v>
+      </c>
+      <c r="I114" s="1">
+        <v>40.760779300000003</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -6201,8 +6735,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H115" s="1">
+        <v>-113.5684164</v>
+      </c>
+      <c r="I115" s="1">
+        <v>37.096527799999997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -6226,8 +6766,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H116" s="1">
+        <v>-78.476678100000001</v>
+      </c>
+      <c r="I116" s="1">
+        <v>38.029305899999997</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -6251,8 +6797,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H117" s="1">
+        <v>-76.285872600000005</v>
+      </c>
+      <c r="I117" s="1">
+        <v>36.850768899999998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -6276,8 +6828,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H118" s="1">
+        <v>-77.436048099999994</v>
+      </c>
+      <c r="I118" s="1">
+        <v>37.540724599999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -6301,8 +6859,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H119" s="1">
+        <v>-73.212072000000006</v>
+      </c>
+      <c r="I119" s="1">
+        <v>44.475882499999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -6326,8 +6890,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H120" s="1">
+        <v>-72.575386899999998</v>
+      </c>
+      <c r="I120" s="1">
+        <v>44.260059300000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -6351,8 +6921,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H121" s="1">
+        <v>-122.90069509999999</v>
+      </c>
+      <c r="I121" s="1">
+        <v>47.037874100000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -6376,8 +6952,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H122" s="1">
+        <v>-122.3320708</v>
+      </c>
+      <c r="I122" s="1">
+        <v>47.606209499999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -6401,8 +6983,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H123" s="1">
+        <v>-117.42604660000001</v>
+      </c>
+      <c r="I123" s="1">
+        <v>47.658780200000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -6426,8 +7014,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H124" s="1">
+        <v>-88.013295799999995</v>
+      </c>
+      <c r="I124" s="1">
+        <v>44.5133188</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -6451,8 +7045,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H125" s="1">
+        <v>-89.401230200000001</v>
+      </c>
+      <c r="I125" s="1">
+        <v>43.073051700000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -6476,8 +7076,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H126" s="1">
+        <v>-87.906473599999998</v>
+      </c>
+      <c r="I126" s="1">
+        <v>43.038902499999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -6501,8 +7107,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H127" s="1">
+        <v>-81.6326234</v>
+      </c>
+      <c r="I127" s="1">
+        <v>38.349819500000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -6526,8 +7138,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H128" s="1">
+        <v>-106.2980824</v>
+      </c>
+      <c r="I128" s="1">
+        <v>42.848708999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -6550,6 +7168,12 @@
       <c r="G129" s="1">
         <f t="shared" si="3"/>
         <v>2</v>
+      </c>
+      <c r="H129" s="1">
+        <v>-104.8202462</v>
+      </c>
+      <c r="I129" s="1">
+        <v>41.139981400000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create skeleton for the opportunity panel
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA0E59C-0811-4943-94FA-D76E9F3884AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9129A5-D53A-F447-8DE4-B460B1A6C17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24320" yWindow="-1240" windowWidth="18800" windowHeight="20520" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
@@ -3169,8 +3169,8 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I52" sqref="H52:I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Building quality testing infrastructure; build quality tests for the Data Imports functions and the explanation panel
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9129A5-D53A-F447-8DE4-B460B1A6C17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F61CAB8-6F67-F34C-AA82-B5B21BACA3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24320" yWindow="-1240" windowWidth="18800" windowHeight="20520" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-35580" yWindow="-1760" windowWidth="18800" windowHeight="20520" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="289">
   <si>
     <t>Num</t>
   </si>
@@ -901,6 +901,12 @@
   </si>
   <si>
     <t>lat</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Atlanta,+GA/Helen,+GA/Nashville,+TN/Knoxville,+TN/Charlotte,+NC/Greensboro,+NC/Raleigh,+NC/Columbia,+SC/Charleston,+SC/Savannah,+GA/@34.0640266,-87.1468938,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!1m5!1m1!1s0x885f37d40b3a2aa1:0x8ed537fed96523a8!2m2!1d-83.7315675!2d34.7014839!1m5!1m1!1s0x8864ec3213eb903d:0x7d3fb9d0a1e9daa0!2m2!1d-86.7816016!2d36.1626638!1m5!1m1!1s0x885c162246ce42a9:0x7bea92dac4f534c5!2m2!1d-83.9207392!2d35.9606384!1m5!1m1!1s0x88541fc4fc381a81:0x884650e6bf43d164!2m2!1d-80.8431267!2d35.2270869!1m5!1m1!1s0x8853193f38c77b79:0x93b9c49478be12c8!2m2!1d-79.7919754!2d36.0726354!1m5!1m1!1s0x89ac5a2f9f51e0f7:0x6790b6528a11f0ad!2m2!1d-78.6381787!2d35.7795897!1m5!1m1!1s0x88f8a5697931d1e3:0xf32808f4b379fa96!2m2!1d-81.0348144!2d34.0007104!1m5!1m1!1s0x88fe7a42dca82477:0x35faf7e0aee1ec6b!2m2!1d-79.9310512!2d32.7764749!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1095,131 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -1156,7 +1286,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="44609.611265740743" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="129" xr:uid="{EA2F0253-6C76-7441-B1BF-F3AA56816A8F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="44614.534418055555" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="129" xr:uid="{EA2F0253-6C76-7441-B1BF-F3AA56816A8F}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G1048576" sheet="Cities"/>
   </cacheSource>
@@ -2195,7 +2325,7 @@
     <n v="104"/>
     <s v="Memphis TN"/>
     <x v="44"/>
-    <x v="1"/>
+    <x v="5"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -2429,7 +2559,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2531,11 +2661,11 @@
     <dataField name="Sum of Photo" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Sum of Score" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="7">
-    <format dxfId="6">
+  <formats count="9">
+    <format dxfId="24">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2544,7 +2674,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2553,7 +2683,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2562,7 +2692,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2571,7 +2701,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2580,11 +2710,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
             <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -2603,7 +2751,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3168,9 +3316,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I52" sqref="H52:I52"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6413,7 +6561,7 @@
         <v>TN</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E105" s="1">
         <v>0</v>
@@ -7193,8 +7341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7515,8 +7663,8 @@
         <v>212</v>
       </c>
       <c r="C8" s="1">
-        <f>1097+1202+(234*2)</f>
-        <v>2767</v>
+        <f>1097+1202+(237*2)</f>
+        <v>2773</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
@@ -7680,8 +7828,8 @@
         <v>212</v>
       </c>
       <c r="C12" s="1">
-        <f>1947+(270*2)</f>
-        <v>2487</v>
+        <f>1951+(278*2)</f>
+        <v>2507</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
@@ -7696,9 +7844,15 @@
       <c r="G12" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
+      <c r="H12" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>264</v>
+      </c>
       <c r="K12" s="1">
         <v>0</v>
       </c>
@@ -7888,7 +8042,7 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8030,7 +8184,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="20">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -8056,17 +8210,17 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="20">
         <v>7</v>
       </c>
-      <c r="C8" s="8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="8">
-        <v>15</v>
+      <c r="C8" s="20">
+        <v>0</v>
+      </c>
+      <c r="D8" s="20">
+        <v>17</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>

</xml_diff>

<commit_message>
Flesh out quality testing and streamline/centralize text functionality
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F61CAB8-6F67-F34C-AA82-B5B21BACA3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08215EB9-2A55-7D45-8481-B7322E1E8EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35580" yWindow="-1760" windowWidth="18800" windowHeight="20520" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-33440" yWindow="-1820" windowWidth="18800" windowHeight="20520" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -678,9 +678,6 @@
     <t>States</t>
   </si>
   <si>
-    <t>Drive</t>
-  </si>
-  <si>
     <t>Autotrain</t>
   </si>
   <si>
@@ -816,9 +813,6 @@
     <t>bt2</t>
   </si>
   <si>
-    <t>Northeastern US + MD, DE, VA</t>
-  </si>
-  <si>
     <t>states_etc</t>
   </si>
   <si>
@@ -891,12 +885,6 @@
     <t>https://www.google.com/maps/dir/Jackson,+MS/Little+Rock,+AR/Fayetteville,+AR/Dallas,+TX/@32.5477822,-99.0081422,5.75z/data=!4m29!4m28!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!1m5!1m1!1s0x87d2a134a11f569b:0x3405f5100df35b17!2m2!1d-92.2895948!2d34.7464809!1m5!1m1!1s0x87c96f7b2fb53e9d:0x4519f069fcb4c8cf!2m2!1d-94.157853!2d36.0662419!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!2m1!2b1!3e0!4e1</t>
   </si>
   <si>
-    <t>SEA &gt; ANC</t>
-  </si>
-  <si>
-    <t>SFO &gt; HNL</t>
-  </si>
-  <si>
     <t>lon</t>
   </si>
   <si>
@@ -907,6 +895,18 @@
   </si>
   <si>
     <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>Northeast + MD, DE, VA</t>
+  </si>
+  <si>
+    <t>SFO, HNL</t>
+  </si>
+  <si>
+    <t>SEA, ANC</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1095,121 +1095,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -2559,7 +2445,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2662,10 +2548,10 @@
     <dataField name="Sum of Score" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="9">
-    <format dxfId="24">
+    <format dxfId="8">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2674,7 +2560,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2683,7 +2569,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2692,7 +2578,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2701,7 +2587,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2710,7 +2596,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2719,7 +2605,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2728,7 +2614,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2751,7 +2637,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3317,8 +3203,8 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3356,10 +3242,10 @@
         <v>152</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4484,7 +4370,7 @@
         <v>HI</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>144</v>
+        <v>222</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -6344,7 +6230,7 @@
         <v>PR</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>144</v>
+        <v>223</v>
       </c>
       <c r="E98" s="1">
         <v>1</v>
@@ -7342,7 +7228,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7362,43 +7248,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -7406,7 +7292,7 @@
         <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C2" s="1">
         <v>1056</v>
@@ -7416,22 +7302,22 @@
         <v>10</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>134</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K2" s="1">
         <f>2</f>
@@ -7449,7 +7335,7 @@
         <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1">
         <v>719</v>
@@ -7459,22 +7345,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>153</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K3" s="1">
         <f>(3*2)+3-2</f>
@@ -7492,7 +7378,7 @@
         <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="1">
         <v>2211</v>
@@ -7502,22 +7388,22 @@
         <v>14</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -7534,7 +7420,7 @@
         <v>133</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C5" s="1">
         <v>1610</v>
@@ -7544,22 +7430,22 @@
         <v>11</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -7576,7 +7462,7 @@
         <v>141</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C6" s="1">
         <v>1955</v>
@@ -7586,22 +7472,22 @@
         <v>12</v>
       </c>
       <c r="E6" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -7618,32 +7504,32 @@
         <v>206</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>212</v>
+        <v>288</v>
       </c>
       <c r="C7" s="1">
         <v>2403</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="H7" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="J7" s="24" t="s">
         <v>269</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>271</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
@@ -7660,7 +7546,7 @@
         <v>132</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>288</v>
       </c>
       <c r="C8" s="1">
         <f>1097+1202+(237*2)</f>
@@ -7668,25 +7554,25 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -7703,7 +7589,7 @@
         <v>135</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C9" s="1">
         <v>1963</v>
@@ -7713,13 +7599,13 @@
         <v>12</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
@@ -7739,7 +7625,7 @@
         <v>140</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="1">
         <f>971+490</f>
@@ -7750,22 +7636,22 @@
         <v>10</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -7782,7 +7668,7 @@
         <v>139</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C11" s="1">
         <f>2228+113</f>
@@ -7793,22 +7679,22 @@
         <v>14</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
@@ -7825,7 +7711,7 @@
         <v>130</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>212</v>
+        <v>288</v>
       </c>
       <c r="C12" s="1">
         <f>1951+(278*2)</f>
@@ -7833,25 +7719,25 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
@@ -7868,7 +7754,7 @@
         <v>137</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C13" s="1">
         <f>1448+783</f>
@@ -7879,22 +7765,22 @@
         <v>14</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
@@ -7911,7 +7797,7 @@
         <v>131</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C14" s="1">
         <v>1384</v>
@@ -7921,19 +7807,19 @@
         <v>9</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>162</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J14" s="23"/>
       <c r="K14" s="1">
@@ -7948,10 +7834,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -7961,19 +7847,19 @@
         <v>9</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>164</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J15" s="23"/>
       <c r="K15" s="1">
@@ -7989,10 +7875,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -8002,19 +7888,19 @@
         <v>5</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>192</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="1">

</xml_diff>

<commit_message>
Update information table with weather findings from the travel_weather project
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6D4078-BD9F-E740-A2E3-0E1319B78EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED0102F-A671-AF48-8C77-4BD13E1DDDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3220" windowWidth="20620" windowHeight="14260" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-34280" yWindow="2120" windowWidth="20400" windowHeight="11660" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="286">
   <si>
     <t>Num</t>
   </si>
@@ -759,154 +759,145 @@
     <t>Dec</t>
   </si>
   <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>best_temp_1</t>
+  </si>
+  <si>
+    <t>best_temp_2</t>
+  </si>
+  <si>
+    <t>bt1</t>
+  </si>
+  <si>
+    <t>bt2</t>
+  </si>
+  <si>
+    <t>states_etc</t>
+  </si>
+  <si>
+    <t>url1</t>
+  </si>
+  <si>
+    <t>url2</t>
+  </si>
+  <si>
+    <t>url3</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Toronto,+ON,+Canada/Ottawa,+ON,+Canada/Montreal,+QC,+Canada/Qu%C3%A9bec,+QC,+Canada/Montr%C3%A9al,+QC,+Canada/Toronto,+ON,+Canada/@45.1540678,-79.7807285,6z/data=!3m1!4b1!4m41!4m40!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!1m5!1m1!1s0x4cce05b25f5113af:0x8a6a51e131dd15ed!2m2!1d-75.6971931!2d45.4215296!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x4cb8968a05db8893:0x8fc52d63f0e83a03!2m2!1d-71.2079809!2d46.8138783!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Anchorage,+AK/Fairbanks,+AK/Anchorage,+AK/@63.8441792,-152.4627417,6.14z/data=!4m22!4m21!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!1m5!1m1!1s0x5132454f67fd65a9:0xb3d805e009fef73a!2m2!1d-147.7163888!2d64.8377778!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!2m1!2b1!3e0</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Denver,+CO/Grand+Junction,+CO/Salt+Lake+City,+UT/Boise,+ID/Idaho+Falls,+ID/Helena,+MT/Billings,+MT/Casper,+WY/Cheyenne,+WY/Denver,+Colorado/@42.4201276,-119.4822548,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!1m5!1m1!1s0x8746d6e322e77057:0xcc63f451cebf7c56!2m2!1d-108.5506486!2d39.0638705!1m5!1m1!1s0x87523d9488d131ed:0x5b53b7a0484d31ca!2m2!1d-111.8910474!2d40.7607793!1m5!1m1!1s0x54aef172e947b49d:0x9a5b989b36679d9b!2m2!1d-116.2023137!2d43.6150186!1m5!1m1!1s0x5354594e739512b5:0x2311c9fc094c49c9!2m2!1d-112.0407584!2d43.4926607!1m5!1m1!1s0x5343510fedc7db4d:0x214c1d71e3fdf714!2m2!1d-112.0391057!2d46.5891452!1m5!1m1!1s0x53486f8888fa9d97:0x373556d4f179b550!2m2!1d-108.5006904!2d45.7832856!1m5!1m1!1s0x87609365c85e7a63:0x69cefc3917343e53!2m2!1d-106.2980824!2d42.848709!1m5!1m1!1s0x876f38762e73ef93:0xb10a30418f972d2b!2m2!1d-104.8202462!2d41.1399814!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Minneapolis,+MN/Sioux+Falls,+SD/Pierre,+SD/Bismarck,+ND/Fargo,+ND/Winnipeg,+MB,+Canada/Duluth,+MN/Minneapolis,+MN/@46.6404497,-100.928197,6z/data=!3m1!4b1!4m53!4m52!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!1m5!1m1!1s0x878eb498e0bdacd7:0xde95ff3aa8b2fccf!2m2!1d-96.731265!2d43.5460223!1m5!1m1!1s0x52d54a64b288f891:0x9e9950165931af92!2m2!1d-100.3537522!2d44.3667876!1m5!1m1!1s0x52d7831257d8e963:0xccaabd12f9bbca93!2m2!1d-100.7837392!2d46.8083268!1m5!1m1!1s0x52c8cb8d84677145:0x81aa30a52791aaca!2m2!1d-96.7898034!2d46.8771863!1m5!1m1!1s0x52ea73fbf91a2b11:0x2b2a1afac6b9ca64!2m2!1d-97.1383744!2d49.895136!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Seattle,+WA/Vancouver,+BC,+Canada/Leavenworth,+WA/Spokane,+WA/Redding,+CA/Gold+Beach,+OR/Salem,+OR/Portland,+OR/Olympia,+WA/Seattle,+WA/@44.8374018,-125.1438928,6.26z/data=!4m65!4m64!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!1m5!1m1!1s0x548673f143a94fb3:0xbb9196ea9b81f38b!2m2!1d-123.1207375!2d49.2827291!1m5!1m1!1s0x549a4d92a4f8f98d:0xa14f95fb0abfef7e!2m2!1d-120.6614765!2d47.5962326!1m5!1m1!1s0x549e185c30bbe7e5:0xddfcc9d60b84d9b1!2m2!1d-117.4260465!2d47.6587802!1m5!1m1!1s0x54d291d63b4a202f:0x1f3358ec7b360f57!2m2!1d-122.3916754!2d40.5865396!1m5!1m1!1s0x54dace49bf9ae73d:0x121195079f68806d!2m2!1d-124.4217741!2d42.4073334!1m5!1m1!1s0x54bffefcbc4b9c63:0xf93429e08f0357c2!2m2!1d-123.0350963!2d44.9428975!1m5!1m1!1s0x54950b0b7da97427:0x1c36b9e6f6d18591!2m2!1d-122.6783853!2d45.515232!1m5!1m1!1s0x5491c9c1ae285569:0x4f146197e2881b83!2m2!1d-122.9006951!2d47.0378741!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Albany,+NY/Burlington,+VT/Montpelier,+VT/Concord,+NH/Augusta,+ME/Portland,+ME/Boston,+MA/Barnstable,+MA/Providence,+RI/Hartford,+CT/@41.8793352,-74.5474305,7z/data=!4m65!4m64!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!1m5!1m1!1s0x4cca7a55b69b55e5:0xc35fe519720e498e!2m2!1d-73.212072!2d44.4758825!1m5!1m1!1s0x4cb5a78cc44dea05:0x4891e094ceb5836!2m2!1d-72.5753869!2d44.2600593!1m5!1m1!1s0x89e26a96154a8917:0x5a871a0a62528f1!2m2!1d-71.5375718!2d43.2081366!1m5!1m1!1s0x4cb200fdafacc49d:0x79a3488d64220b2d!2m2!1d-69.7794897!2d44.3106241!1m5!1m1!1s0x4cb29c72aab0ee2d:0x7e9db6b53372fa29!2m2!1d-70.2568189!2d43.6590993!1m5!1m1!1s0x89e3652d0d3d311b:0x787cbf240162e8a0!2m2!1d-71.0588801!2d42.3600825!1m5!1m1!1s0x89fb33b67f8ec5e5:0xea7648efbb136d73!2m2!1d-70.3002024!2d41.7003208!1m5!1m1!1s0x89e444e0437e735d:0x69df7c4d48b3b627!2m2!1d-71.4128343!2d41.8239891!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Hartford,+CT/New+York,+NY/Trenton,+NJ/Philadelphia,+PA/Dover,+DE/Annapolis,+MD/Baltimore,+MD/Washington+D.C.,+DC/Richmond,+VA/Williamsburg,+VA/@39.5003974,-77.3244192,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!1m5!1m1!1s0x89c24fa5d33f083b:0xc80b8f06e177fe62!2m2!1d-74.0059728!2d40.7127753!1m5!1m1!1s0x89c143482d3dbbb9:0xcf16567f895cd7bc!2m2!1d-74.759717!2d40.2205824!1m5!1m1!1s0x89c6b7d8d4b54beb:0x89f514d88c3e58c1!2m2!1d-75.1652215!2d39.9525839!1m5!1m1!1s0x89c7633375685ead:0xa9e2e447fb006cf0!2m2!1d-75.5243682!2d39.158168!1m5!1m1!1s0x89b7f66570672fd5:0x43f854fdd3a8274b!2m2!1d-76.4921829!2d38.9784453!1m5!1m1!1s0x89c803aed6f483b7:0x44896a84223e758!2m2!1d-76.6121893!2d39.2903848!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x89b111095799c9ed:0xbfd83e6de2423cc5!2m2!1d-77.4360481!2d37.5407246!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Williamsburg,+VA/Norfolk,+VA/Charlottesville,+VA/Harrisburg,+PA/Buffalo,+NY/Rochester,+NY/Albany,+NY/@40.2169587,-81.2677638,5.7z/data=!4m47!4m46!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!1m5!1m1!1s0x89ba973a5322ca45:0xab99107fce7a1e0a!2m2!1d-76.2858726!2d36.8507689!1m5!1m1!1s0x89b3862dea50a48f:0x9086f096c38b74fc!2m2!1d-78.4766781!2d38.0293059!1m5!1m1!1s0x89c8c116b8079e97:0xbb6e42c8128d46d5!2m2!1d-76.8867008!2d40.2731911!1m5!1m1!1s0x89d3126152dfe5a1:0x982304a5181f8171!2m2!1d-78.8783689!2d42.8864468!1m5!1m1!1s0x89d6b3059614b353:0x5a001ffc4125e61e!2m2!1d-77.6088465!2d43.1565779!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Pittsburgh,+PA/Charleston,+WV/Columbus,+OH/Cincinnati,+OH/Frankfort,+KY/Louisville,+KY/Indianapolis,+IN/Chicago,+IL/Milwaukee,+WI/Madison,+WI/@40.5504662,-89.1782838,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!1m5!1m1!1s0x884f2cce88145d39:0x7661a84704c91b0b!2m2!1d-81.6326234!2d38.3498195!1m5!1m1!1s0x883889c1b990de71:0xe43266f8cfb1b533!2m2!1d-82.9987942!2d39.9611755!1m5!1m1!1s0x884051b1de3821f9:0x69fb7e8be4c09317!2m2!1d-84.5120196!2d39.1031182!1m5!1m1!1s0x8842734c8b1953c9:0x536418a08867425c!2m2!1d-84.8732835!2d38.2009055!1m5!1m1!1s0x88690b1ab35bd511:0xd4d3b4282071fd32!2m2!1d-85.7584557!2d38.2526647!1m5!1m1!1s0x886b50ffa7796a03:0xd68e9df640b9ea7c!2m2!1d-86.158068!2d39.768403!1m5!1m1!1s0x880e2c3cd0f4cbed:0xafe0a6ad09c0c000!2m2!1d-87.6297982!2d41.8781136!1m5!1m1!1s0x880502d7578b47e7:0x445f1922b5417b84!2m2!1d-87.9064736!2d43.0389025!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Madison,+Wisconsin/Green+Bay,+WI/Mackinaw+City,+MI/Grand+Rapids,+MI/Lansing,+MI/Frankenmuth,+MI/Detroit,+MI/Cleveland,+OH/Pittsburgh,+PA/@43.1918863,-89.1853954,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!1m5!1m1!1s0x8802e2e809b380f3:0x6370045214dcf571!2m2!1d-88.0132958!2d44.5133188!1m5!1m1!1s0x4d358b3940a9ad83:0xeac771ab20cc7a7a!2m2!1d-84.7271465!2d45.7774987!1m5!1m1!1s0x88185460bb502815:0xa593aacb1bd3a8d0!2m2!1d-85.6680863!2d42.9633599!1m5!1m1!1s0x8822c01c7f318c37:0x4378b62389029d9e!2m2!1d-84.5555347!2d42.732535!1m5!1m1!1s0x8823f287285df793:0x8050516199bcb01f!2m2!1d-83.7380194!2d43.331691!1m5!1m1!1s0x8824ca0110cb1d75:0x5776864e35b9c4d2!2m2!1d-83.0457538!2d42.331427!1m5!1m1!1s0x8830ef2ee3686b2d:0xed04cb55f7621842!2m2!1d-81.6943605!2d41.49932!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/San+Juan,+Puerto+Rico/@28.406847,-80.5870322,5z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x8c03686fe268196f:0xad6b7f0f5c935adc!2m2!1d-66.1057355!2d18.4655394!3e4</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/Honolulu,+HI/@24.8112769,-154.8564566,3z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x7c00183b8cc3464d:0x4b28f55ff3a7976c!2m2!1d-157.8583333!2d21.3069444!3e4</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Orlando,+FL/Miami,+FL/Key+West,+FL/Everglades+City,+FL/Tampa,+FL/Tarpon+Springs,+FL/Tallahassee,+FL/Jacksonville,+FL/St.+Augustine,+FL/Orlando,+FL/@27.5091232,-84.4177219,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!1m5!1m1!1s0x88d9b0a20ec8c111:0xff96f271ddad4f65!2m2!1d-80.1917902!2d25.7616798!1m5!1m1!1s0x88d1b134ad952377:0x3fcee92f77463b5e!2m2!1d-81.7799871!2d24.5550593!1m5!1m1!1s0x88da5c605ba45fb1:0x92bcf49fb504533a!2m2!1d-81.3850695!2d25.8582443!1m5!1m1!1s0x88c2b782b3b9d1e1:0xa75f1389af96b463!2m2!1d-82.4571776!2d27.950575!1m5!1m1!1s0x88c28cfd6f0942df:0xf4297f0ce0bf24b7!2m2!1d-82.7567679!2d28.1461248!1m5!1m1!1s0x88ec8a5187124b53:0xebee077ad4fdb1f8!2m2!1d-84.2807329!2d30.4382559!1m5!1m1!1s0x88e5b716f1ceafeb:0xc4cd7d3896fcc7e2!2m2!1d-81.655651!2d30.3321838!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Los+Angeles,+CA/Santa+Barbara,+CA/Solvang,+CA/San+Jose,+CA/San+Francisco,+CA/Sacramento,+CA/Reno,+NV/Virginia+City,+NV/Carson+City,+NV/Fresno,+CA/@36.7777641,-122.6363689,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!1m5!1m1!1s0x80e914c76f2d83d5:0xc8d13a64d7ba7648!2m2!1d-119.6981901!2d34.4208305!1m5!1m1!1s0x80e954a0fc922285:0x2d0e281b060bc156!2m2!1d-120.1376481!2d34.5958201!1m5!1m1!1s0x808fcae48af93ff5:0xb99d8c0aca9f717b!2m2!1d-121.8863286!2d37.3382082!1m5!1m1!1s0x80859a6d00690021:0x4a501367f076adff!2m2!1d-122.4194155!2d37.7749295!1m5!1m1!1s0x809ac672b28397f9:0x921f6aaa74197fdb!2m2!1d-121.4943996!2d38.5815719!1m5!1m1!1s0x809940ae9292a09d:0x40c5c5ce7438f787!2m2!1d-119.8138027!2d39.5296329!1m5!1m1!1s0x80990faad3daafd1:0x29dad257dc576fa9!2m2!1d-119.6499793!2d39.3095135!1m5!1m1!1s0x80990aa1f8deb471:0xf79c6c82bde23828!2m2!1d-119.7674034!2d39.1637984!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Fresno,+CA/Riverside,+CA/San+Diego,+CA/Los+Angeles,+CA/@34.7127545,-120.6716835,7z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!1m5!1m1!1s0x80dca6df7ff47dbb:0xf7a1d705135e0ae8!2m2!1d-117.3754942!2d33.9806005!1m5!1m1!1s0x80d9530fad921e4b:0xd3a21fdfd15df79!2m2!1d-117.1610838!2d32.715738!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Phoenix,+AZ/Sedona,+AZ/Las+Vegas,+NV/St.+George,+UT/Taos,+NM/Santa+Fe,+NM/Albuquerque,+NM/Lubbock,+TX/El+Paso,+TX/Tucson,+AZ/@34.1501088,-117.508012,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!1m5!1m1!1s0x872da132f942b00d:0x5548c523fa6c8efd!2m2!1d-111.7609896!2d34.8697395!1m5!1m1!1s0x80beb782a4f57dd1:0x3accd5e6d5b379a3!2m2!1d-115.1398296!2d36.1699412!1m5!1m1!1s0x80ca44d0984939e5:0x531707f2f8a11c1e!2m2!1d-113.5684164!2d37.0965278!1m5!1m1!1s0x871764da7f11fcb1:0x90ea918361a9b782!2m2!1d-105.5733788!2d36.4072134!1m5!1m1!1s0x87185043e79852a9:0x8c902373fd88df40!2m2!1d-105.937799!2d35.6869752!1m5!1m1!1s0x87220addd309837b:0xc0d3f8ceb8d9f6fd!2m2!1d-106.650422!2d35.0843859!1m5!1m1!1s0x86fe12add37ddd39:0x1af0042922e84287!2m2!1d-101.8551665!2d33.5778631!1m5!1m1!1s0x86e73f8bc5fe3b69:0xe39184e3ab9d0222!2m2!1d-106.4850217!2d31.7618778!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Tucson,+AZ/Phoenix,+AZ/@32.6659365,-112.3105217,7.68z/data=!4m17!4m16!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Dallas,+TX/Austin,+TX/San+Antonio,+TX/McAllen,+TX/Houston,+TX/Baton+Rouge,+LA/New+Orleans,+LA/Gulfport,+MS/Jackson,+MS/@29.4197283,-98.2903561,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!1m5!1m1!1s0x8644b599a0cc032f:0x5d9b464bd469d57a!2m2!1d-97.7430608!2d30.267153!1m5!1m1!1s0x865c58af04d00eaf:0x856e13b10a016bc!2m2!1d-98.4936282!2d29.4241219!1m5!1m1!1s0x866576324d9637df:0x2f1d39a9b52c0eb8!2m2!1d-98.2300124!2d26.2034071!1m5!1m1!1s0x8640b8b4488d8501:0xca0d02def365053b!2m2!1d-95.3698028!2d29.7604267!1m5!1m1!1s0x86243867325f74cb:0x2123f1db91579a1d!2m2!1d-91.1871466!2d30.4514677!1m5!1m1!1s0x8620a454b2118265:0xdb065be85e22d3b4!2m2!1d-90.0715323!2d29.9510658!1m5!1m1!1s0x889c166ee80114e5:0xc2614d446e819544!2m2!1d-89.0928155!2d30.3674198!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Jackson,+MS/Little+Rock,+AR/Fayetteville,+AR/Dallas,+TX/@32.5477822,-99.0081422,5.75z/data=!4m29!4m28!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!1m5!1m1!1s0x87d2a134a11f569b:0x3405f5100df35b17!2m2!1d-92.2895948!2d34.7464809!1m5!1m1!1s0x87c96f7b2fb53e9d:0x4519f069fcb4c8cf!2m2!1d-94.157853!2d36.0662419!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Atlanta,+GA/Helen,+GA/Nashville,+TN/Knoxville,+TN/Charlotte,+NC/Greensboro,+NC/Raleigh,+NC/Columbia,+SC/Charleston,+SC/Savannah,+GA/@34.0640266,-87.1468938,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!1m5!1m1!1s0x885f37d40b3a2aa1:0x8ed537fed96523a8!2m2!1d-83.7315675!2d34.7014839!1m5!1m1!1s0x8864ec3213eb903d:0x7d3fb9d0a1e9daa0!2m2!1d-86.7816016!2d36.1626638!1m5!1m1!1s0x885c162246ce42a9:0x7bea92dac4f534c5!2m2!1d-83.9207392!2d35.9606384!1m5!1m1!1s0x88541fc4fc381a81:0x884650e6bf43d164!2m2!1d-80.8431267!2d35.2270869!1m5!1m1!1s0x8853193f38c77b79:0x93b9c49478be12c8!2m2!1d-79.7919754!2d36.0726354!1m5!1m1!1s0x89ac5a2f9f51e0f7:0x6790b6528a11f0ad!2m2!1d-78.6381787!2d35.7795897!1m5!1m1!1s0x88f8a5697931d1e3:0xf32808f4b379fa96!2m2!1d-81.0348144!2d34.0007104!1m5!1m1!1s0x88fe7a42dca82477:0x35faf7e0aee1ec6b!2m2!1d-79.9310512!2d32.7764749!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>Northeast + MD, DE, VA</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>SEA &gt; ANC</t>
+  </si>
+  <si>
+    <t>SFO &gt; HNL</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>old_order</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
     <t>Apr</t>
   </si>
   <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>best_temp_1</t>
-  </si>
-  <si>
-    <t>best_temp_2</t>
-  </si>
-  <si>
-    <t>Aug-Sep</t>
-  </si>
-  <si>
-    <t>Oct-Nov</t>
-  </si>
-  <si>
-    <t>Nov-Dec</t>
-  </si>
-  <si>
-    <t>Jul-Aug</t>
-  </si>
-  <si>
-    <t>May-Jun</t>
-  </si>
-  <si>
-    <t>Apr-May</t>
-  </si>
-  <si>
-    <t>Mar-Apr</t>
-  </si>
-  <si>
-    <t>Jan-Mar</t>
-  </si>
-  <si>
-    <t>Jan-Feb</t>
-  </si>
-  <si>
-    <t>bt1</t>
-  </si>
-  <si>
-    <t>bt2</t>
-  </si>
-  <si>
-    <t>states_etc</t>
-  </si>
-  <si>
-    <t>url1</t>
-  </si>
-  <si>
-    <t>url2</t>
-  </si>
-  <si>
-    <t>url3</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Toronto,+ON,+Canada/Ottawa,+ON,+Canada/Montreal,+QC,+Canada/Qu%C3%A9bec,+QC,+Canada/Montr%C3%A9al,+QC,+Canada/Toronto,+ON,+Canada/@45.1540678,-79.7807285,6z/data=!3m1!4b1!4m41!4m40!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!1m5!1m1!1s0x4cce05b25f5113af:0x8a6a51e131dd15ed!2m2!1d-75.6971931!2d45.4215296!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x4cb8968a05db8893:0x8fc52d63f0e83a03!2m2!1d-71.2079809!2d46.8138783!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Anchorage,+AK/Fairbanks,+AK/Anchorage,+AK/@63.8441792,-152.4627417,6.14z/data=!4m22!4m21!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!1m5!1m1!1s0x5132454f67fd65a9:0xb3d805e009fef73a!2m2!1d-147.7163888!2d64.8377778!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!2m1!2b1!3e0</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Denver,+CO/Grand+Junction,+CO/Salt+Lake+City,+UT/Boise,+ID/Idaho+Falls,+ID/Helena,+MT/Billings,+MT/Casper,+WY/Cheyenne,+WY/Denver,+Colorado/@42.4201276,-119.4822548,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!1m5!1m1!1s0x8746d6e322e77057:0xcc63f451cebf7c56!2m2!1d-108.5506486!2d39.0638705!1m5!1m1!1s0x87523d9488d131ed:0x5b53b7a0484d31ca!2m2!1d-111.8910474!2d40.7607793!1m5!1m1!1s0x54aef172e947b49d:0x9a5b989b36679d9b!2m2!1d-116.2023137!2d43.6150186!1m5!1m1!1s0x5354594e739512b5:0x2311c9fc094c49c9!2m2!1d-112.0407584!2d43.4926607!1m5!1m1!1s0x5343510fedc7db4d:0x214c1d71e3fdf714!2m2!1d-112.0391057!2d46.5891452!1m5!1m1!1s0x53486f8888fa9d97:0x373556d4f179b550!2m2!1d-108.5006904!2d45.7832856!1m5!1m1!1s0x87609365c85e7a63:0x69cefc3917343e53!2m2!1d-106.2980824!2d42.848709!1m5!1m1!1s0x876f38762e73ef93:0xb10a30418f972d2b!2m2!1d-104.8202462!2d41.1399814!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Minneapolis,+MN/Sioux+Falls,+SD/Pierre,+SD/Bismarck,+ND/Fargo,+ND/Winnipeg,+MB,+Canada/Duluth,+MN/Minneapolis,+MN/@46.6404497,-100.928197,6z/data=!3m1!4b1!4m53!4m52!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!1m5!1m1!1s0x878eb498e0bdacd7:0xde95ff3aa8b2fccf!2m2!1d-96.731265!2d43.5460223!1m5!1m1!1s0x52d54a64b288f891:0x9e9950165931af92!2m2!1d-100.3537522!2d44.3667876!1m5!1m1!1s0x52d7831257d8e963:0xccaabd12f9bbca93!2m2!1d-100.7837392!2d46.8083268!1m5!1m1!1s0x52c8cb8d84677145:0x81aa30a52791aaca!2m2!1d-96.7898034!2d46.8771863!1m5!1m1!1s0x52ea73fbf91a2b11:0x2b2a1afac6b9ca64!2m2!1d-97.1383744!2d49.895136!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Seattle,+WA/Vancouver,+BC,+Canada/Leavenworth,+WA/Spokane,+WA/Redding,+CA/Gold+Beach,+OR/Salem,+OR/Portland,+OR/Olympia,+WA/Seattle,+WA/@44.8374018,-125.1438928,6.26z/data=!4m65!4m64!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!1m5!1m1!1s0x548673f143a94fb3:0xbb9196ea9b81f38b!2m2!1d-123.1207375!2d49.2827291!1m5!1m1!1s0x549a4d92a4f8f98d:0xa14f95fb0abfef7e!2m2!1d-120.6614765!2d47.5962326!1m5!1m1!1s0x549e185c30bbe7e5:0xddfcc9d60b84d9b1!2m2!1d-117.4260465!2d47.6587802!1m5!1m1!1s0x54d291d63b4a202f:0x1f3358ec7b360f57!2m2!1d-122.3916754!2d40.5865396!1m5!1m1!1s0x54dace49bf9ae73d:0x121195079f68806d!2m2!1d-124.4217741!2d42.4073334!1m5!1m1!1s0x54bffefcbc4b9c63:0xf93429e08f0357c2!2m2!1d-123.0350963!2d44.9428975!1m5!1m1!1s0x54950b0b7da97427:0x1c36b9e6f6d18591!2m2!1d-122.6783853!2d45.515232!1m5!1m1!1s0x5491c9c1ae285569:0x4f146197e2881b83!2m2!1d-122.9006951!2d47.0378741!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Albany,+NY/Burlington,+VT/Montpelier,+VT/Concord,+NH/Augusta,+ME/Portland,+ME/Boston,+MA/Barnstable,+MA/Providence,+RI/Hartford,+CT/@41.8793352,-74.5474305,7z/data=!4m65!4m64!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!1m5!1m1!1s0x4cca7a55b69b55e5:0xc35fe519720e498e!2m2!1d-73.212072!2d44.4758825!1m5!1m1!1s0x4cb5a78cc44dea05:0x4891e094ceb5836!2m2!1d-72.5753869!2d44.2600593!1m5!1m1!1s0x89e26a96154a8917:0x5a871a0a62528f1!2m2!1d-71.5375718!2d43.2081366!1m5!1m1!1s0x4cb200fdafacc49d:0x79a3488d64220b2d!2m2!1d-69.7794897!2d44.3106241!1m5!1m1!1s0x4cb29c72aab0ee2d:0x7e9db6b53372fa29!2m2!1d-70.2568189!2d43.6590993!1m5!1m1!1s0x89e3652d0d3d311b:0x787cbf240162e8a0!2m2!1d-71.0588801!2d42.3600825!1m5!1m1!1s0x89fb33b67f8ec5e5:0xea7648efbb136d73!2m2!1d-70.3002024!2d41.7003208!1m5!1m1!1s0x89e444e0437e735d:0x69df7c4d48b3b627!2m2!1d-71.4128343!2d41.8239891!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Hartford,+CT/New+York,+NY/Trenton,+NJ/Philadelphia,+PA/Dover,+DE/Annapolis,+MD/Baltimore,+MD/Washington+D.C.,+DC/Richmond,+VA/Williamsburg,+VA/@39.5003974,-77.3244192,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!1m5!1m1!1s0x89c24fa5d33f083b:0xc80b8f06e177fe62!2m2!1d-74.0059728!2d40.7127753!1m5!1m1!1s0x89c143482d3dbbb9:0xcf16567f895cd7bc!2m2!1d-74.759717!2d40.2205824!1m5!1m1!1s0x89c6b7d8d4b54beb:0x89f514d88c3e58c1!2m2!1d-75.1652215!2d39.9525839!1m5!1m1!1s0x89c7633375685ead:0xa9e2e447fb006cf0!2m2!1d-75.5243682!2d39.158168!1m5!1m1!1s0x89b7f66570672fd5:0x43f854fdd3a8274b!2m2!1d-76.4921829!2d38.9784453!1m5!1m1!1s0x89c803aed6f483b7:0x44896a84223e758!2m2!1d-76.6121893!2d39.2903848!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x89b111095799c9ed:0xbfd83e6de2423cc5!2m2!1d-77.4360481!2d37.5407246!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Williamsburg,+VA/Norfolk,+VA/Charlottesville,+VA/Harrisburg,+PA/Buffalo,+NY/Rochester,+NY/Albany,+NY/@40.2169587,-81.2677638,5.7z/data=!4m47!4m46!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!1m5!1m1!1s0x89ba973a5322ca45:0xab99107fce7a1e0a!2m2!1d-76.2858726!2d36.8507689!1m5!1m1!1s0x89b3862dea50a48f:0x9086f096c38b74fc!2m2!1d-78.4766781!2d38.0293059!1m5!1m1!1s0x89c8c116b8079e97:0xbb6e42c8128d46d5!2m2!1d-76.8867008!2d40.2731911!1m5!1m1!1s0x89d3126152dfe5a1:0x982304a5181f8171!2m2!1d-78.8783689!2d42.8864468!1m5!1m1!1s0x89d6b3059614b353:0x5a001ffc4125e61e!2m2!1d-77.6088465!2d43.1565779!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Pittsburgh,+PA/Charleston,+WV/Columbus,+OH/Cincinnati,+OH/Frankfort,+KY/Louisville,+KY/Indianapolis,+IN/Chicago,+IL/Milwaukee,+WI/Madison,+WI/@40.5504662,-89.1782838,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!1m5!1m1!1s0x884f2cce88145d39:0x7661a84704c91b0b!2m2!1d-81.6326234!2d38.3498195!1m5!1m1!1s0x883889c1b990de71:0xe43266f8cfb1b533!2m2!1d-82.9987942!2d39.9611755!1m5!1m1!1s0x884051b1de3821f9:0x69fb7e8be4c09317!2m2!1d-84.5120196!2d39.1031182!1m5!1m1!1s0x8842734c8b1953c9:0x536418a08867425c!2m2!1d-84.8732835!2d38.2009055!1m5!1m1!1s0x88690b1ab35bd511:0xd4d3b4282071fd32!2m2!1d-85.7584557!2d38.2526647!1m5!1m1!1s0x886b50ffa7796a03:0xd68e9df640b9ea7c!2m2!1d-86.158068!2d39.768403!1m5!1m1!1s0x880e2c3cd0f4cbed:0xafe0a6ad09c0c000!2m2!1d-87.6297982!2d41.8781136!1m5!1m1!1s0x880502d7578b47e7:0x445f1922b5417b84!2m2!1d-87.9064736!2d43.0389025!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Madison,+Wisconsin/Green+Bay,+WI/Mackinaw+City,+MI/Grand+Rapids,+MI/Lansing,+MI/Frankenmuth,+MI/Detroit,+MI/Cleveland,+OH/Pittsburgh,+PA/@43.1918863,-89.1853954,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!1m5!1m1!1s0x8802e2e809b380f3:0x6370045214dcf571!2m2!1d-88.0132958!2d44.5133188!1m5!1m1!1s0x4d358b3940a9ad83:0xeac771ab20cc7a7a!2m2!1d-84.7271465!2d45.7774987!1m5!1m1!1s0x88185460bb502815:0xa593aacb1bd3a8d0!2m2!1d-85.6680863!2d42.9633599!1m5!1m1!1s0x8822c01c7f318c37:0x4378b62389029d9e!2m2!1d-84.5555347!2d42.732535!1m5!1m1!1s0x8823f287285df793:0x8050516199bcb01f!2m2!1d-83.7380194!2d43.331691!1m5!1m1!1s0x8824ca0110cb1d75:0x5776864e35b9c4d2!2m2!1d-83.0457538!2d42.331427!1m5!1m1!1s0x8830ef2ee3686b2d:0xed04cb55f7621842!2m2!1d-81.6943605!2d41.49932!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/San+Juan,+Puerto+Rico/@28.406847,-80.5870322,5z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x8c03686fe268196f:0xad6b7f0f5c935adc!2m2!1d-66.1057355!2d18.4655394!3e4</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/Honolulu,+HI/@24.8112769,-154.8564566,3z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x7c00183b8cc3464d:0x4b28f55ff3a7976c!2m2!1d-157.8583333!2d21.3069444!3e4</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Orlando,+FL/Miami,+FL/Key+West,+FL/Everglades+City,+FL/Tampa,+FL/Tarpon+Springs,+FL/Tallahassee,+FL/Jacksonville,+FL/St.+Augustine,+FL/Orlando,+FL/@27.5091232,-84.4177219,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!1m5!1m1!1s0x88d9b0a20ec8c111:0xff96f271ddad4f65!2m2!1d-80.1917902!2d25.7616798!1m5!1m1!1s0x88d1b134ad952377:0x3fcee92f77463b5e!2m2!1d-81.7799871!2d24.5550593!1m5!1m1!1s0x88da5c605ba45fb1:0x92bcf49fb504533a!2m2!1d-81.3850695!2d25.8582443!1m5!1m1!1s0x88c2b782b3b9d1e1:0xa75f1389af96b463!2m2!1d-82.4571776!2d27.950575!1m5!1m1!1s0x88c28cfd6f0942df:0xf4297f0ce0bf24b7!2m2!1d-82.7567679!2d28.1461248!1m5!1m1!1s0x88ec8a5187124b53:0xebee077ad4fdb1f8!2m2!1d-84.2807329!2d30.4382559!1m5!1m1!1s0x88e5b716f1ceafeb:0xc4cd7d3896fcc7e2!2m2!1d-81.655651!2d30.3321838!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Los+Angeles,+CA/Santa+Barbara,+CA/Solvang,+CA/San+Jose,+CA/San+Francisco,+CA/Sacramento,+CA/Reno,+NV/Virginia+City,+NV/Carson+City,+NV/Fresno,+CA/@36.7777641,-122.6363689,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!1m5!1m1!1s0x80e914c76f2d83d5:0xc8d13a64d7ba7648!2m2!1d-119.6981901!2d34.4208305!1m5!1m1!1s0x80e954a0fc922285:0x2d0e281b060bc156!2m2!1d-120.1376481!2d34.5958201!1m5!1m1!1s0x808fcae48af93ff5:0xb99d8c0aca9f717b!2m2!1d-121.8863286!2d37.3382082!1m5!1m1!1s0x80859a6d00690021:0x4a501367f076adff!2m2!1d-122.4194155!2d37.7749295!1m5!1m1!1s0x809ac672b28397f9:0x921f6aaa74197fdb!2m2!1d-121.4943996!2d38.5815719!1m5!1m1!1s0x809940ae9292a09d:0x40c5c5ce7438f787!2m2!1d-119.8138027!2d39.5296329!1m5!1m1!1s0x80990faad3daafd1:0x29dad257dc576fa9!2m2!1d-119.6499793!2d39.3095135!1m5!1m1!1s0x80990aa1f8deb471:0xf79c6c82bde23828!2m2!1d-119.7674034!2d39.1637984!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Fresno,+CA/Riverside,+CA/San+Diego,+CA/Los+Angeles,+CA/@34.7127545,-120.6716835,7z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!1m5!1m1!1s0x80dca6df7ff47dbb:0xf7a1d705135e0ae8!2m2!1d-117.3754942!2d33.9806005!1m5!1m1!1s0x80d9530fad921e4b:0xd3a21fdfd15df79!2m2!1d-117.1610838!2d32.715738!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Phoenix,+AZ/Sedona,+AZ/Las+Vegas,+NV/St.+George,+UT/Taos,+NM/Santa+Fe,+NM/Albuquerque,+NM/Lubbock,+TX/El+Paso,+TX/Tucson,+AZ/@34.1501088,-117.508012,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!1m5!1m1!1s0x872da132f942b00d:0x5548c523fa6c8efd!2m2!1d-111.7609896!2d34.8697395!1m5!1m1!1s0x80beb782a4f57dd1:0x3accd5e6d5b379a3!2m2!1d-115.1398296!2d36.1699412!1m5!1m1!1s0x80ca44d0984939e5:0x531707f2f8a11c1e!2m2!1d-113.5684164!2d37.0965278!1m5!1m1!1s0x871764da7f11fcb1:0x90ea918361a9b782!2m2!1d-105.5733788!2d36.4072134!1m5!1m1!1s0x87185043e79852a9:0x8c902373fd88df40!2m2!1d-105.937799!2d35.6869752!1m5!1m1!1s0x87220addd309837b:0xc0d3f8ceb8d9f6fd!2m2!1d-106.650422!2d35.0843859!1m5!1m1!1s0x86fe12add37ddd39:0x1af0042922e84287!2m2!1d-101.8551665!2d33.5778631!1m5!1m1!1s0x86e73f8bc5fe3b69:0xe39184e3ab9d0222!2m2!1d-106.4850217!2d31.7618778!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Tucson,+AZ/Phoenix,+AZ/@32.6659365,-112.3105217,7.68z/data=!4m17!4m16!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Dallas,+TX/Austin,+TX/San+Antonio,+TX/McAllen,+TX/Houston,+TX/Baton+Rouge,+LA/New+Orleans,+LA/Gulfport,+MS/Jackson,+MS/@29.4197283,-98.2903561,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!1m5!1m1!1s0x8644b599a0cc032f:0x5d9b464bd469d57a!2m2!1d-97.7430608!2d30.267153!1m5!1m1!1s0x865c58af04d00eaf:0x856e13b10a016bc!2m2!1d-98.4936282!2d29.4241219!1m5!1m1!1s0x866576324d9637df:0x2f1d39a9b52c0eb8!2m2!1d-98.2300124!2d26.2034071!1m5!1m1!1s0x8640b8b4488d8501:0xca0d02def365053b!2m2!1d-95.3698028!2d29.7604267!1m5!1m1!1s0x86243867325f74cb:0x2123f1db91579a1d!2m2!1d-91.1871466!2d30.4514677!1m5!1m1!1s0x8620a454b2118265:0xdb065be85e22d3b4!2m2!1d-90.0715323!2d29.9510658!1m5!1m1!1s0x889c166ee80114e5:0xc2614d446e819544!2m2!1d-89.0928155!2d30.3674198!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Jackson,+MS/Little+Rock,+AR/Fayetteville,+AR/Dallas,+TX/@32.5477822,-99.0081422,5.75z/data=!4m29!4m28!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!1m5!1m1!1s0x87d2a134a11f569b:0x3405f5100df35b17!2m2!1d-92.2895948!2d34.7464809!1m5!1m1!1s0x87c96f7b2fb53e9d:0x4519f069fcb4c8cf!2m2!1d-94.157853!2d36.0662419!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Atlanta,+GA/Helen,+GA/Nashville,+TN/Knoxville,+TN/Charlotte,+NC/Greensboro,+NC/Raleigh,+NC/Columbia,+SC/Charleston,+SC/Savannah,+GA/@34.0640266,-87.1468938,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!1m5!1m1!1s0x885f37d40b3a2aa1:0x8ed537fed96523a8!2m2!1d-83.7315675!2d34.7014839!1m5!1m1!1s0x8864ec3213eb903d:0x7d3fb9d0a1e9daa0!2m2!1d-86.7816016!2d36.1626638!1m5!1m1!1s0x885c162246ce42a9:0x7bea92dac4f534c5!2m2!1d-83.9207392!2d35.9606384!1m5!1m1!1s0x88541fc4fc381a81:0x884650e6bf43d164!2m2!1d-80.8431267!2d35.2270869!1m5!1m1!1s0x8853193f38c77b79:0x93b9c49478be12c8!2m2!1d-79.7919754!2d36.0726354!1m5!1m1!1s0x89ac5a2f9f51e0f7:0x6790b6528a11f0ad!2m2!1d-78.6381787!2d35.7795897!1m5!1m1!1s0x88f8a5697931d1e3:0xf32808f4b379fa96!2m2!1d-81.0348144!2d34.0007104!1m5!1m1!1s0x88fe7a42dca82477:0x35faf7e0aee1ec6b!2m2!1d-79.9310512!2d32.7764749!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>Northeast + MD, DE, VA</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>SEA &gt; ANC</t>
-  </si>
-  <si>
-    <t>SFO &gt; HNL</t>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Mar</t>
   </si>
 </sst>
 </file>
@@ -2445,7 +2436,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2637,7 +2628,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3242,10 +3233,10 @@
         <v>152</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -7225,10 +7216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7243,10 +7234,12 @@
     <col min="8" max="10" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>235</v>
       </c>
@@ -7260,192 +7253,205 @@
         <v>234</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>237</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="1">
+        <v>719</v>
+      </c>
+      <c r="D2" s="1">
+        <f>IF(B2="Drive",0,2)+_xlfn.CEILING.MATH(C2/200,1)+K2</f>
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="1">
+        <f>(3*2)+3-2</f>
+        <v>7</v>
+      </c>
+      <c r="L2" s="1">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
         <v>1056</v>
       </c>
-      <c r="D2" s="1">
-        <f t="shared" ref="D2:D16" si="0">IF(B2="Drive",0,2)+_xlfn.CEILING.MATH(C2/200,1)+K2</f>
+      <c r="D3" s="1">
+        <f>IF(B3="Drive",0,2)+_xlfn.CEILING.MATH(C3/200,1)+K3</f>
         <v>10</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E3" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="H3" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K3" s="1">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="L2" s="1">
-        <v>6</v>
-      </c>
-      <c r="M2" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C3" s="1">
-        <v>719</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="E3" s="23" t="s">
+      <c r="L3" s="1">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1610</v>
+      </c>
+      <c r="D4" s="1">
+        <f>IF(B4="Drive",0,2)+_xlfn.CEILING.MATH(C4/200,1)+K4</f>
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K3" s="1">
-        <f>(3*2)+3-2</f>
+      <c r="G4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
         <v>7</v>
       </c>
-      <c r="L3" s="1">
-        <v>6</v>
-      </c>
-      <c r="M3" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2211</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="E4" s="23" t="s">
+      <c r="M4" s="1">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="1">
+        <f>1097+1202+(237*2)</f>
+        <v>2773</v>
+      </c>
+      <c r="D5" s="1">
+        <f>IF(B5="Drive",0,2)+_xlfn.CEILING.MATH(C5/200,1)+K5</f>
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>6</v>
-      </c>
-      <c r="M4" s="1">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1610</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -7456,8 +7462,11 @@
       <c r="M5" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>141</v>
       </c>
@@ -7468,123 +7477,131 @@
         <v>1955</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(B6="Drive",0,2)+_xlfn.CEILING.MATH(C6/200,1)+K6</f>
         <v>12</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>241</v>
+      <c r="E6" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>220</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
       </c>
       <c r="L6" s="1">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2211</v>
+      </c>
+      <c r="D7" s="1">
+        <f>IF(B7="Drive",0,2)+_xlfn.CEILING.MATH(C7/200,1)+K7</f>
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>6</v>
       </c>
-      <c r="M6" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="M7" s="1">
+        <v>10</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B8" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" s="1">
         <v>2403</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
+      <c r="D8" s="1">
+        <f>IF(B8="Drive",0,2)+_xlfn.CEILING.MATH(C8/200,1)+K8</f>
         <v>16</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>5.5</v>
-      </c>
-      <c r="M7" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C8" s="1">
-        <f>1097+1202+(237*2)</f>
-        <v>2773</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>243</v>
+      <c r="E8" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>270</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>271</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>262</v>
+        <v>274</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>258</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M8" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="N8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>135</v>
       </c>
@@ -7595,14 +7612,14 @@
         <v>1963</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(B9="Drive",0,2)+_xlfn.CEILING.MATH(C9/200,1)+K9</f>
         <v>12</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>243</v>
+      <c r="E9" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>218</v>
@@ -7614,13 +7631,16 @@
         <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M9" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>140</v>
       </c>
@@ -7632,26 +7652,26 @@
         <v>1461</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(B10="Drive",0,2)+_xlfn.CEILING.MATH(C10/200,1)+K10</f>
         <v>10</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>243</v>
+      <c r="E10" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>221</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -7660,84 +7680,90 @@
         <v>5</v>
       </c>
       <c r="M10" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="N10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="1">
+        <f>1951+(278*2)</f>
+        <v>2507</v>
+      </c>
+      <c r="D11" s="1">
+        <f>IF(B11="Drive",0,2)+_xlfn.CEILING.MATH(C11/200,1)+K11</f>
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1">
+        <v>11</v>
+      </c>
+      <c r="N11" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <f>2228+113</f>
         <v>2341</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
+      <c r="D12" s="1">
+        <f>IF(B12="Drive",0,2)+_xlfn.CEILING.MATH(C12/200,1)+K12</f>
         <v>14</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E12" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="J12" s="23" t="s">
         <v>251</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="M11" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="1">
-        <f>1951+(278*2)</f>
-        <v>2507</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>262</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
@@ -7746,10 +7772,13 @@
         <v>4</v>
       </c>
       <c r="M12" s="1">
+        <v>11</v>
+      </c>
+      <c r="N12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>137</v>
       </c>
@@ -7761,163 +7790,175 @@
         <v>2231</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(B13="Drive",0,2)+_xlfn.CEILING.MATH(C13/200,1)+K13</f>
         <v>14</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>252</v>
+      <c r="E13" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>216</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="J13" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>4</v>
+      </c>
+      <c r="M13" s="1">
+        <v>12</v>
+      </c>
+      <c r="N13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <f>IF(B14="Drive",0,2)+_xlfn.CEILING.MATH(C14/200,1)+K14</f>
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H14" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="M13" s="1">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1384</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>253</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>274</v>
-      </c>
       <c r="I14" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J14" s="23"/>
       <c r="K14" s="1">
-        <v>0</v>
+        <f>(3*2)+3-2</f>
+        <v>7</v>
       </c>
       <c r="L14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M14" s="1">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="N14" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>288</v>
+        <v>232</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>254</v>
+        <f>IF(B15="Drive",0,2)+_xlfn.CEILING.MATH(C15/200,1)+K15</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>238</v>
+        <v>284</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J15" s="23"/>
       <c r="K15" s="1">
-        <f>(3*2)+3-2</f>
-        <v>7</v>
+        <f>(1*2)+3-2</f>
+        <v>3</v>
       </c>
       <c r="L15" s="1">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="M15" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="N15" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>223</v>
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>1384</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>254</v>
+        <f>IF(B16="Drive",0,2)+_xlfn.CEILING.MATH(C16/200,1)+K16</f>
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>238</v>
+        <v>284</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="1">
-        <f>(1*2)+3-2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M16" s="1">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="N16" s="1">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L16">
-    <sortCondition ref="L2:L16"/>
-    <sortCondition descending="1" ref="K2:K16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N16">
+    <sortCondition ref="M2:M16"/>
+    <sortCondition descending="1" ref="L2:L16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update project with new travel (New Orleans)
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED0102F-A671-AF48-8C77-4BD13E1DDDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B413607E-1851-4445-B105-41B491D9EE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34280" yWindow="2120" windowWidth="20400" windowHeight="11660" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-34280" yWindow="2120" windowWidth="23380" windowHeight="15340" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2436,7 +2436,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2628,7 +2628,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3193,9 +3193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3204,8 +3204,8 @@
     <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -4770,11 +4770,11 @@
         <v>1</v>
       </c>
       <c r="F51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="1">
         <v>-90.071532300000001</v>
@@ -7218,7 +7218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -7294,7 +7294,7 @@
         <v>719</v>
       </c>
       <c r="D2" s="1">
-        <f>IF(B2="Drive",0,2)+_xlfn.CEILING.MATH(C2/200,1)+K2</f>
+        <f t="shared" ref="D2:D16" si="0">IF(B2="Drive",0,2)+_xlfn.CEILING.MATH(C2/200,1)+K2</f>
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -7340,7 +7340,7 @@
         <v>1056</v>
       </c>
       <c r="D3" s="1">
-        <f>IF(B3="Drive",0,2)+_xlfn.CEILING.MATH(C3/200,1)+K3</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -7386,7 +7386,7 @@
         <v>1610</v>
       </c>
       <c r="D4" s="1">
-        <f>IF(B4="Drive",0,2)+_xlfn.CEILING.MATH(C4/200,1)+K4</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -7432,7 +7432,7 @@
         <v>2773</v>
       </c>
       <c r="D5" s="1">
-        <f>IF(B5="Drive",0,2)+_xlfn.CEILING.MATH(C5/200,1)+K5</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -7477,7 +7477,7 @@
         <v>1955</v>
       </c>
       <c r="D6" s="1">
-        <f>IF(B6="Drive",0,2)+_xlfn.CEILING.MATH(C6/200,1)+K6</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -7522,7 +7522,7 @@
         <v>2211</v>
       </c>
       <c r="D7" s="1">
-        <f>IF(B7="Drive",0,2)+_xlfn.CEILING.MATH(C7/200,1)+K7</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -7567,7 +7567,7 @@
         <v>2403</v>
       </c>
       <c r="D8" s="1">
-        <f>IF(B8="Drive",0,2)+_xlfn.CEILING.MATH(C8/200,1)+K8</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -7612,7 +7612,7 @@
         <v>1963</v>
       </c>
       <c r="D9" s="1">
-        <f>IF(B9="Drive",0,2)+_xlfn.CEILING.MATH(C9/200,1)+K9</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -7652,7 +7652,7 @@
         <v>1461</v>
       </c>
       <c r="D10" s="1">
-        <f>IF(B10="Drive",0,2)+_xlfn.CEILING.MATH(C10/200,1)+K10</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -7698,7 +7698,7 @@
         <v>2507</v>
       </c>
       <c r="D11" s="1">
-        <f>IF(B11="Drive",0,2)+_xlfn.CEILING.MATH(C11/200,1)+K11</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -7744,7 +7744,7 @@
         <v>2341</v>
       </c>
       <c r="D12" s="1">
-        <f>IF(B12="Drive",0,2)+_xlfn.CEILING.MATH(C12/200,1)+K12</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -7790,7 +7790,7 @@
         <v>2231</v>
       </c>
       <c r="D13" s="1">
-        <f>IF(B13="Drive",0,2)+_xlfn.CEILING.MATH(C13/200,1)+K13</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -7835,7 +7835,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <f>IF(B14="Drive",0,2)+_xlfn.CEILING.MATH(C14/200,1)+K14</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -7879,7 +7879,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <f>IF(B15="Drive",0,2)+_xlfn.CEILING.MATH(C15/200,1)+K15</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -7923,7 +7923,7 @@
         <v>1384</v>
       </c>
       <c r="D16" s="1">
-        <f>IF(B16="Drive",0,2)+_xlfn.CEILING.MATH(C16/200,1)+K16</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">

</xml_diff>

<commit_message>
Prepare to fork draft #1
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B413607E-1851-4445-B105-41B491D9EE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2971302-3F3B-7040-8B01-98E6A59E937F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34280" yWindow="2120" windowWidth="23380" windowHeight="15340" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -3194,8 +3194,8 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4040,28 +4040,28 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="4" t="str">
+      <c r="C28" s="2" t="str">
         <f t="shared" si="1"/>
         <v>DE</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E28" s="5">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H28" s="1">
         <v>-75.524368199999998</v>

</xml_diff>

<commit_message>
Write draft #2 of the data import section
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2971302-3F3B-7040-8B01-98E6A59E937F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1B5089-0F6F-174D-BA8B-FA773A349136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-29980" yWindow="240" windowWidth="30720" windowHeight="18700" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2436,7 +2436,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2628,7 +2628,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3193,7 +3193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
@@ -7218,7 +7218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Write D2 text section and D2 progress panel
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1B5089-0F6F-174D-BA8B-FA773A349136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037C03C-6F72-DA40-9629-C94B4691BA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29980" yWindow="240" windowWidth="30720" windowHeight="18700" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-30720" yWindow="240" windowWidth="30720" windowHeight="18700" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -3193,9 +3193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7218,7 +7218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Write D2 tests, completing the revised code draft
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037C03C-6F72-DA40-9629-C94B4691BA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2B2A14-F299-C045-AFD9-D5B0424D05AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30720" yWindow="240" windowWidth="30720" windowHeight="18700" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-38040" yWindow="-1780" windowWidth="21560" windowHeight="17320" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -864,9 +864,6 @@
     <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
   </si>
   <si>
-    <t>Northeast + MD, DE, VA</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -898,6 +895,9 @@
   </si>
   <si>
     <t>Mar</t>
+  </si>
+  <si>
+    <t>Northeast + DC, DE, MD, VA</t>
   </si>
 </sst>
 </file>
@@ -2436,7 +2436,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2628,7 +2628,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3193,7 +3193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
@@ -7218,8 +7218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7280,7 +7280,7 @@
         <v>245</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -7288,7 +7288,7 @@
         <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="1">
         <v>719</v>
@@ -7298,7 +7298,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>241</v>
@@ -7344,7 +7344,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>241</v>
@@ -7390,7 +7390,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>241</v>
@@ -7425,7 +7425,7 @@
         <v>132</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C5" s="1">
         <f>1097+1202+(237*2)</f>
@@ -7481,7 +7481,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>239</v>
@@ -7561,7 +7561,7 @@
         <v>206</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C8" s="1">
         <v>2403</v>
@@ -7577,7 +7577,7 @@
         <v>239</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="H8" s="24" t="s">
         <v>256</v>
@@ -7656,10 +7656,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>221</v>
@@ -7691,7 +7691,7 @@
         <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C11" s="1">
         <f>1951+(278*2)</f>
@@ -7702,10 +7702,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>215</v>
@@ -7748,10 +7748,10 @@
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>219</v>
@@ -7794,7 +7794,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>238</v>
@@ -7829,7 +7829,7 @@
         <v>222</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -7839,10 +7839,10 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>164</v>
@@ -7883,10 +7883,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>192</v>
@@ -7927,10 +7927,10 @@
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
Substitute Helen GA -> Frankenmuth MI
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C0EA00-1173-1C41-B473-157E9DFD37B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661A834-D85D-3548-AE32-32CCB60BB3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19720" yWindow="-1820" windowWidth="22120" windowHeight="21100" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-31600" yWindow="-1820" windowWidth="16520" windowHeight="21100" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Analysis" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cities!$A$1:$F$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cities!$A$1:$J$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="305">
   <si>
     <t>Num</t>
   </si>
@@ -822,9 +822,6 @@
     <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/Honolulu,+HI/@24.8112769,-154.8564566,3z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x7c00183b8cc3464d:0x4b28f55ff3a7976c!2m2!1d-157.8583333!2d21.3069444!3e4</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/dir/Orlando,+FL/Miami,+FL/Key+West,+FL/Everglades+City,+FL/Tampa,+FL/Tarpon+Springs,+FL/Tallahassee,+FL/Jacksonville,+FL/St.+Augustine,+FL/Orlando,+FL/@27.5091232,-84.4177219,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!1m5!1m1!1s0x88d9b0a20ec8c111:0xff96f271ddad4f65!2m2!1d-80.1917902!2d25.7616798!1m5!1m1!1s0x88d1b134ad952377:0x3fcee92f77463b5e!2m2!1d-81.7799871!2d24.5550593!1m5!1m1!1s0x88da5c605ba45fb1:0x92bcf49fb504533a!2m2!1d-81.3850695!2d25.8582443!1m5!1m1!1s0x88c2b782b3b9d1e1:0xa75f1389af96b463!2m2!1d-82.4571776!2d27.950575!1m5!1m1!1s0x88c28cfd6f0942df:0xf4297f0ce0bf24b7!2m2!1d-82.7567679!2d28.1461248!1m5!1m1!1s0x88ec8a5187124b53:0xebee077ad4fdb1f8!2m2!1d-84.2807329!2d30.4382559!1m5!1m1!1s0x88e5b716f1ceafeb:0xc4cd7d3896fcc7e2!2m2!1d-81.655651!2d30.3321838!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
     <t>https://www.google.com/maps/dir/Los+Angeles,+CA/Santa+Barbara,+CA/Solvang,+CA/San+Jose,+CA/San+Francisco,+CA/Sacramento,+CA/Reno,+NV/Virginia+City,+NV/Carson+City,+NV/Fresno,+CA/@36.7777641,-122.6363689,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!1m5!1m1!1s0x80e914c76f2d83d5:0xc8d13a64d7ba7648!2m2!1d-119.6981901!2d34.4208305!1m5!1m1!1s0x80e954a0fc922285:0x2d0e281b060bc156!2m2!1d-120.1376481!2d34.5958201!1m5!1m1!1s0x808fcae48af93ff5:0xb99d8c0aca9f717b!2m2!1d-121.8863286!2d37.3382082!1m5!1m1!1s0x80859a6d00690021:0x4a501367f076adff!2m2!1d-122.4194155!2d37.7749295!1m5!1m1!1s0x809ac672b28397f9:0x921f6aaa74197fdb!2m2!1d-121.4943996!2d38.5815719!1m5!1m1!1s0x809940ae9292a09d:0x40c5c5ce7438f787!2m2!1d-119.8138027!2d39.5296329!1m5!1m1!1s0x80990faad3daafd1:0x29dad257dc576fa9!2m2!1d-119.6499793!2d39.3095135!1m5!1m1!1s0x80990aa1f8deb471:0xf79c6c82bde23828!2m2!1d-119.7674034!2d39.1637984!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!2m1!2b1!3e0!4e1</t>
   </si>
   <si>
@@ -907,6 +904,57 @@
   </si>
   <si>
     <t>https://www.google.com/maps/dir/Savannah,+GA/Charleston,+SC/Columbia,+SC/Raleigh,+NC/Arlington,+VA/@35.4655519,-81.3347427,7z/data=!3m1!4b1!4m32!4m31!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x88fe7a42dca82477:0x35faf7e0aee1ec6b!2m2!1d-79.9310512!2d32.7764749!1m5!1m1!1s0x88f8a5697931d1e3:0xf32808f4b379fa96!2m2!1d-81.0348144!2d34.0007104!1m5!1m1!1s0x89ac5a2f9f51e0f7:0x6790b6528a11f0ad!2m2!1d-78.6381787!2d35.7795897!1m5!1m1!1s0x89b7b69d7ba7a70f:0xf8cf6fc845f6b093!2m2!1d-77.1067698!2d38.8799697!3e0</t>
+  </si>
+  <si>
+    <t>Photo_Date</t>
+  </si>
+  <si>
+    <t>2021-06</t>
+  </si>
+  <si>
+    <t>2021-10</t>
+  </si>
+  <si>
+    <t>2022-03</t>
+  </si>
+  <si>
+    <t>2021-05</t>
+  </si>
+  <si>
+    <t>2022-04</t>
+  </si>
+  <si>
+    <t>2021-08</t>
+  </si>
+  <si>
+    <t>2021-11</t>
+  </si>
+  <si>
+    <t>2021-00</t>
+  </si>
+  <si>
+    <t>Currently</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Great Lakes</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Pct</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Sanford,+FL/Orlando,+FL/Miami,+FL/Key+West,+FL/Everglades+City,+FL/Tampa,+FL/Tarpon+Springs,+FL/Tallahassee,+FL/Jacksonville,+FL/St.+Augustine,+FL/@27.4662724,-86.6569807,6z/data=!3m1!4b1!4m64!4m63!1m5!1m1!1s0x88e7130dec2388f7:0xc3317e4e9680554c!2m2!1d-81.269453!2d28.8028612!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!1m5!1m1!1s0x88d9b0a20ec8c111:0xff96f271ddad4f65!2m2!1d-80.1917902!2d25.7616798!1m5!1m1!1s0x88d1b134ad952377:0x3fcee92f77463b5e!2m2!1d-81.7799871!2d24.5550593!1m5!1m1!1s0x88da5c605ba45fb1:0x92bcf49fb504533a!2m2!1d-81.3850695!2d25.8582443!1m5!1m1!1s0x88c2b782b3b9d1e1:0xa75f1389af96b463!2m2!1d-82.4571776!2d27.950575!1m5!1m1!1s0x88c28cfd6f0942df:0xf4297f0ce0bf24b7!2m2!1d-82.7567679!2d28.1461248!1m5!1m1!1s0x88ec8a5187124b53:0xebee077ad4fdb1f8!2m2!1d-84.2807329!2d30.4382559!1m5!1m1!1s0x88e5b716f1ceafeb:0xc4cd7d3896fcc7e2!2m2!1d-81.655651!2d30.3321838!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!2m1!2b1!3e0</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/St.+Augustine,+FL/Sanford,+FL/@29.3490527,-81.754888,9z/data=!3m1!4b1!4m16!4m15!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e7130dec2388f7:0xc3317e4e9680554c!2m2!1d-81.269453!2d28.8028612!2m1!2b1!3e0</t>
   </si>
 </sst>
 </file>
@@ -961,7 +1009,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -980,8 +1028,26 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1032,13 +1098,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1073,12 +1154,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3190,11 +3285,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3206,10 +3301,12 @@
     <col min="5" max="5" width="6.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="10.83203125" style="23"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3232,13 +3329,16 @@
         <v>151</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3269,7 +3369,7 @@
         <v>61.2180556</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3300,7 +3400,7 @@
         <v>64.837777799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3331,7 +3431,7 @@
         <v>36.737798099999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3361,8 +3461,11 @@
       <c r="I5" s="1">
         <v>34.052234200000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3392,8 +3495,11 @@
       <c r="I6" s="1">
         <v>33.980600500000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3424,7 +3530,7 @@
         <v>38.5815719</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3454,8 +3560,11 @@
       <c r="I8" s="1">
         <v>32.715738000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3486,7 +3595,7 @@
         <v>37.774929499999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3517,7 +3626,7 @@
         <v>37.338208199999997</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3548,7 +3657,7 @@
         <v>34.420830500000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3579,7 +3688,7 @@
         <v>39.163798399999997</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3609,7 +3718,7 @@
         <v>45.508889000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3639,7 +3748,7 @@
         <v>45.4215296</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3669,7 +3778,7 @@
         <v>46.813878299999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3699,7 +3808,7 @@
         <v>43.653225999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3729,8 +3838,9 @@
       <c r="I17" s="1">
         <v>30.332183799999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3760,8 +3870,9 @@
       <c r="I18" s="1">
         <v>24.555418299999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3791,8 +3902,9 @@
       <c r="I19" s="1">
         <v>25.7616798</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3822,8 +3934,9 @@
       <c r="I20" s="1">
         <v>28.538383199999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3853,8 +3966,9 @@
       <c r="I21" s="1">
         <v>30.438255900000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3884,8 +3998,9 @@
       <c r="I22" s="1">
         <v>27.950575000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3916,7 +4031,7 @@
         <v>33.518589200000001</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3947,7 +4062,7 @@
         <v>32.3792233</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3978,7 +4093,7 @@
         <v>33.748995399999998</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -4009,7 +4124,7 @@
         <v>32.080898900000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -4040,7 +4155,7 @@
         <v>35.227086900000003</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -4071,7 +4186,7 @@
         <v>36.072635400000003</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -4101,8 +4216,11 @@
       <c r="I29" s="1">
         <v>35.779589700000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -4133,7 +4251,7 @@
         <v>32.776474899999997</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -4164,7 +4282,7 @@
         <v>34.000710400000003</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -4195,7 +4313,7 @@
         <v>35.960638400000001</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -4226,7 +4344,7 @@
         <v>36.162663799999997</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -4257,7 +4375,7 @@
         <v>21.306944399999999</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -4287,8 +4405,9 @@
       <c r="I35" s="1">
         <v>41.878113599999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="25"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -4318,8 +4437,11 @@
       <c r="I36" s="1">
         <v>39.768402999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -4349,8 +4471,11 @@
       <c r="I37" s="1">
         <v>38.200905499999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -4380,8 +4505,11 @@
       <c r="I38" s="1">
         <v>38.252664699999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -4411,13 +4539,14 @@
       <c r="I39" s="1">
         <v>42.331426999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="25"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="2"/>
@@ -4442,8 +4571,9 @@
       <c r="I40" s="1">
         <v>43.331667000000003</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="25"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -4473,8 +4603,9 @@
       <c r="I41" s="1">
         <v>42.9633599</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="25"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -4504,8 +4635,9 @@
       <c r="I42" s="1">
         <v>42.732534999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="25"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -4535,8 +4667,11 @@
       <c r="I43" s="1">
         <v>39.103118199999997</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -4566,8 +4701,9 @@
       <c r="I44" s="1">
         <v>41.499319999999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" s="25"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -4597,8 +4733,11 @@
       <c r="I45" s="1">
         <v>39.961175500000003</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -4609,7 +4748,7 @@
         <f t="shared" si="2"/>
         <v>PA</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="D46" s="22" t="s">
         <v>131</v>
       </c>
       <c r="E46" s="1">
@@ -4628,8 +4767,9 @@
       <c r="I46" s="1">
         <v>40.440624800000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="25"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -4640,7 +4780,7 @@
         <f t="shared" si="2"/>
         <v>WI</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="22" t="s">
         <v>131</v>
       </c>
       <c r="E47" s="1">
@@ -4659,8 +4799,9 @@
       <c r="I47" s="1">
         <v>44.5133188</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" s="25"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -4690,8 +4831,9 @@
       <c r="I48" s="1">
         <v>43.073051700000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" s="25"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -4721,8 +4863,9 @@
       <c r="I49" s="1">
         <v>43.038902499999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" s="25"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -4752,8 +4895,11 @@
       <c r="I50" s="1">
         <v>38.349819500000002</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -4784,7 +4930,7 @@
         <v>36.066241900000001</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -4815,7 +4961,7 @@
         <v>34.746480900000002</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4846,7 +4992,7 @@
         <v>30.451467699999998</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4876,8 +5022,11 @@
       <c r="I54" s="1">
         <v>29.951065799999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J54" s="23" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4907,8 +5056,9 @@
       <c r="I55" s="1">
         <v>30.3674198</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55" s="24"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4939,7 +5089,7 @@
         <v>32.298757299999998</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4970,7 +5120,7 @@
         <v>35.149534299999999</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -5001,7 +5151,7 @@
         <v>30.267153</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -5032,7 +5182,7 @@
         <v>32.776664199999999</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -5063,7 +5213,7 @@
         <v>29.7604267</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -5094,7 +5244,7 @@
         <v>26.2034071</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -5125,7 +5275,7 @@
         <v>29.424121899999999</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -5155,7 +5305,7 @@
         <v>49.895136000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -5186,7 +5336,7 @@
         <v>46.786671900000002</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -5217,7 +5367,7 @@
         <v>44.977753</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -5248,7 +5398,7 @@
         <v>46.808326800000003</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -5279,7 +5429,7 @@
         <v>46.877186299999998</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -5310,7 +5460,7 @@
         <v>44.366787600000002</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -5341,7 +5491,7 @@
         <v>43.546022299999997</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -5371,8 +5521,9 @@
       <c r="I70" s="1">
         <v>41.523643700000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70" s="25"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -5402,8 +5553,11 @@
       <c r="I71" s="1">
         <v>41.586835299999997</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -5433,8 +5587,11 @@
       <c r="I72" s="1">
         <v>39.781721300000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -5445,7 +5602,7 @@
         <f t="shared" si="4"/>
         <v>KS</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D73" s="21" t="s">
         <v>134</v>
       </c>
       <c r="E73" s="1">
@@ -5464,8 +5621,11 @@
       <c r="I73" s="1">
         <v>39.047345100000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -5476,7 +5636,7 @@
         <f t="shared" si="4"/>
         <v>KS</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D74" s="21" t="s">
         <v>134</v>
       </c>
       <c r="E74" s="1">
@@ -5496,7 +5656,7 @@
         <v>37.687176100000002</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -5507,7 +5667,7 @@
         <f t="shared" si="4"/>
         <v>MO</v>
       </c>
-      <c r="D75" s="23" t="s">
+      <c r="D75" s="22" t="s">
         <v>134</v>
       </c>
       <c r="E75" s="1">
@@ -5526,8 +5686,11 @@
       <c r="I75" s="1">
         <v>38.576701700000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -5538,7 +5701,7 @@
         <f t="shared" si="4"/>
         <v>MO</v>
       </c>
-      <c r="D76" s="23" t="s">
+      <c r="D76" s="22" t="s">
         <v>134</v>
       </c>
       <c r="E76" s="1">
@@ -5557,8 +5720,11 @@
       <c r="I76" s="1">
         <v>39.099726500000003</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -5588,8 +5754,11 @@
       <c r="I77" s="1">
         <v>38.627002500000003</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -5600,7 +5769,7 @@
         <f t="shared" si="4"/>
         <v>NE</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="D78" s="21" t="s">
         <v>134</v>
       </c>
       <c r="E78" s="1">
@@ -5619,8 +5788,11 @@
       <c r="I78" s="1">
         <v>40.813616000000003</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -5631,7 +5803,7 @@
         <f t="shared" si="4"/>
         <v>NE</v>
       </c>
-      <c r="D79" s="22" t="s">
+      <c r="D79" s="21" t="s">
         <v>134</v>
       </c>
       <c r="E79" s="1">
@@ -5650,8 +5822,11 @@
       <c r="I79" s="1">
         <v>41.2565369</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -5662,7 +5837,7 @@
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="D80" s="21" t="s">
         <v>134</v>
       </c>
       <c r="E80" s="1">
@@ -5682,7 +5857,7 @@
         <v>35.467560200000001</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -5693,7 +5868,7 @@
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="D81" s="21" t="s">
         <v>134</v>
       </c>
       <c r="E81" s="1">
@@ -5713,7 +5888,7 @@
         <v>36.153981600000002</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -5744,7 +5919,7 @@
         <v>33.448377100000002</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -5775,7 +5950,7 @@
         <v>32.222606599999999</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -5806,7 +5981,7 @@
         <v>35.084385900000001</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -5837,7 +6012,7 @@
         <v>35.686975199999999</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -5868,7 +6043,7 @@
         <v>36.407213400000003</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -5898,8 +6073,11 @@
       <c r="I87" s="1">
         <v>36.169941199999997</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -5930,7 +6108,7 @@
         <v>31.761877800000001</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -5961,7 +6139,7 @@
         <v>33.577863100000002</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -5992,7 +6170,7 @@
         <v>37.096527799999997</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -6003,7 +6181,7 @@
         <f t="shared" si="4"/>
         <v>CT</v>
       </c>
-      <c r="D91" s="23" t="s">
+      <c r="D91" s="22" t="s">
         <v>205</v>
       </c>
       <c r="E91" s="1">
@@ -6022,8 +6200,11 @@
       <c r="I91" s="1">
         <v>41.765804299999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J91" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -6034,7 +6215,7 @@
         <f t="shared" si="4"/>
         <v>DC</v>
       </c>
-      <c r="D92" s="23" t="s">
+      <c r="D92" s="22" t="s">
         <v>205</v>
       </c>
       <c r="E92" s="1">
@@ -6053,8 +6234,11 @@
       <c r="I92" s="1">
         <v>38.907192299999998</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J92" s="23" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -6084,8 +6268,11 @@
       <c r="I93" s="1">
         <v>39.158168000000003</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J93" s="23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -6116,7 +6303,7 @@
         <v>41.7003208</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -6146,8 +6333,11 @@
       <c r="I95" s="1">
         <v>42.360082499999997</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J95" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -6155,7 +6345,7 @@
         <v>65</v>
       </c>
       <c r="C96" s="2" t="str">
-        <f t="shared" ref="C96:C127" si="6">RIGHT(B96,2)</f>
+        <f t="shared" ref="C96:C113" si="6">RIGHT(B96,2)</f>
         <v>MD</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -6177,39 +6367,43 @@
       <c r="I96" s="1">
         <v>38.978445299999997</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J96" s="23" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B97" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C97" s="20" t="str">
+      <c r="C97" s="2" t="str">
         <f t="shared" si="6"/>
         <v>MD</v>
       </c>
-      <c r="D97" s="21" t="s">
+      <c r="D97" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E97" s="21">
-        <v>1</v>
-      </c>
-      <c r="F97" s="21">
-        <v>0</v>
-      </c>
-      <c r="G97" s="21">
+      <c r="E97" s="1">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H97" s="21">
+      <c r="H97" s="1">
         <v>-76.612189299999997</v>
       </c>
-      <c r="I97" s="21">
+      <c r="I97" s="1">
         <v>39.290384799999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J97" s="26"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -6239,8 +6433,11 @@
       <c r="I98" s="1">
         <v>44.310624099999998</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J98" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -6270,8 +6467,11 @@
       <c r="I99" s="1">
         <v>43.659099300000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J99" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -6301,8 +6501,11 @@
       <c r="I100" s="1">
         <v>43.208136600000003</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J100" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -6332,8 +6535,11 @@
       <c r="I101" s="1">
         <v>40.220582399999998</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J101" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -6363,8 +6569,11 @@
       <c r="I102" s="1">
         <v>42.652579299999999</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J102" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -6394,8 +6603,11 @@
       <c r="I103" s="1">
         <v>42.886446800000002</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J103" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -6425,8 +6637,11 @@
       <c r="I104" s="1">
         <v>40.712775299999997</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J104" s="23" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -6456,8 +6671,11 @@
       <c r="I105" s="1">
         <v>43.156577900000002</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J105" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -6487,8 +6705,11 @@
       <c r="I106" s="1">
         <v>40.273191099999998</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J106" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -6518,8 +6739,11 @@
       <c r="I107" s="1">
         <v>39.9525839</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J107" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -6549,8 +6773,11 @@
       <c r="I108" s="1">
         <v>41.823989099999999</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J108" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -6580,39 +6807,43 @@
       <c r="I109" s="1">
         <v>38.029305899999997</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J109" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B110" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C110" s="20" t="str">
+      <c r="C110" s="2" t="str">
         <f t="shared" si="6"/>
         <v>VA</v>
       </c>
-      <c r="D110" s="21" t="s">
+      <c r="D110" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E110" s="21">
-        <v>1</v>
-      </c>
-      <c r="F110" s="21">
-        <v>0</v>
-      </c>
-      <c r="G110" s="21">
+      <c r="E110" s="1">
+        <v>1</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0</v>
+      </c>
+      <c r="G110" s="1">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="H110" s="21">
+      <c r="H110" s="1">
         <v>-76.285872600000005</v>
       </c>
-      <c r="I110" s="21">
+      <c r="I110" s="1">
         <v>36.850768899999998</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J110" s="26"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -6642,8 +6873,11 @@
       <c r="I111" s="1">
         <v>37.540724599999997</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J111" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -6673,8 +6907,11 @@
       <c r="I112" s="1">
         <v>44.475882499999997</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J112" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -6704,8 +6941,11 @@
       <c r="I113" s="1">
         <v>44.260059300000002</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J113" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -6735,7 +6975,7 @@
         <v>49.282729099999997</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -6766,7 +7006,7 @@
         <v>45.515231999999997</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -6797,7 +7037,7 @@
         <v>44.942897500000001</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -6827,8 +7067,9 @@
       <c r="I117" s="1">
         <v>47.037874100000003</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J117" s="24"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -6859,7 +7100,7 @@
         <v>47.606209499999999</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -6890,7 +7131,7 @@
         <v>47.658780200000002</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -6921,7 +7162,7 @@
         <v>18.465539400000001</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -6952,7 +7193,7 @@
         <v>39.739235800000003</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -6983,7 +7224,7 @@
         <v>39.0638705</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -7014,7 +7255,7 @@
         <v>43.615018599999999</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -7045,7 +7286,7 @@
         <v>43.492660700000002</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -7076,7 +7317,7 @@
         <v>45.783285599999999</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -7107,7 +7348,7 @@
         <v>46.589145199999997</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -7138,7 +7379,7 @@
         <v>40.760779300000003</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -7201,11 +7442,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F129" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F129">
-      <sortCondition ref="A1:A129"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:J129" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I129">
     <sortCondition ref="D2:D129"/>
     <sortCondition ref="C2:C129"/>
@@ -7219,8 +7456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7286,7 +7523,7 @@
         <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" s="1">
         <v>719</v>
@@ -7299,7 +7536,7 @@
         <v>239</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>152</v>
@@ -7342,7 +7579,7 @@
         <v>239</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>133</v>
@@ -7382,10 +7619,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>213</v>
@@ -7424,7 +7661,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>240</v>
@@ -7466,10 +7703,10 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>219</v>
@@ -7498,7 +7735,7 @@
         <v>205</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="1">
         <v>2403</v>
@@ -7508,13 +7745,13 @@
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>255</v>
@@ -7540,7 +7777,7 @@
         <v>131</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="1">
         <v>2652</v>
@@ -7550,19 +7787,19 @@
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>216</v>
       </c>
       <c r="H8" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>284</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>285</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>250</v>
@@ -7592,7 +7829,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>238</v>
@@ -7618,7 +7855,7 @@
         <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C10" s="1">
         <v>2339</v>
@@ -7628,7 +7865,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>238</v>
@@ -7637,10 +7874,10 @@
         <v>214</v>
       </c>
       <c r="H10" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="I10" s="18" t="s">
         <v>287</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>288</v>
       </c>
       <c r="J10" s="18" t="s">
         <v>250</v>
@@ -7671,7 +7908,7 @@
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>238</v>
@@ -7680,10 +7917,10 @@
         <v>218</v>
       </c>
       <c r="H11" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="I11" s="18" t="s">
         <v>263</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>264</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>250</v>
@@ -7714,19 +7951,19 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>220</v>
       </c>
       <c r="H12" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>261</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>262</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>250</v>
@@ -7757,19 +7994,19 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>215</v>
       </c>
       <c r="H13" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="I13" s="18" t="s">
         <v>265</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>266</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>250</v>
@@ -7789,7 +8026,7 @@
         <v>221</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -7799,7 +8036,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>237</v>
@@ -7840,7 +8077,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>237</v>
@@ -7874,14 +8111,14 @@
         <v>211</v>
       </c>
       <c r="C16" s="1">
-        <v>1384</v>
+        <v>1396</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>237</v>
@@ -7889,13 +8126,15 @@
       <c r="G16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H16" s="18" t="s">
-        <v>260</v>
+      <c r="H16" s="29" t="s">
+        <v>303</v>
       </c>
       <c r="I16" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="J16" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="J16" s="18"/>
       <c r="K16" s="1">
         <v>0</v>
       </c>
@@ -7917,10 +8156,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01B0898-0BB8-CE48-8A78-B23E3CEFACCF}">
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7936,7 +8175,7 @@
     <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>147</v>
       </c>
@@ -7959,7 +8198,7 @@
       </c>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>141</v>
       </c>
@@ -7986,7 +8225,7 @@
       </c>
       <c r="M2" s="10"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>139</v>
       </c>
@@ -8013,7 +8252,7 @@
       </c>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
@@ -8033,7 +8272,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>130</v>
       </c>
@@ -8051,7 +8290,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>129</v>
       </c>
@@ -8069,7 +8308,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>131</v>
       </c>
@@ -8087,7 +8326,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>136</v>
       </c>
@@ -8105,7 +8344,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>132</v>
       </c>
@@ -8123,7 +8362,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>134</v>
       </c>
@@ -8141,7 +8380,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>138</v>
       </c>
@@ -8159,7 +8398,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>205</v>
       </c>
@@ -8177,7 +8416,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>140</v>
       </c>
@@ -8194,8 +8433,14 @@
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M13" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>143</v>
       </c>
@@ -8212,8 +8457,17 @@
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L14" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="M14" s="1">
+        <v>40</v>
+      </c>
+      <c r="N14" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>142</v>
       </c>
@@ -8230,8 +8484,19 @@
       <c r="G15" s="8"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L15" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M15" s="1">
+        <f>M14+2</f>
+        <v>42</v>
+      </c>
+      <c r="N15" s="1">
+        <f>N14+0</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>204</v>
       </c>
@@ -8240,8 +8505,19 @@
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L16" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="M16" s="1">
+        <f>M15+11</f>
+        <v>53</v>
+      </c>
+      <c r="N16" s="1">
+        <f>N15+2</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>148</v>
       </c>
@@ -8255,8 +8531,19 @@
         <v>150</v>
       </c>
       <c r="E17" s="13"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L17" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="M17" s="1">
+        <f>M16+6</f>
+        <v>59</v>
+      </c>
+      <c r="N17" s="1">
+        <f>N16+1</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>147</v>
       </c>
@@ -8267,8 +8554,19 @@
         <v>208</v>
       </c>
       <c r="D19" s="16"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L19" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M19" s="1">
+        <f>M17-M14</f>
+        <v>19</v>
+      </c>
+      <c r="N19" s="1">
+        <f>N17-N14</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>152</v>
       </c>
@@ -8279,8 +8577,19 @@
         <v>0</v>
       </c>
       <c r="D20" s="16"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L20" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="M20" s="28">
+        <f>M19/M14</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="N20" s="28">
+        <f>N19/N14</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>153</v>
       </c>
@@ -8292,7 +8601,7 @@
       </c>
       <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>154</v>
       </c>
@@ -8304,7 +8613,7 @@
       </c>
       <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>155</v>
       </c>
@@ -8316,7 +8625,7 @@
       </c>
       <c r="D23" s="16"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>156</v>
       </c>
@@ -8328,7 +8637,7 @@
       </c>
       <c r="D24" s="16"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>133</v>
       </c>
@@ -8340,7 +8649,7 @@
       </c>
       <c r="D25" s="16"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>157</v>
       </c>
@@ -8352,7 +8661,7 @@
       </c>
       <c r="D26" s="16"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>158</v>
       </c>
@@ -8364,7 +8673,7 @@
       </c>
       <c r="D27" s="16"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>159</v>
       </c>
@@ -8376,7 +8685,7 @@
       </c>
       <c r="D28" s="16"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>160</v>
       </c>
@@ -8388,7 +8697,7 @@
       </c>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>161</v>
       </c>
@@ -8400,7 +8709,7 @@
       </c>
       <c r="D30" s="16"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>162</v>
       </c>
@@ -8412,7 +8721,7 @@
       </c>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
Update Baltimore checklist status
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661A834-D85D-3548-AE32-32CCB60BB3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B17E30-5041-EF41-B6F4-F118A11F5BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31600" yWindow="-1820" windowWidth="16520" windowHeight="21100" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="13320" yWindow="500" windowWidth="18380" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="306">
   <si>
     <t>Num</t>
   </si>
@@ -955,6 +955,9 @@
   </si>
   <si>
     <t>https://www.google.com/maps/dir/St.+Augustine,+FL/Sanford,+FL/@29.3490527,-81.754888,9z/data=!3m1!4b1!4m16!4m15!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e7130dec2388f7:0xc3317e4e9680554c!2m2!1d-81.269453!2d28.8028612!2m1!2b1!3e0</t>
+  </si>
+  <si>
+    <t>2022-08</t>
   </si>
 </sst>
 </file>
@@ -3287,9 +3290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6389,11 +6392,11 @@
         <v>1</v>
       </c>
       <c r="F97" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" s="1">
         <v>-76.612189299999997</v>
@@ -6401,7 +6404,9 @@
       <c r="I97" s="1">
         <v>39.290384799999998</v>
       </c>
-      <c r="J97" s="26"/>
+      <c r="J97" s="23" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
@@ -7456,7 +7461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reduce the scope of the OR and MN routes
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE82A48-B753-3843-B312-371CBD25FB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243551C4-C89F-C84D-B2CA-CE8849590B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="500" windowWidth="18380" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="9240" yWindow="500" windowWidth="24800" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
     <sheet name="Routes" sheetId="3" r:id="rId2"/>
     <sheet name="Analysis" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cities!$A$1:$J$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -675,9 +676,6 @@
     <t>CO, ID, MT, UT, WY</t>
   </si>
   <si>
-    <t>MN, ND, SD, CAN</t>
-  </si>
-  <si>
     <t>AL, GA, NC, SC, TN</t>
   </si>
   <si>
@@ -693,9 +691,6 @@
     <t>AZ, NM, NV, TX, UT</t>
   </si>
   <si>
-    <t>CA, OR, WA, CAN</t>
-  </si>
-  <si>
     <t>CA, NV</t>
   </si>
   <si>
@@ -795,12 +790,6 @@
     <t>https://www.google.com/maps/dir/Denver,+CO/Grand+Junction,+CO/Salt+Lake+City,+UT/Boise,+ID/Idaho+Falls,+ID/Helena,+MT/Billings,+MT/Casper,+WY/Cheyenne,+WY/Denver,+Colorado/@42.4201276,-119.4822548,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!1m5!1m1!1s0x8746d6e322e77057:0xcc63f451cebf7c56!2m2!1d-108.5506486!2d39.0638705!1m5!1m1!1s0x87523d9488d131ed:0x5b53b7a0484d31ca!2m2!1d-111.8910474!2d40.7607793!1m5!1m1!1s0x54aef172e947b49d:0x9a5b989b36679d9b!2m2!1d-116.2023137!2d43.6150186!1m5!1m1!1s0x5354594e739512b5:0x2311c9fc094c49c9!2m2!1d-112.0407584!2d43.4926607!1m5!1m1!1s0x5343510fedc7db4d:0x214c1d71e3fdf714!2m2!1d-112.0391057!2d46.5891452!1m5!1m1!1s0x53486f8888fa9d97:0x373556d4f179b550!2m2!1d-108.5006904!2d45.7832856!1m5!1m1!1s0x87609365c85e7a63:0x69cefc3917343e53!2m2!1d-106.2980824!2d42.848709!1m5!1m1!1s0x876f38762e73ef93:0xb10a30418f972d2b!2m2!1d-104.8202462!2d41.1399814!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!2m1!2b1!3e0!4e1</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/dir/Minneapolis,+MN/Sioux+Falls,+SD/Pierre,+SD/Bismarck,+ND/Fargo,+ND/Winnipeg,+MB,+Canada/Duluth,+MN/Minneapolis,+MN/@46.6404497,-100.928197,6z/data=!3m1!4b1!4m53!4m52!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!1m5!1m1!1s0x878eb498e0bdacd7:0xde95ff3aa8b2fccf!2m2!1d-96.731265!2d43.5460223!1m5!1m1!1s0x52d54a64b288f891:0x9e9950165931af92!2m2!1d-100.3537522!2d44.3667876!1m5!1m1!1s0x52d7831257d8e963:0xccaabd12f9bbca93!2m2!1d-100.7837392!2d46.8083268!1m5!1m1!1s0x52c8cb8d84677145:0x81aa30a52791aaca!2m2!1d-96.7898034!2d46.8771863!1m5!1m1!1s0x52ea73fbf91a2b11:0x2b2a1afac6b9ca64!2m2!1d-97.1383744!2d49.895136!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Seattle,+WA/Vancouver,+BC,+Canada/Leavenworth,+WA/Spokane,+WA/Redding,+CA/Gold+Beach,+OR/Salem,+OR/Portland,+OR/Olympia,+WA/Seattle,+WA/@44.8374018,-125.1438928,6.26z/data=!4m65!4m64!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!1m5!1m1!1s0x548673f143a94fb3:0xbb9196ea9b81f38b!2m2!1d-123.1207375!2d49.2827291!1m5!1m1!1s0x549a4d92a4f8f98d:0xa14f95fb0abfef7e!2m2!1d-120.6614765!2d47.5962326!1m5!1m1!1s0x549e185c30bbe7e5:0xddfcc9d60b84d9b1!2m2!1d-117.4260465!2d47.6587802!1m5!1m1!1s0x54d291d63b4a202f:0x1f3358ec7b360f57!2m2!1d-122.3916754!2d40.5865396!1m5!1m1!1s0x54dace49bf9ae73d:0x121195079f68806d!2m2!1d-124.4217741!2d42.4073334!1m5!1m1!1s0x54bffefcbc4b9c63:0xf93429e08f0357c2!2m2!1d-123.0350963!2d44.9428975!1m5!1m1!1s0x54950b0b7da97427:0x1c36b9e6f6d18591!2m2!1d-122.6783853!2d45.515232!1m5!1m1!1s0x5491c9c1ae285569:0x4f146197e2881b83!2m2!1d-122.9006951!2d47.0378741!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
     <t>https://www.google.com/maps/dir/Albany,+NY/Burlington,+VT/Montpelier,+VT/Concord,+NH/Augusta,+ME/Portland,+ME/Boston,+MA/Barnstable,+MA/Providence,+RI/Hartford,+CT/@41.8793352,-74.5474305,7z/data=!4m65!4m64!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!1m5!1m1!1s0x4cca7a55b69b55e5:0xc35fe519720e498e!2m2!1d-73.212072!2d44.4758825!1m5!1m1!1s0x4cb5a78cc44dea05:0x4891e094ceb5836!2m2!1d-72.5753869!2d44.2600593!1m5!1m1!1s0x89e26a96154a8917:0x5a871a0a62528f1!2m2!1d-71.5375718!2d43.2081366!1m5!1m1!1s0x4cb200fdafacc49d:0x79a3488d64220b2d!2m2!1d-69.7794897!2d44.3106241!1m5!1m1!1s0x4cb29c72aab0ee2d:0x7e9db6b53372fa29!2m2!1d-70.2568189!2d43.6590993!1m5!1m1!1s0x89e3652d0d3d311b:0x787cbf240162e8a0!2m2!1d-71.0588801!2d42.3600825!1m5!1m1!1s0x89fb33b67f8ec5e5:0xea7648efbb136d73!2m2!1d-70.3002024!2d41.7003208!1m5!1m1!1s0x89e444e0437e735d:0x69df7c4d48b3b627!2m2!1d-71.4128343!2d41.8239891!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!2m1!2b1!3e0!4e1</t>
   </si>
   <si>
@@ -955,6 +944,18 @@
   </si>
   <si>
     <t>Taos NM</t>
+  </si>
+  <si>
+    <t>MN, ND, SD</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Duluth,+Minnesota/Minneapolis,+MN/Sioux+Falls,+SD/Pierre,+SD/Bismarck,+ND/Fargo,+ND/Duluth,+MN/@44.9724271,-105.4148687,5z/data=!3m1!4b1!4m44!4m43!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!1m5!1m1!1s0x878eb498e0bdacd7:0xde95ff3aa8b2fccf!2m2!1d-96.731265!2d43.5460223!1m5!1m1!1s0x52d54a64b288f891:0x9e9950165931af92!2m2!1d-100.3537522!2d44.3667876!1m5!1m1!1s0x52d7831257d8e963:0xccaabd12f9bbca93!2m2!1d-100.7876931!2d46.8054947!1m5!1m1!1s0x52c8cb8d84677145:0x81aa30a52791aaca!2m2!1d-96.7898034!2d46.8771863!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!3e0</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Seattle,+WA/Olympia,+WA/Portland,+OR/Salem,+OR/Spokane,+WA/Seattle,+WA/@46.2205565,-124.7181307,6z/data=!3m1!4b1!4m38!4m37!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!1m5!1m1!1s0x5491c9c1ae285569:0x4f146197e2881b83!2m2!1d-122.9006951!2d47.0378741!1m5!1m1!1s0x54950b0b7da97427:0x1c36b9e6f6d18591!2m2!1d-122.6783853!2d45.515232!1m5!1m1!1s0x54bffefcbc4b9c63:0xf93429e08f0357c2!2m2!1d-123.0350963!2d44.9428975!1m5!1m1!1s0x549e185c30bbe7e5:0xddfcc9d60b84d9b1!2m2!1d-117.4260465!2d47.6587802!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!3e0</t>
+  </si>
+  <si>
+    <t>OR, WA</t>
   </si>
 </sst>
 </file>
@@ -965,7 +966,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1008,8 +1009,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,26 +1038,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="1"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1F4E78"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1167,18 +1163,18 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1266,7 +1262,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="44614.534418055555" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="129" xr:uid="{EA2F0253-6C76-7441-B1BF-F3AA56816A8F}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:G1048576" sheet="Cities"/>
+    <worksheetSource ref="A1:F1048576" sheet="Cities"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Num" numFmtId="0">
@@ -2537,7 +2533,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF45142-A6BF-5043-B5DB-C6D8F20294A7}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C74" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2804,7 +2800,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E27A4137-60C9-F84F-8E12-E06B21833754}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3292,11 +3288,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H82" sqref="H82"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J118" sqref="J118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3336,13 +3332,13 @@
         <v>149</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3469,7 +3465,7 @@
         <v>34.052234200000001</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -3503,7 +3499,7 @@
         <v>33.980600500000001</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -3568,7 +3564,7 @@
         <v>32.715738000000002</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3845,7 +3841,6 @@
       <c r="I17" s="1">
         <v>30.332183799999999</v>
       </c>
-      <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -3877,7 +3872,6 @@
       <c r="I18" s="1">
         <v>24.555418299999999</v>
       </c>
-      <c r="J18" s="25"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -3909,7 +3903,6 @@
       <c r="I19" s="1">
         <v>25.7616798</v>
       </c>
-      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -3941,7 +3934,6 @@
       <c r="I20" s="1">
         <v>28.538383199999998</v>
       </c>
-      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -3973,7 +3965,6 @@
       <c r="I21" s="1">
         <v>30.438255900000001</v>
       </c>
-      <c r="J21" s="25"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -4005,7 +3996,6 @@
       <c r="I22" s="1">
         <v>27.950575000000001</v>
       </c>
-      <c r="J22" s="25"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
@@ -4224,7 +4214,7 @@
         <v>35.779589700000002</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -4363,7 +4353,7 @@
         <v>HI</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -4412,8 +4402,8 @@
       <c r="I35" s="1">
         <v>41.878113599999999</v>
       </c>
-      <c r="J35" s="23" t="s">
-        <v>302</v>
+      <c r="J35" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -4447,7 +4437,7 @@
         <v>39.768402999999999</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -4481,7 +4471,7 @@
         <v>38.200905499999998</v>
       </c>
       <c r="J37" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -4515,7 +4505,7 @@
         <v>38.252664699999997</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -4548,8 +4538,8 @@
       <c r="I39" s="1">
         <v>42.331426999999998</v>
       </c>
-      <c r="J39" s="23" t="s">
-        <v>302</v>
+      <c r="J39" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -4582,8 +4572,8 @@
       <c r="I40" s="1">
         <v>42.9633599</v>
       </c>
-      <c r="J40" s="23" t="s">
-        <v>302</v>
+      <c r="J40" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -4616,8 +4606,8 @@
       <c r="I41" s="1">
         <v>42.732534999999999</v>
       </c>
-      <c r="J41" s="23" t="s">
-        <v>302</v>
+      <c r="J41" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -4651,7 +4641,7 @@
         <v>39.103118199999997</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -4684,8 +4674,8 @@
       <c r="I43" s="1">
         <v>41.499319999999997</v>
       </c>
-      <c r="J43" s="23" t="s">
-        <v>302</v>
+      <c r="J43" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -4719,7 +4709,7 @@
         <v>39.961175500000003</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -4752,8 +4742,8 @@
       <c r="I45" s="1">
         <v>40.440624800000002</v>
       </c>
-      <c r="J45" s="23" t="s">
-        <v>302</v>
+      <c r="J45" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -4786,8 +4776,8 @@
       <c r="I46" s="1">
         <v>44.5133188</v>
       </c>
-      <c r="J46" s="23" t="s">
-        <v>302</v>
+      <c r="J46" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4820,8 +4810,8 @@
       <c r="I47" s="1">
         <v>43.073051700000001</v>
       </c>
-      <c r="J47" s="23" t="s">
-        <v>302</v>
+      <c r="J47" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -4854,8 +4844,8 @@
       <c r="I48" s="1">
         <v>43.038902499999999</v>
       </c>
-      <c r="J48" s="23" t="s">
-        <v>302</v>
+      <c r="J48" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -4889,7 +4879,7 @@
         <v>38.349819500000002</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -5016,7 +5006,7 @@
         <v>29.951065799999999</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -5273,10 +5263,11 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>131</v>
+        <v>18</v>
+      </c>
+      <c r="C62" s="2" t="str">
+        <f t="shared" ref="C62:C93" si="4">RIGHT(B62,2)</f>
+        <v>MN</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>130</v>
@@ -5292,10 +5283,10 @@
         <v>2</v>
       </c>
       <c r="H62" s="1">
-        <v>-97.138374400000004</v>
+        <v>-92.100485199999994</v>
       </c>
       <c r="I62" s="1">
-        <v>49.895136000000001</v>
+        <v>46.786671900000002</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -5303,10 +5294,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C63" s="2" t="str">
-        <f t="shared" ref="C63:C93" si="4">RIGHT(B63,2)</f>
+        <f t="shared" si="4"/>
         <v>MN</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -5323,10 +5314,10 @@
         <v>2</v>
       </c>
       <c r="H63" s="1">
-        <v>-92.100485199999994</v>
+        <v>-93.265010799999999</v>
       </c>
       <c r="I63" s="1">
-        <v>46.786671900000002</v>
+        <v>44.977753</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -5334,11 +5325,11 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C64" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>MN</v>
+        <v>ND</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>130</v>
@@ -5354,10 +5345,10 @@
         <v>2</v>
       </c>
       <c r="H64" s="1">
-        <v>-93.265010799999999</v>
+        <v>-100.7837392</v>
       </c>
       <c r="I64" s="1">
-        <v>44.977753</v>
+        <v>46.808326800000003</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -5365,7 +5356,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C65" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5381,14 +5372,14 @@
         <v>0</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" ref="G65:G95" si="5">((1-E65)-(1-F65))+((1-F65)*2)</f>
+        <f t="shared" ref="G65:G96" si="5">((1-E65)-(1-F65))+((1-F65)*2)</f>
         <v>2</v>
       </c>
       <c r="H65" s="1">
-        <v>-100.7837392</v>
+        <v>-96.789803399999997</v>
       </c>
       <c r="I65" s="1">
-        <v>46.808326800000003</v>
+        <v>46.877186299999998</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -5396,11 +5387,11 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C66" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>ND</v>
+        <v>SD</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>130</v>
@@ -5416,10 +5407,10 @@
         <v>2</v>
       </c>
       <c r="H66" s="1">
-        <v>-96.789803399999997</v>
+        <v>-100.3537522</v>
       </c>
       <c r="I66" s="1">
-        <v>46.877186299999998</v>
+        <v>44.366787600000002</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -5427,7 +5418,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5447,10 +5438,10 @@
         <v>2</v>
       </c>
       <c r="H67" s="1">
-        <v>-100.3537522</v>
+        <v>-96.731264999999993</v>
       </c>
       <c r="I67" s="1">
-        <v>44.366787600000002</v>
+        <v>43.546022299999997</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -5458,30 +5449,33 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C68" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>SD</v>
+        <v>IA</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H68" s="1">
-        <v>-96.731264999999993</v>
+        <v>-90.577636699999999</v>
       </c>
       <c r="I68" s="1">
-        <v>43.546022299999997</v>
+        <v>41.523643700000001</v>
+      </c>
+      <c r="J68" s="25" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -5489,7 +5483,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="C69" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5509,13 +5503,13 @@
         <v>0</v>
       </c>
       <c r="H69" s="1">
-        <v>-90.577636699999999</v>
+        <v>-93.6249593</v>
       </c>
       <c r="I69" s="1">
-        <v>41.523643700000001</v>
-      </c>
-      <c r="J69" s="28" t="s">
-        <v>302</v>
+        <v>41.586835299999997</v>
+      </c>
+      <c r="J69" s="21" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -5523,11 +5517,11 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="C70" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>IA</v>
+        <v>IL</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>132</v>
@@ -5543,13 +5537,13 @@
         <v>0</v>
       </c>
       <c r="H70" s="1">
-        <v>-93.6249593</v>
+        <v>-89.650148099999996</v>
       </c>
       <c r="I70" s="1">
-        <v>41.586835299999997</v>
+        <v>39.781721300000001</v>
       </c>
       <c r="J70" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -5557,13 +5551,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C71" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>IL</v>
-      </c>
-      <c r="D71" s="1" t="s">
+        <v>KS</v>
+      </c>
+      <c r="D71" s="19" t="s">
         <v>132</v>
       </c>
       <c r="E71" s="1">
@@ -5577,13 +5571,13 @@
         <v>0</v>
       </c>
       <c r="H71" s="1">
-        <v>-89.650148099999996</v>
+        <v>-95.675157600000006</v>
       </c>
       <c r="I71" s="1">
-        <v>39.781721300000001</v>
+        <v>39.047345100000001</v>
       </c>
       <c r="J71" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -5591,7 +5585,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C72" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5601,23 +5595,20 @@
         <v>132</v>
       </c>
       <c r="E72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H72" s="1">
-        <v>-95.675157600000006</v>
+        <v>-97.330053000000007</v>
       </c>
       <c r="I72" s="1">
-        <v>39.047345100000001</v>
-      </c>
-      <c r="J72" s="21" t="s">
-        <v>287</v>
+        <v>37.687176100000002</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -5625,30 +5616,33 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C73" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>KS</v>
-      </c>
-      <c r="D73" s="19" t="s">
+        <v>MO</v>
+      </c>
+      <c r="D73" s="20" t="s">
         <v>132</v>
       </c>
       <c r="E73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="1">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H73" s="1">
-        <v>-97.330053000000007</v>
+        <v>-92.173516399999997</v>
       </c>
       <c r="I73" s="1">
-        <v>37.687176100000002</v>
+        <v>38.576701700000001</v>
+      </c>
+      <c r="J73" s="21" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -5656,7 +5650,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C74" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5676,13 +5670,13 @@
         <v>0</v>
       </c>
       <c r="H74" s="1">
-        <v>-92.173516399999997</v>
+        <v>-94.578566699999996</v>
       </c>
       <c r="I74" s="1">
-        <v>38.576701700000001</v>
+        <v>39.099726500000003</v>
       </c>
       <c r="J74" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -5690,13 +5684,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C75" s="2" t="str">
         <f t="shared" si="4"/>
         <v>MO</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D75" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E75" s="1">
@@ -5710,13 +5704,13 @@
         <v>0</v>
       </c>
       <c r="H75" s="1">
-        <v>-94.578566699999996</v>
+        <v>-90.199404200000004</v>
       </c>
       <c r="I75" s="1">
-        <v>39.099726500000003</v>
+        <v>38.627002500000003</v>
       </c>
       <c r="J75" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -5724,13 +5718,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C76" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>MO</v>
-      </c>
-      <c r="D76" s="1" t="s">
+        <v>NE</v>
+      </c>
+      <c r="D76" s="19" t="s">
         <v>132</v>
       </c>
       <c r="E76" s="1">
@@ -5744,13 +5738,13 @@
         <v>0</v>
       </c>
       <c r="H76" s="1">
-        <v>-90.199404200000004</v>
+        <v>-96.702595500000001</v>
       </c>
       <c r="I76" s="1">
-        <v>38.627002500000003</v>
+        <v>40.813616000000003</v>
       </c>
       <c r="J76" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -5758,7 +5752,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C77" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5778,13 +5772,13 @@
         <v>0</v>
       </c>
       <c r="H77" s="1">
-        <v>-96.702595500000001</v>
+        <v>-95.934503399999997</v>
       </c>
       <c r="I77" s="1">
-        <v>40.813616000000003</v>
+        <v>41.2565369</v>
       </c>
       <c r="J77" s="21" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
@@ -5792,33 +5786,30 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="C78" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>NE</v>
+        <v>OK</v>
       </c>
       <c r="D78" s="19" t="s">
         <v>132</v>
       </c>
       <c r="E78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H78" s="1">
-        <v>-95.934503399999997</v>
+        <v>-97.5164276</v>
       </c>
       <c r="I78" s="1">
-        <v>41.2565369</v>
-      </c>
-      <c r="J78" s="21" t="s">
-        <v>287</v>
+        <v>35.467560200000001</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
@@ -5826,7 +5817,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C79" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5846,10 +5837,10 @@
         <v>2</v>
       </c>
       <c r="H79" s="1">
-        <v>-97.5164276</v>
+        <v>-95.992774999999995</v>
       </c>
       <c r="I79" s="1">
-        <v>35.467560200000001</v>
+        <v>36.153981600000002</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
@@ -5857,30 +5848,30 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C80" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>132</v>
+        <v>AZ</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="E80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" s="1">
         <v>0</v>
       </c>
       <c r="G80" s="1">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H80" s="1">
-        <v>-95.992774999999995</v>
+        <v>-112.0740373</v>
       </c>
       <c r="I80" s="1">
-        <v>36.153981600000002</v>
+        <v>33.448377100000002</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -5888,7 +5879,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C81" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5898,20 +5889,20 @@
         <v>136</v>
       </c>
       <c r="E81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" s="1">
         <v>0</v>
       </c>
       <c r="G81" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H81" s="1">
-        <v>-112.0740373</v>
+        <v>-110.9747108</v>
       </c>
       <c r="I81" s="1">
-        <v>33.448377100000002</v>
+        <v>32.222606599999999</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -5919,30 +5910,33 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="C82" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>AZ</v>
+        <v>NM</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="1">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H82" s="1">
-        <v>-110.9747108</v>
+        <v>-106.65042200000001</v>
       </c>
       <c r="I82" s="1">
-        <v>32.222606599999999</v>
+        <v>35.084385900000001</v>
+      </c>
+      <c r="J82" s="21" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
@@ -5950,7 +5944,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="C83" s="2" t="str">
         <f t="shared" si="4"/>
@@ -5970,13 +5964,13 @@
         <v>0</v>
       </c>
       <c r="H83" s="1">
-        <v>-106.65042200000001</v>
+        <v>-105.937799</v>
       </c>
       <c r="I83" s="1">
-        <v>35.084385900000001</v>
+        <v>35.686975199999999</v>
       </c>
       <c r="J83" s="21" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
@@ -5984,7 +5978,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>144</v>
+        <v>300</v>
       </c>
       <c r="C84" s="2" t="str">
         <f t="shared" si="4"/>
@@ -6004,18 +5998,18 @@
         <v>0</v>
       </c>
       <c r="H84" s="1">
-        <v>-105.937799</v>
+        <v>-105.576667</v>
       </c>
       <c r="I84" s="1">
-        <v>35.686975199999999</v>
+        <v>36.393889000000001</v>
       </c>
       <c r="J84" s="21" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>103</v>
@@ -6044,12 +6038,12 @@
         <v>36.169941199999997</v>
       </c>
       <c r="J85" s="21" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>77</v>
@@ -6080,7 +6074,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>79</v>
@@ -6111,7 +6105,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>107</v>
@@ -6120,7 +6114,7 @@
         <f t="shared" si="4"/>
         <v>UT</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" s="20" t="s">
         <v>136</v>
       </c>
       <c r="E88" s="1">
@@ -6142,7 +6136,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>16</v>
@@ -6171,12 +6165,12 @@
         <v>41.765804299999999</v>
       </c>
       <c r="J89" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>50</v>
@@ -6185,7 +6179,7 @@
         <f t="shared" si="4"/>
         <v>DC</v>
       </c>
-      <c r="D90" s="20" t="s">
+      <c r="D90" s="1" t="s">
         <v>203</v>
       </c>
       <c r="E90" s="1">
@@ -6205,12 +6199,12 @@
         <v>38.907192299999998</v>
       </c>
       <c r="J90" s="21" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>51</v>
@@ -6239,22 +6233,22 @@
         <v>39.158168000000003</v>
       </c>
       <c r="J91" s="21" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>304</v>
+        <v>3</v>
       </c>
       <c r="C92" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>NM</v>
+        <v>MA</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>136</v>
+        <v>203</v>
       </c>
       <c r="E92" s="1">
         <v>1</v>
@@ -6267,13 +6261,13 @@
         <v>0</v>
       </c>
       <c r="H92" s="1">
-        <v>-105.576667</v>
+        <v>-71.058880099999996</v>
       </c>
       <c r="I92" s="1">
-        <v>36.393889000000001</v>
+        <v>42.360082499999997</v>
       </c>
       <c r="J92" s="21" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
@@ -6281,11 +6275,11 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="C93" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>MA</v>
+        <v>MD</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>203</v>
@@ -6301,13 +6295,13 @@
         <v>0</v>
       </c>
       <c r="H93" s="1">
-        <v>-71.058880099999996</v>
+        <v>-76.492182900000003</v>
       </c>
       <c r="I93" s="1">
-        <v>42.360082499999997</v>
+        <v>38.978445299999997</v>
       </c>
       <c r="J93" s="21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
@@ -6315,10 +6309,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C94" s="2" t="str">
-        <f t="shared" ref="C94:C111" si="6">RIGHT(B94,2)</f>
+        <f t="shared" ref="C94:C110" si="6">RIGHT(B94,2)</f>
         <v>MD</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -6335,13 +6329,13 @@
         <v>0</v>
       </c>
       <c r="H94" s="1">
-        <v>-76.492182900000003</v>
+        <v>-76.612189299999997</v>
       </c>
       <c r="I94" s="1">
-        <v>38.978445299999997</v>
+        <v>39.290384799999998</v>
       </c>
       <c r="J94" s="21" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
@@ -6349,11 +6343,11 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="C95" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>MD</v>
+        <v>ME</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>203</v>
@@ -6369,13 +6363,13 @@
         <v>0</v>
       </c>
       <c r="H95" s="1">
-        <v>-76.612189299999997</v>
+        <v>-69.779489699999999</v>
       </c>
       <c r="I95" s="1">
-        <v>39.290384799999998</v>
+        <v>44.310624099999998</v>
       </c>
       <c r="J95" s="21" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -6383,7 +6377,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C96" s="2" t="str">
         <f t="shared" si="6"/>
@@ -6399,17 +6393,17 @@
         <v>1</v>
       </c>
       <c r="G96" s="1">
-        <f t="shared" ref="G96:G127" si="7">((1-E96)-(1-F96))+((1-F96)*2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H96" s="1">
-        <v>-69.779489699999999</v>
+        <v>-70.256818899999999</v>
       </c>
       <c r="I96" s="1">
-        <v>44.310624099999998</v>
+        <v>43.659099300000001</v>
       </c>
       <c r="J96" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -6417,11 +6411,11 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C97" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>ME</v>
+        <v>NH</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>203</v>
@@ -6433,17 +6427,17 @@
         <v>1</v>
       </c>
       <c r="G97" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="G97:G125" si="7">((1-E97)-(1-F97))+((1-F97)*2)</f>
         <v>0</v>
       </c>
       <c r="H97" s="1">
-        <v>-70.256818899999999</v>
+        <v>-71.537571799999995</v>
       </c>
       <c r="I97" s="1">
-        <v>43.659099300000001</v>
+        <v>43.208136600000003</v>
       </c>
       <c r="J97" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -6451,11 +6445,11 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C98" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>NH</v>
+        <v>NJ</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>203</v>
@@ -6471,13 +6465,13 @@
         <v>0</v>
       </c>
       <c r="H98" s="1">
-        <v>-71.537571799999995</v>
+        <v>-74.759716999999995</v>
       </c>
       <c r="I98" s="1">
-        <v>43.208136600000003</v>
+        <v>40.220582399999998</v>
       </c>
       <c r="J98" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
@@ -6485,11 +6479,11 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C99" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>NJ</v>
+        <v>NY</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>203</v>
@@ -6505,13 +6499,13 @@
         <v>0</v>
       </c>
       <c r="H99" s="1">
-        <v>-74.759716999999995</v>
+        <v>-73.756231700000001</v>
       </c>
       <c r="I99" s="1">
-        <v>40.220582399999998</v>
+        <v>42.652579299999999</v>
       </c>
       <c r="J99" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
@@ -6519,7 +6513,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C100" s="2" t="str">
         <f t="shared" si="6"/>
@@ -6539,13 +6533,13 @@
         <v>0</v>
       </c>
       <c r="H100" s="1">
-        <v>-73.756231700000001</v>
+        <v>-78.878368899999998</v>
       </c>
       <c r="I100" s="1">
-        <v>42.652579299999999</v>
+        <v>42.886446800000002</v>
       </c>
       <c r="J100" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -6553,7 +6547,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="C101" s="2" t="str">
         <f t="shared" si="6"/>
@@ -6573,13 +6567,13 @@
         <v>0</v>
       </c>
       <c r="H101" s="1">
-        <v>-78.878368899999998</v>
+        <v>-74.005972799999995</v>
       </c>
       <c r="I101" s="1">
-        <v>42.886446800000002</v>
+        <v>40.712775299999997</v>
       </c>
       <c r="J101" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -6587,7 +6581,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>125</v>
+        <v>9</v>
       </c>
       <c r="C102" s="2" t="str">
         <f t="shared" si="6"/>
@@ -6607,13 +6601,13 @@
         <v>0</v>
       </c>
       <c r="H102" s="1">
-        <v>-74.005972799999995</v>
+        <v>-77.608846499999999</v>
       </c>
       <c r="I102" s="1">
-        <v>40.712775299999997</v>
+        <v>43.156577900000002</v>
       </c>
       <c r="J102" s="21" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
@@ -6621,11 +6615,11 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C103" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>NY</v>
+        <v>PA</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>203</v>
@@ -6641,13 +6635,13 @@
         <v>0</v>
       </c>
       <c r="H103" s="1">
-        <v>-77.608846499999999</v>
+        <v>-76.8867008</v>
       </c>
       <c r="I103" s="1">
-        <v>43.156577900000002</v>
+        <v>40.273191099999998</v>
       </c>
       <c r="J103" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
@@ -6655,7 +6649,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C104" s="2" t="str">
         <f t="shared" si="6"/>
@@ -6675,13 +6669,13 @@
         <v>0</v>
       </c>
       <c r="H104" s="1">
-        <v>-76.8867008</v>
+        <v>-75.165221500000001</v>
       </c>
       <c r="I104" s="1">
-        <v>40.273191099999998</v>
+        <v>39.9525839</v>
       </c>
       <c r="J104" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
@@ -6689,11 +6683,11 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C105" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>PA</v>
+        <v>RI</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>203</v>
@@ -6709,13 +6703,13 @@
         <v>0</v>
       </c>
       <c r="H105" s="1">
-        <v>-75.165221500000001</v>
+        <v>-71.4128343</v>
       </c>
       <c r="I105" s="1">
-        <v>39.9525839</v>
+        <v>41.823989099999999</v>
       </c>
       <c r="J105" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
@@ -6723,11 +6717,11 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C106" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>RI</v>
+        <v>VA</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>203</v>
@@ -6743,55 +6737,53 @@
         <v>0</v>
       </c>
       <c r="H106" s="1">
-        <v>-71.4128343</v>
+        <v>-78.476678100000001</v>
       </c>
       <c r="I106" s="1">
-        <v>41.823989099999999</v>
+        <v>38.029305899999997</v>
       </c>
       <c r="J106" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C107" s="2" t="str">
+      <c r="B107" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C107" s="26" t="str">
         <f t="shared" si="6"/>
         <v>VA</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="E107" s="1">
-        <v>1</v>
-      </c>
-      <c r="F107" s="1">
-        <v>1</v>
-      </c>
-      <c r="G107" s="1">
+      <c r="E107" s="18">
+        <v>1</v>
+      </c>
+      <c r="F107" s="18">
+        <v>0</v>
+      </c>
+      <c r="G107" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H107" s="1">
-        <v>-78.476678100000001</v>
-      </c>
-      <c r="I107" s="1">
-        <v>38.029305899999997</v>
-      </c>
-      <c r="J107" s="21" t="s">
-        <v>289</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H107" s="18">
+        <v>-76.285872600000005</v>
+      </c>
+      <c r="I107" s="18">
+        <v>36.850768899999998</v>
+      </c>
+      <c r="J107" s="27"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A108" s="2">
+      <c r="A108" s="26">
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C108" s="2" t="str">
         <f t="shared" si="6"/>
@@ -6804,30 +6796,32 @@
         <v>1</v>
       </c>
       <c r="F108" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H108" s="1">
-        <v>-76.285872600000005</v>
+        <v>-77.436048099999994</v>
       </c>
       <c r="I108" s="1">
-        <v>36.850768899999998</v>
-      </c>
-      <c r="J108" s="24"/>
+        <v>37.540724599999997</v>
+      </c>
+      <c r="J108" s="21" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="C109" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>VA</v>
+        <v>VT</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>203</v>
@@ -6843,13 +6837,13 @@
         <v>0</v>
       </c>
       <c r="H109" s="1">
-        <v>-77.436048099999994</v>
+        <v>-73.212072000000006</v>
       </c>
       <c r="I109" s="1">
-        <v>37.540724599999997</v>
+        <v>44.475882499999997</v>
       </c>
       <c r="J109" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -6857,7 +6851,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C110" s="2" t="str">
         <f t="shared" si="6"/>
@@ -6877,13 +6871,13 @@
         <v>0</v>
       </c>
       <c r="H110" s="1">
-        <v>-73.212072000000006</v>
+        <v>-72.575386899999998</v>
       </c>
       <c r="I110" s="1">
-        <v>44.475882499999997</v>
+        <v>44.260059300000002</v>
       </c>
       <c r="J110" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -6891,33 +6885,30 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="C111" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>VT</v>
+        <f t="shared" ref="C111:C125" si="8">RIGHT(B111,2)</f>
+        <v>OR</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>203</v>
+        <v>138</v>
       </c>
       <c r="E111" s="1">
         <v>1</v>
       </c>
       <c r="F111" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G111" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H111" s="1">
-        <v>-72.575386899999998</v>
+        <v>-122.6783853</v>
       </c>
       <c r="I111" s="1">
-        <v>44.260059300000002</v>
-      </c>
-      <c r="J111" s="21" t="s">
-        <v>289</v>
+        <v>45.515231999999997</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
@@ -6925,10 +6916,11 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>131</v>
+        <v>105</v>
+      </c>
+      <c r="C112" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>OR</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>138</v>
@@ -6944,80 +6936,81 @@
         <v>2</v>
       </c>
       <c r="H112" s="1">
-        <v>-123.1207375</v>
+        <v>-123.03509630000001</v>
       </c>
       <c r="I112" s="1">
-        <v>49.282729099999997</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+        <v>44.942897500000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C113" s="2" t="str">
-        <f t="shared" ref="C113:C127" si="8">RIGHT(B113,2)</f>
-        <v>OR</v>
+        <f t="shared" si="8"/>
+        <v>WA</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F113" s="1">
         <v>0</v>
       </c>
       <c r="G113" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H113" s="1">
-        <v>-122.6783853</v>
+        <v>-122.90069509999999</v>
       </c>
       <c r="I113" s="1">
-        <v>45.515231999999997</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+        <v>47.037874100000003</v>
+      </c>
+      <c r="J113" s="22"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C114" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>OR</v>
+        <v>WA</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E114" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F114" s="1">
         <v>0</v>
       </c>
       <c r="G114" s="1">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H114" s="1">
-        <v>-123.03509630000001</v>
+        <v>-122.3320708</v>
       </c>
       <c r="I114" s="1">
-        <v>44.942897500000001</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+        <v>47.606209499999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C115" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7037,57 +7030,59 @@
         <v>2</v>
       </c>
       <c r="H115" s="1">
-        <v>-122.90069509999999</v>
+        <v>-117.42604660000001</v>
       </c>
       <c r="I115" s="1">
-        <v>47.037874100000003</v>
-      </c>
-      <c r="J115" s="22"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+        <v>47.658780200000002</v>
+      </c>
+      <c r="J115" s="21"/>
+      <c r="L115" s="1"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C116" s="2" t="str">
+      <c r="B116" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C116" s="26" t="str">
         <f t="shared" si="8"/>
-        <v>WA</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E116" s="1">
-        <v>1</v>
-      </c>
-      <c r="F116" s="1">
-        <v>0</v>
-      </c>
-      <c r="G116" s="1">
+        <v>PR</v>
+      </c>
+      <c r="D116" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E116" s="18">
+        <v>1</v>
+      </c>
+      <c r="F116" s="18">
+        <v>0</v>
+      </c>
+      <c r="G116" s="18">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="H116" s="1">
-        <v>-122.3320708</v>
-      </c>
-      <c r="I116" s="1">
-        <v>47.606209499999999</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H116" s="18">
+        <v>-66.105735499999994</v>
+      </c>
+      <c r="I116" s="18">
+        <v>18.465539400000001</v>
+      </c>
+      <c r="J116" s="27"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C117" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>WA</v>
+        <v>CO</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E117" s="1">
         <v>0</v>
@@ -7100,53 +7095,55 @@
         <v>2</v>
       </c>
       <c r="H117" s="1">
-        <v>-117.42604660000001</v>
+        <v>-104.990251</v>
       </c>
       <c r="I117" s="1">
-        <v>47.658780200000002</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A118" s="2">
+        <v>39.739235800000003</v>
+      </c>
+      <c r="J117" s="28"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A118" s="26">
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="C118" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>PR</v>
+        <v>CO</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="E118" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F118" s="1">
         <v>0</v>
       </c>
       <c r="G118" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H118" s="1">
-        <v>-66.105735499999994</v>
+        <v>-108.5506486</v>
       </c>
       <c r="I118" s="1">
-        <v>18.465539400000001</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+        <v>39.0638705</v>
+      </c>
+      <c r="J118" s="28"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C119" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>CO</v>
+        <v>ID</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>140</v>
@@ -7162,22 +7159,23 @@
         <v>2</v>
       </c>
       <c r="H119" s="1">
-        <v>-104.990251</v>
+        <v>-116.2023137</v>
       </c>
       <c r="I119" s="1">
-        <v>39.739235800000003</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+        <v>43.615018599999999</v>
+      </c>
+      <c r="J119" s="28"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C120" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>CO</v>
+        <v>ID</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>140</v>
@@ -7193,22 +7191,23 @@
         <v>2</v>
       </c>
       <c r="H120" s="1">
-        <v>-108.5506486</v>
+        <v>-112.0407584</v>
       </c>
       <c r="I120" s="1">
-        <v>39.0638705</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+        <v>43.492660700000002</v>
+      </c>
+      <c r="J120" s="28"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C121" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>ID</v>
+        <v>MT</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>140</v>
@@ -7224,22 +7223,23 @@
         <v>2</v>
       </c>
       <c r="H121" s="1">
-        <v>-116.2023137</v>
+        <v>-108.5006904</v>
       </c>
       <c r="I121" s="1">
-        <v>43.615018599999999</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+        <v>45.783285599999999</v>
+      </c>
+      <c r="J121" s="28"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C122" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>ID</v>
+        <v>MT</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>140</v>
@@ -7255,22 +7255,23 @@
         <v>2</v>
       </c>
       <c r="H122" s="1">
-        <v>-112.0407584</v>
+        <v>-112.03910569999999</v>
       </c>
       <c r="I122" s="1">
-        <v>43.492660700000002</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+        <v>46.589145199999997</v>
+      </c>
+      <c r="J122" s="28"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C123" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>MT</v>
+        <v>UT</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>140</v>
@@ -7286,22 +7287,23 @@
         <v>2</v>
       </c>
       <c r="H123" s="1">
-        <v>-108.5006904</v>
+        <v>-111.89104740000001</v>
       </c>
       <c r="I123" s="1">
-        <v>45.783285599999999</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+        <v>40.760779300000003</v>
+      </c>
+      <c r="J123" s="28"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C124" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>MT</v>
+        <v>WY</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>140</v>
@@ -7317,22 +7319,23 @@
         <v>2</v>
       </c>
       <c r="H124" s="1">
-        <v>-112.03910569999999</v>
+        <v>-106.2980824</v>
       </c>
       <c r="I124" s="1">
-        <v>46.589145199999997</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+        <v>42.848708999999999</v>
+      </c>
+      <c r="J124" s="28"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C125" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>UT</v>
+        <v>WY</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>140</v>
@@ -7348,76 +7351,25 @@
         <v>2</v>
       </c>
       <c r="H125" s="1">
-        <v>-111.89104740000001</v>
+        <v>-104.8202462</v>
       </c>
       <c r="I125" s="1">
-        <v>40.760779300000003</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A126" s="2">
-        <v>125</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C126" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>WY</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E126" s="1">
-        <v>0</v>
-      </c>
-      <c r="F126" s="1">
-        <v>0</v>
-      </c>
-      <c r="G126" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="H126" s="1">
-        <v>-106.2980824</v>
-      </c>
-      <c r="I126" s="1">
-        <v>42.848708999999999</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A127" s="2">
-        <v>126</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C127" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>WY</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E127" s="1">
-        <v>0</v>
-      </c>
-      <c r="F127" s="1">
-        <v>0</v>
-      </c>
-      <c r="G127" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="H127" s="1">
-        <v>-104.8202462</v>
-      </c>
-      <c r="I127" s="1">
         <v>41.139981400000003</v>
       </c>
+      <c r="J125" s="28"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A126" s="2"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A127" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J127" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}"/>
+  <autoFilter ref="A1:J127" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J127">
+      <sortCondition ref="D1:D127"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I127">
     <sortCondition ref="D2:D127"/>
     <sortCondition ref="C2:C127"/>
@@ -7432,13 +7384,13 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
@@ -7453,43 +7405,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -7497,36 +7449,35 @@
         <v>139</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C2" s="1">
         <v>719</v>
       </c>
       <c r="D2" s="1">
         <f>IF(B2="None",0,2)+_xlfn.CEILING.MATH(C2/200,1)+K2</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>150</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K2" s="1">
-        <f>(3*2)+3-2</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1">
         <v>6</v>
@@ -7540,7 +7491,7 @@
         <v>126</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C3" s="1">
         <v>1056</v>
@@ -7550,22 +7501,22 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>131</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K3" s="1">
         <f>2</f>
@@ -7583,32 +7534,32 @@
         <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C4" s="1">
-        <v>1610</v>
+        <v>1255</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>211</v>
+        <v>301</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -7625,7 +7576,7 @@
         <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C5" s="1">
         <v>2211</v>
@@ -7635,22 +7586,22 @@
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>210</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -7667,32 +7618,32 @@
         <v>138</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C6" s="1">
-        <v>1955</v>
+        <v>897</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>217</v>
+        <v>304</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -7709,7 +7660,7 @@
         <v>203</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C7" s="1">
         <v>2403</v>
@@ -7719,22 +7670,22 @@
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
@@ -7751,7 +7702,7 @@
         <v>129</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C8" s="1">
         <v>2652</v>
@@ -7761,22 +7712,22 @@
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -7793,7 +7744,7 @@
         <v>132</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C9" s="1">
         <v>1963</v>
@@ -7803,13 +7754,13 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
@@ -7826,7 +7777,7 @@
         <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C10" s="1">
         <v>2339</v>
@@ -7836,22 +7787,22 @@
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -7868,7 +7819,7 @@
         <v>136</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C11" s="1">
         <f>2228+113</f>
@@ -7879,22 +7830,22 @@
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
@@ -7911,7 +7862,7 @@
         <v>137</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C12" s="1">
         <f>971+490</f>
@@ -7922,22 +7873,22 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
@@ -7954,7 +7905,7 @@
         <v>134</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C13" s="1">
         <f>1448+783</f>
@@ -7965,22 +7916,22 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
@@ -7994,36 +7945,35 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>IF(B14="None",0,2)+_xlfn.CEILING.MATH(C14/200,1)+K14</f>
+        <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>161</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K14" s="1">
-        <f>(3*2)+3-2</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L14" s="1">
         <v>2</v>
@@ -8034,36 +7984,35 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>IF(B15="None",0,2)+_xlfn.CEILING.MATH(C15/200,1)+K15</f>
+        <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>189</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K15" s="1">
-        <f>(1*2)+3-2</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L15" s="1">
         <v>2</v>
@@ -8087,22 +8036,22 @@
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H16" s="27" t="s">
-        <v>300</v>
+      <c r="H16" s="24" t="s">
+        <v>296</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K16" s="1">
         <v>0</v>
@@ -8427,7 +8376,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="L14" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="M14" s="1">
         <v>40</v>
@@ -8454,7 +8403,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="L15" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="M15" s="1">
         <f>M14+2</f>
@@ -8475,7 +8424,7 @@
       <c r="E16" s="5"/>
       <c r="G16" s="6"/>
       <c r="L16" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="M16" s="1">
         <f>M15+11</f>
@@ -8501,7 +8450,7 @@
       </c>
       <c r="E17" s="12"/>
       <c r="L17" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="M17" s="1">
         <f>M16+6</f>
@@ -8524,7 +8473,7 @@
       </c>
       <c r="D19" s="15"/>
       <c r="L19" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="M19" s="1">
         <f>M17-M14</f>
@@ -8547,13 +8496,13 @@
       </c>
       <c r="D20" s="15"/>
       <c r="L20" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="M20" s="26">
+        <v>294</v>
+      </c>
+      <c r="M20" s="23">
         <f>M19/M14</f>
         <v>0.47499999999999998</v>
       </c>
-      <c r="N20" s="26">
+      <c r="N20" s="23">
         <f>N19/N14</f>
         <v>0.12</v>
       </c>
@@ -9211,4 +9160,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AB13DC-0E22-5540-A84A-EF51CCCABDEE}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1">
+        <f t="shared" ref="F1" si="0">((1-D1)-(1-E1))+((1-E1)*2)</f>
+        <v>2</v>
+      </c>
+      <c r="G1" s="1">
+        <v>-97.138374400000004</v>
+      </c>
+      <c r="H1" s="1">
+        <v>49.895136000000001</v>
+      </c>
+      <c r="I1" s="21"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <f>((1-D2)-(1-E2))+((1-E2)*2)</f>
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>-123.1207375</v>
+      </c>
+      <c r="H2" s="1">
+        <v>49.282729099999997</v>
+      </c>
+      <c r="I2" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update map with 2023 FL trip
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60B6CE8-EE4D-184B-BA72-B786454FB0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1AB98E-8BA0-5D48-8243-C065D6A4A97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15860" yWindow="500" windowWidth="19740" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
@@ -24,18 +24,28 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="269">
   <si>
     <t>Num</t>
   </si>
@@ -839,6 +849,9 @@
   </si>
   <si>
     <t>Count of City</t>
+  </si>
+  <si>
+    <t>2023-12</t>
   </si>
 </sst>
 </file>
@@ -849,7 +862,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -901,13 +914,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="7" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -921,7 +927,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,12 +961,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,7 +1038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1075,29 +1075,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1111,90 +1101,18 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -2523,7 +2441,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA690870-6F02-8241-A4A1-03EC49FAE78F}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA690870-6F02-8241-A4A1-03EC49FAE78F}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -2614,44 +2532,44 @@
     <dataField name="Count of City" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="23">
+    <format dxfId="11">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="10">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="8">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="5">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="3">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -2967,8 +2885,8 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2982,7 +2900,7 @@
     <col min="7" max="7" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="10.83203125" style="8"/>
-    <col min="11" max="11" width="30.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5" style="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" style="3"/>
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -3018,7 +2936,7 @@
       <c r="J1" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="19" t="s">
         <v>243</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -3055,7 +2973,7 @@
       <c r="I2" s="1">
         <v>61.2180556</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -3089,7 +3007,7 @@
       <c r="I3" s="1">
         <v>58.301448999999998</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3124,7 +3042,7 @@
         <v>36.737798099999999</v>
       </c>
       <c r="J4" s="16"/>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3161,7 +3079,7 @@
       <c r="J5" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3198,7 +3116,7 @@
       <c r="J6" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3233,7 +3151,7 @@
         <v>38.5815719</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="19" t="s">
         <v>245</v>
       </c>
     </row>
@@ -3270,7 +3188,7 @@
       <c r="J8" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="19" t="s">
         <v>256</v>
       </c>
     </row>
@@ -3305,7 +3223,7 @@
         <v>37.774929499999999</v>
       </c>
       <c r="J9" s="16"/>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3340,7 +3258,7 @@
         <v>37.338208199999997</v>
       </c>
       <c r="J10" s="16"/>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3375,7 +3293,7 @@
         <v>39.163798399999997</v>
       </c>
       <c r="J11" s="16"/>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3383,34 +3301,36 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="18" t="str">
+      <c r="C12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FL</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="19">
-        <v>1</v>
-      </c>
-      <c r="F12" s="19">
-        <v>0</v>
-      </c>
-      <c r="G12" s="19">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H12" s="19">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
         <v>-81.655651000000006</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="1">
         <v>30.332183799999999</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="22" t="s">
+      <c r="J12" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K12" s="19" t="s">
         <v>256</v>
       </c>
     </row>
@@ -3418,34 +3338,36 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="18" t="str">
+      <c r="C13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FL</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E13" s="19">
-        <v>0</v>
-      </c>
-      <c r="F13" s="19">
-        <v>0</v>
-      </c>
-      <c r="G13" s="19">
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H13" s="19">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
         <v>-80.1917902</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="1">
         <v>25.7616798</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="28" t="s">
+      <c r="J13" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K13" s="31" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3453,34 +3375,36 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="18" t="str">
+      <c r="C14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FL</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E14" s="19">
-        <v>1</v>
-      </c>
-      <c r="F14" s="19">
-        <v>0</v>
-      </c>
-      <c r="G14" s="19">
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
         <v>-81.378926899999996</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="1">
         <v>28.538383199999998</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="29" t="s">
+      <c r="J14" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K14" s="25" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3488,34 +3412,36 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="18" t="str">
+      <c r="C15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FL</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="19">
-        <v>1</v>
-      </c>
-      <c r="F15" s="19">
-        <v>0</v>
-      </c>
-      <c r="G15" s="19">
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="19">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
         <v>-84.280732900000004</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="1">
         <v>30.438255900000001</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="22" t="s">
+      <c r="J15" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K15" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3523,34 +3449,36 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="18" t="str">
+      <c r="C16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FL</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E16" s="19">
-        <v>1</v>
-      </c>
-      <c r="F16" s="19">
-        <v>0</v>
-      </c>
-      <c r="G16" s="19">
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
         <v>-82.457177599999994</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="1">
         <v>27.950575000000001</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="22" t="s">
+      <c r="J16" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K16" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3587,7 +3515,7 @@
       <c r="J17" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="K17" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3624,7 +3552,7 @@
       <c r="J18" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="K18" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3661,7 +3589,7 @@
       <c r="J19" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -3698,7 +3626,7 @@
       <c r="J20" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K20" s="22" t="s">
+      <c r="K20" s="19" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3735,7 +3663,7 @@
       <c r="J21" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="K21" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3772,7 +3700,7 @@
       <c r="J22" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="K22" s="22" t="s">
+      <c r="K22" s="19" t="s">
         <v>245</v>
       </c>
     </row>
@@ -3809,7 +3737,7 @@
       <c r="J23" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K23" s="22" t="s">
+      <c r="K23" s="19" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3846,7 +3774,7 @@
       <c r="J24" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K24" s="22" t="s">
+      <c r="K24" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3883,7 +3811,7 @@
       <c r="J25" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K25" s="22" t="s">
+      <c r="K25" s="19" t="s">
         <v>264</v>
       </c>
     </row>
@@ -3920,7 +3848,7 @@
       <c r="J26" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K26" s="22" t="s">
+      <c r="K26" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -3954,7 +3882,7 @@
       <c r="I27" s="1">
         <v>21.306944399999999</v>
       </c>
-      <c r="K27" s="22" t="s">
+      <c r="K27" s="19" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3991,7 +3919,7 @@
       <c r="J28" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4028,7 +3956,7 @@
       <c r="J29" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4065,7 +3993,7 @@
       <c r="J30" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="K30" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4102,7 +4030,7 @@
       <c r="J31" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="K31" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4139,7 +4067,7 @@
       <c r="J32" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K32" s="22" t="s">
+      <c r="K32" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4176,7 +4104,7 @@
       <c r="J33" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K33" s="22" t="s">
+      <c r="K33" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4188,7 +4116,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f>RIGHT(B34,2)</f>
+        <f t="shared" ref="C34:C64" si="2">RIGHT(B34,2)</f>
         <v>MI</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -4201,7 +4129,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="1">
-        <f>((1-E34)-(1-F34))+((1-F34)*2)</f>
+        <f t="shared" ref="G34:G64" si="3">((1-E34)-(1-F34))+((1-F34)*2)</f>
         <v>0</v>
       </c>
       <c r="H34" s="1">
@@ -4213,7 +4141,7 @@
       <c r="J34" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K34" s="22" t="s">
+      <c r="K34" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4225,7 +4153,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f>RIGHT(B35,2)</f>
+        <f t="shared" si="2"/>
         <v>OH</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -4238,7 +4166,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="1">
-        <f>((1-E35)-(1-F35))+((1-F35)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H35" s="1">
@@ -4250,7 +4178,7 @@
       <c r="J35" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K35" s="22" t="s">
+      <c r="K35" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4262,7 +4190,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f>RIGHT(B36,2)</f>
+        <f t="shared" si="2"/>
         <v>OH</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -4275,7 +4203,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="1">
-        <f>((1-E36)-(1-F36))+((1-F36)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H36" s="1">
@@ -4287,7 +4215,7 @@
       <c r="J36" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K36" s="22" t="s">
+      <c r="K36" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4299,7 +4227,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f>RIGHT(B37,2)</f>
+        <f t="shared" si="2"/>
         <v>OH</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -4312,7 +4240,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="1">
-        <f>((1-E37)-(1-F37))+((1-F37)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H37" s="1">
@@ -4324,7 +4252,7 @@
       <c r="J37" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K37" s="22" t="s">
+      <c r="K37" s="19" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4336,7 +4264,7 @@
         <v>11</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f>RIGHT(B38,2)</f>
+        <f t="shared" si="2"/>
         <v>PA</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -4349,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="1">
-        <f>((1-E38)-(1-F38))+((1-F38)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H38" s="1">
@@ -4361,7 +4289,7 @@
       <c r="J38" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K38" s="22" t="s">
+      <c r="K38" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4373,7 +4301,7 @@
         <v>40</v>
       </c>
       <c r="C39" s="2" t="str">
-        <f>RIGHT(B39,2)</f>
+        <f t="shared" si="2"/>
         <v>WI</v>
       </c>
       <c r="D39" s="7" t="s">
@@ -4386,7 +4314,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="1">
-        <f>((1-E39)-(1-F39))+((1-F39)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H39" s="1">
@@ -4398,7 +4326,7 @@
       <c r="J39" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K39" s="22" t="s">
+      <c r="K39" s="19" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4410,7 +4338,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="2" t="str">
-        <f>RIGHT(B40,2)</f>
+        <f t="shared" si="2"/>
         <v>WI</v>
       </c>
       <c r="D40" s="7" t="s">
@@ -4423,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="1">
-        <f>((1-E40)-(1-F40))+((1-F40)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H40" s="1">
@@ -4435,7 +4363,7 @@
       <c r="J40" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K40" s="22" t="s">
+      <c r="K40" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4447,7 +4375,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="2" t="str">
-        <f>RIGHT(B41,2)</f>
+        <f t="shared" si="2"/>
         <v>WI</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -4460,7 +4388,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="1">
-        <f>((1-E41)-(1-F41))+((1-F41)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H41" s="1">
@@ -4472,7 +4400,7 @@
       <c r="J41" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K41" s="22" t="s">
+      <c r="K41" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4484,7 +4412,7 @@
         <v>83</v>
       </c>
       <c r="C42" s="2" t="str">
-        <f>RIGHT(B42,2)</f>
+        <f t="shared" si="2"/>
         <v>WV</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -4497,7 +4425,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="1">
-        <f>((1-E42)-(1-F42))+((1-F42)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H42" s="1">
@@ -4509,7 +4437,7 @@
       <c r="J42" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K42" s="22" t="s">
+      <c r="K42" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4521,7 +4449,7 @@
         <v>132</v>
       </c>
       <c r="C43" s="2" t="str">
-        <f>RIGHT(B43,2)</f>
+        <f t="shared" si="2"/>
         <v>AR</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -4534,7 +4462,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="1">
-        <f>((1-E43)-(1-F43))+((1-F43)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H43" s="1">
@@ -4543,7 +4471,7 @@
       <c r="I43" s="1">
         <v>34.746480900000002</v>
       </c>
-      <c r="K43" s="22" t="s">
+      <c r="K43" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4555,7 +4483,7 @@
         <v>61</v>
       </c>
       <c r="C44" s="2" t="str">
-        <f>RIGHT(B44,2)</f>
+        <f t="shared" si="2"/>
         <v>LA</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -4568,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <f>((1-E44)-(1-F44))+((1-F44)*2)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H44" s="1">
@@ -4577,7 +4505,7 @@
       <c r="I44" s="1">
         <v>30.451467699999998</v>
       </c>
-      <c r="K44" s="22" t="s">
+      <c r="K44" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4589,7 +4517,7 @@
         <v>62</v>
       </c>
       <c r="C45" s="2" t="str">
-        <f>RIGHT(B45,2)</f>
+        <f t="shared" si="2"/>
         <v>LA</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -4602,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="1">
-        <f>((1-E45)-(1-F45))+((1-F45)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H45" s="1">
@@ -4614,7 +4542,7 @@
       <c r="J45" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="K45" s="22" t="s">
+      <c r="K45" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4626,7 +4554,7 @@
         <v>65</v>
       </c>
       <c r="C46" s="2" t="str">
-        <f>RIGHT(B46,2)</f>
+        <f t="shared" si="2"/>
         <v>MS</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -4639,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="1">
-        <f>((1-E46)-(1-F46))+((1-F46)*2)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H46" s="1">
@@ -4648,7 +4576,7 @@
       <c r="I46" s="1">
         <v>32.298757299999998</v>
       </c>
-      <c r="K46" s="22" t="s">
+      <c r="K46" s="19" t="s">
         <v>249</v>
       </c>
     </row>
@@ -4660,7 +4588,7 @@
         <v>72</v>
       </c>
       <c r="C47" s="2" t="str">
-        <f>RIGHT(B47,2)</f>
+        <f t="shared" si="2"/>
         <v>TN</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -4673,7 +4601,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="1">
-        <f>((1-E47)-(1-F47))+((1-F47)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H47" s="1">
@@ -4682,7 +4610,7 @@
       <c r="I47" s="1">
         <v>35.149534299999999</v>
       </c>
-      <c r="K47" s="22" t="s">
+      <c r="K47" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4694,7 +4622,7 @@
         <v>73</v>
       </c>
       <c r="C48" s="2" t="str">
-        <f>RIGHT(B48,2)</f>
+        <f t="shared" si="2"/>
         <v>TX</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -4707,7 +4635,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="1">
-        <f>((1-E48)-(1-F48))+((1-F48)*2)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H48" s="1">
@@ -4717,10 +4645,10 @@
         <v>30.267153</v>
       </c>
       <c r="J48" s="8"/>
-      <c r="K48" s="22" t="s">
+      <c r="K48" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="L48" s="31"/>
+      <c r="L48" s="27"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -4730,7 +4658,7 @@
         <v>74</v>
       </c>
       <c r="C49" s="2" t="str">
-        <f>RIGHT(B49,2)</f>
+        <f t="shared" si="2"/>
         <v>TX</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -4743,7 +4671,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="1">
-        <f>((1-E49)-(1-F49))+((1-F49)*2)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H49" s="1">
@@ -4752,7 +4680,7 @@
       <c r="I49" s="1">
         <v>32.776664199999999</v>
       </c>
-      <c r="K49" s="22" t="s">
+      <c r="K49" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4764,7 +4692,7 @@
         <v>76</v>
       </c>
       <c r="C50" s="2" t="str">
-        <f>RIGHT(B50,2)</f>
+        <f t="shared" si="2"/>
         <v>TX</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -4777,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="1">
-        <f>((1-E50)-(1-F50))+((1-F50)*2)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H50" s="1">
@@ -4786,7 +4714,7 @@
       <c r="I50" s="1">
         <v>29.7604267</v>
       </c>
-      <c r="K50" s="22" t="s">
+      <c r="K50" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4798,7 +4726,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="2" t="str">
-        <f>RIGHT(B51,2)</f>
+        <f t="shared" si="2"/>
         <v>TX</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -4811,7 +4739,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="1">
-        <f>((1-E51)-(1-F51))+((1-F51)*2)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H51" s="1">
@@ -4820,7 +4748,7 @@
       <c r="I51" s="1">
         <v>29.424121899999999</v>
       </c>
-      <c r="K51" s="22" t="s">
+      <c r="K51" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4832,7 +4760,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="2" t="str">
-        <f>RIGHT(B52,2)</f>
+        <f t="shared" si="2"/>
         <v>MN</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -4845,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <f>((1-E52)-(1-F52))+((1-F52)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H52" s="1">
@@ -4854,7 +4782,7 @@
       <c r="I52" s="1">
         <v>44.977753</v>
       </c>
-      <c r="K52" s="22" t="s">
+      <c r="K52" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4866,7 +4794,7 @@
         <v>32</v>
       </c>
       <c r="C53" s="2" t="str">
-        <f>RIGHT(B53,2)</f>
+        <f t="shared" si="2"/>
         <v>ND</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -4879,7 +4807,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="1">
-        <f>((1-E53)-(1-F53))+((1-F53)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H53" s="1">
@@ -4888,7 +4816,7 @@
       <c r="I53" s="1">
         <v>46.808326800000003</v>
       </c>
-      <c r="K53" s="22" t="s">
+      <c r="K53" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4900,7 +4828,7 @@
         <v>33</v>
       </c>
       <c r="C54" s="2" t="str">
-        <f>RIGHT(B54,2)</f>
+        <f t="shared" si="2"/>
         <v>ND</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -4913,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="1">
-        <f>((1-E54)-(1-F54))+((1-F54)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H54" s="1">
@@ -4922,7 +4850,7 @@
       <c r="I54" s="1">
         <v>46.877186299999998</v>
       </c>
-      <c r="K54" s="22" t="s">
+      <c r="K54" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4934,7 +4862,7 @@
         <v>43</v>
       </c>
       <c r="C55" s="2" t="str">
-        <f>RIGHT(B55,2)</f>
+        <f t="shared" si="2"/>
         <v>SD</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -4947,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <f>((1-E55)-(1-F55))+((1-F55)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H55" s="1">
@@ -4956,7 +4884,7 @@
       <c r="I55" s="1">
         <v>44.366787600000002</v>
       </c>
-      <c r="K55" s="22" t="s">
+      <c r="K55" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4968,7 +4896,7 @@
         <v>42</v>
       </c>
       <c r="C56" s="2" t="str">
-        <f>RIGHT(B56,2)</f>
+        <f t="shared" si="2"/>
         <v>SD</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -4981,7 +4909,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="1">
-        <f>((1-E56)-(1-F56))+((1-F56)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H56" s="1">
@@ -4990,7 +4918,7 @@
       <c r="I56" s="1">
         <v>43.546022299999997</v>
       </c>
-      <c r="K56" s="22" t="s">
+      <c r="K56" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4998,11 +4926,11 @@
       <c r="A57" s="2">
         <v>56</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C57" s="2" t="str">
-        <f>RIGHT(B57,2)</f>
+        <f t="shared" si="2"/>
         <v>IA</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -5015,7 +4943,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="1">
-        <f>((1-E57)-(1-F57))+((1-F57)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H57" s="1">
@@ -5024,10 +4952,10 @@
       <c r="I57" s="1">
         <v>41.523643700000001</v>
       </c>
-      <c r="J57" s="26" t="s">
+      <c r="J57" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="K57" s="22" t="s">
+      <c r="K57" s="19" t="s">
         <v>254</v>
       </c>
     </row>
@@ -5039,7 +4967,7 @@
         <v>130</v>
       </c>
       <c r="C58" s="2" t="str">
-        <f>RIGHT(B58,2)</f>
+        <f t="shared" si="2"/>
         <v>IA</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -5052,7 +4980,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="1">
-        <f>((1-E58)-(1-F58))+((1-F58)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H58" s="1">
@@ -5061,10 +4989,10 @@
       <c r="I58" s="1">
         <v>41.586835299999997</v>
       </c>
-      <c r="J58" s="27" t="s">
+      <c r="J58" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="K58" s="22" t="s">
+      <c r="K58" s="19" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5076,7 +5004,7 @@
         <v>22</v>
       </c>
       <c r="C59" s="2" t="str">
-        <f>RIGHT(B59,2)</f>
+        <f t="shared" si="2"/>
         <v>IL</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -5089,7 +5017,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="1">
-        <f>((1-E59)-(1-F59))+((1-F59)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H59" s="1">
@@ -5101,7 +5029,7 @@
       <c r="J59" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K59" s="22" t="s">
+      <c r="K59" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5113,7 +5041,7 @@
         <v>23</v>
       </c>
       <c r="C60" s="2" t="str">
-        <f>RIGHT(B60,2)</f>
+        <f t="shared" si="2"/>
         <v>KS</v>
       </c>
       <c r="D60" s="6" t="s">
@@ -5126,7 +5054,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="1">
-        <f>((1-E60)-(1-F60))+((1-F60)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H60" s="1">
@@ -5138,7 +5066,7 @@
       <c r="J60" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K60" s="22" t="s">
+      <c r="K60" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5150,7 +5078,7 @@
         <v>24</v>
       </c>
       <c r="C61" s="2" t="str">
-        <f>RIGHT(B61,2)</f>
+        <f t="shared" si="2"/>
         <v>KS</v>
       </c>
       <c r="D61" s="6" t="s">
@@ -5163,7 +5091,7 @@
         <v>0</v>
       </c>
       <c r="G61" s="1">
-        <f>((1-E61)-(1-F61))+((1-F61)*2)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H61" s="1">
@@ -5172,7 +5100,7 @@
       <c r="I61" s="1">
         <v>37.687176100000002</v>
       </c>
-      <c r="K61" s="22" t="s">
+      <c r="K61" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -5184,7 +5112,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="2" t="str">
-        <f>RIGHT(B62,2)</f>
+        <f t="shared" si="2"/>
         <v>MO</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -5197,7 +5125,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="1">
-        <f>((1-E62)-(1-F62))+((1-F62)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H62" s="1">
@@ -5209,7 +5137,7 @@
       <c r="J62" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K62" s="22" t="s">
+      <c r="K62" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5221,7 +5149,7 @@
         <v>28</v>
       </c>
       <c r="C63" s="2" t="str">
-        <f>RIGHT(B63,2)</f>
+        <f t="shared" si="2"/>
         <v>MO</v>
       </c>
       <c r="D63" s="7" t="s">
@@ -5234,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="1">
-        <f>((1-E63)-(1-F63))+((1-F63)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H63" s="1">
@@ -5246,7 +5174,7 @@
       <c r="J63" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K63" s="22" t="s">
+      <c r="K63" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -5258,7 +5186,7 @@
         <v>30</v>
       </c>
       <c r="C64" s="2" t="str">
-        <f>RIGHT(B64,2)</f>
+        <f t="shared" si="2"/>
         <v>MO</v>
       </c>
       <c r="D64" s="7" t="s">
@@ -5271,7 +5199,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="1">
-        <f>((1-E64)-(1-F64))+((1-F64)*2)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H64" s="1">
@@ -5283,7 +5211,7 @@
       <c r="J64" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K64" s="22" t="s">
+      <c r="K64" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -5295,7 +5223,7 @@
         <v>35</v>
       </c>
       <c r="C65" s="2" t="str">
-        <f t="shared" ref="C65:C93" si="2">RIGHT(B65,2)</f>
+        <f t="shared" ref="C65:C93" si="4">RIGHT(B65,2)</f>
         <v>NE</v>
       </c>
       <c r="D65" s="6" t="s">
@@ -5308,7 +5236,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" ref="G65:G93" si="3">((1-E65)-(1-F65))+((1-F65)*2)</f>
+        <f t="shared" ref="G65:G93" si="5">((1-E65)-(1-F65))+((1-F65)*2)</f>
         <v>0</v>
       </c>
       <c r="H65" s="1">
@@ -5320,7 +5248,7 @@
       <c r="J65" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K65" s="22" t="s">
+      <c r="K65" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5332,7 +5260,7 @@
         <v>34</v>
       </c>
       <c r="C66" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NE</v>
       </c>
       <c r="D66" s="6" t="s">
@@ -5345,7 +5273,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H66" s="1">
@@ -5357,7 +5285,7 @@
       <c r="J66" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K66" s="22" t="s">
+      <c r="K66" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5369,7 +5297,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="D67" s="6" t="s">
@@ -5382,7 +5310,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H67" s="1">
@@ -5391,7 +5319,7 @@
       <c r="I67" s="1">
         <v>35.467560200000001</v>
       </c>
-      <c r="K67" s="22" t="s">
+      <c r="K67" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5403,7 +5331,7 @@
         <v>45</v>
       </c>
       <c r="C68" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="D68" s="6" t="s">
@@ -5416,7 +5344,7 @@
         <v>0</v>
       </c>
       <c r="G68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H68" s="1">
@@ -5425,7 +5353,7 @@
       <c r="I68" s="1">
         <v>36.153981600000002</v>
       </c>
-      <c r="K68" s="22" t="s">
+      <c r="K68" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -5437,7 +5365,7 @@
         <v>84</v>
       </c>
       <c r="C69" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>AZ</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -5450,7 +5378,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H69" s="1">
@@ -5459,7 +5387,7 @@
       <c r="I69" s="1">
         <v>33.448377100000002</v>
       </c>
-      <c r="K69" s="22" t="s">
+      <c r="K69" s="19" t="s">
         <v>245</v>
       </c>
     </row>
@@ -5471,7 +5399,7 @@
         <v>85</v>
       </c>
       <c r="C70" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>AZ</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -5484,7 +5412,7 @@
         <v>0</v>
       </c>
       <c r="G70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H70" s="1">
@@ -5493,7 +5421,7 @@
       <c r="I70" s="1">
         <v>32.222606599999999</v>
       </c>
-      <c r="K70" s="22" t="s">
+      <c r="K70" s="19" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5505,7 +5433,7 @@
         <v>100</v>
       </c>
       <c r="C71" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NM</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -5518,7 +5446,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H71" s="1">
@@ -5530,7 +5458,7 @@
       <c r="J71" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="K71" s="22" t="s">
+      <c r="K71" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5542,7 +5470,7 @@
         <v>140</v>
       </c>
       <c r="C72" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NM</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -5555,7 +5483,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H72" s="1">
@@ -5567,7 +5495,7 @@
       <c r="J72" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="K72" s="22" t="s">
+      <c r="K72" s="19" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5579,7 +5507,7 @@
         <v>234</v>
       </c>
       <c r="C73" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NM</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -5592,7 +5520,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H73" s="1">
@@ -5604,7 +5532,7 @@
       <c r="J73" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="K73" s="22" t="s">
+      <c r="K73" s="19" t="s">
         <v>255</v>
       </c>
     </row>
@@ -5616,7 +5544,7 @@
         <v>101</v>
       </c>
       <c r="C74" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NV</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -5629,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H74" s="1">
@@ -5641,7 +5569,7 @@
       <c r="J74" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="K74" s="22" t="s">
+      <c r="K74" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -5653,7 +5581,7 @@
         <v>75</v>
       </c>
       <c r="C75" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>TX</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -5666,7 +5594,7 @@
         <v>0</v>
       </c>
       <c r="G75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H75" s="1">
@@ -5675,7 +5603,7 @@
       <c r="I75" s="1">
         <v>31.761877800000001</v>
       </c>
-      <c r="K75" s="22" t="s">
+      <c r="K75" s="19" t="s">
         <v>264</v>
       </c>
     </row>
@@ -5687,7 +5615,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>CT</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -5700,7 +5628,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H76" s="1">
@@ -5712,7 +5640,7 @@
       <c r="J76" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K76" s="22" t="s">
+      <c r="K76" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5724,7 +5652,7 @@
         <v>50</v>
       </c>
       <c r="C77" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DC</v>
       </c>
       <c r="D77" s="7" t="s">
@@ -5737,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H77" s="1">
@@ -5749,7 +5677,7 @@
       <c r="J77" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="K77" s="22" t="s">
+      <c r="K77" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5761,7 +5689,7 @@
         <v>51</v>
       </c>
       <c r="C78" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DE</v>
       </c>
       <c r="D78" s="7" t="s">
@@ -5774,7 +5702,7 @@
         <v>1</v>
       </c>
       <c r="G78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H78" s="1">
@@ -5786,7 +5714,7 @@
       <c r="J78" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="K78" s="22" t="s">
+      <c r="K78" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5798,7 +5726,7 @@
         <v>3</v>
       </c>
       <c r="C79" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>MA</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -5811,7 +5739,7 @@
         <v>1</v>
       </c>
       <c r="G79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H79" s="1">
@@ -5823,7 +5751,7 @@
       <c r="J79" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K79" s="22" t="s">
+      <c r="K79" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5835,7 +5763,7 @@
         <v>63</v>
       </c>
       <c r="C80" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>MD</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -5848,7 +5776,7 @@
         <v>1</v>
       </c>
       <c r="G80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H80" s="1">
@@ -5860,7 +5788,7 @@
       <c r="J80" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="K80" s="22" t="s">
+      <c r="K80" s="19" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5872,7 +5800,7 @@
         <v>64</v>
       </c>
       <c r="C81" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>MD</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -5885,7 +5813,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H81" s="1">
@@ -5897,7 +5825,7 @@
       <c r="J81" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K81" s="22" t="s">
+      <c r="K81" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -5909,7 +5837,7 @@
         <v>4</v>
       </c>
       <c r="C82" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>ME</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -5922,7 +5850,7 @@
         <v>1</v>
       </c>
       <c r="G82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H82" s="1">
@@ -5934,7 +5862,7 @@
       <c r="J82" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K82" s="22" t="s">
+      <c r="K82" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5946,7 +5874,7 @@
         <v>5</v>
       </c>
       <c r="C83" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>ME</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -5959,7 +5887,7 @@
         <v>1</v>
       </c>
       <c r="G83" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H83" s="1">
@@ -5971,7 +5899,7 @@
       <c r="J83" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K83" s="22" t="s">
+      <c r="K83" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5983,7 +5911,7 @@
         <v>17</v>
       </c>
       <c r="C84" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NH</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -5996,7 +5924,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H84" s="1">
@@ -6008,7 +5936,7 @@
       <c r="J84" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K84" s="22" t="s">
+      <c r="K84" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6020,7 +5948,7 @@
         <v>6</v>
       </c>
       <c r="C85" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NJ</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -6033,7 +5961,7 @@
         <v>1</v>
       </c>
       <c r="G85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H85" s="1">
@@ -6045,7 +5973,7 @@
       <c r="J85" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K85" s="22" t="s">
+      <c r="K85" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6057,7 +5985,7 @@
         <v>7</v>
       </c>
       <c r="C86" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NY</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -6070,7 +5998,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H86" s="1">
@@ -6082,7 +6010,7 @@
       <c r="J86" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K86" s="22" t="s">
+      <c r="K86" s="19" t="s">
         <v>257</v>
       </c>
     </row>
@@ -6094,7 +6022,7 @@
         <v>8</v>
       </c>
       <c r="C87" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NY</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -6107,7 +6035,7 @@
         <v>1</v>
       </c>
       <c r="G87" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H87" s="1">
@@ -6119,7 +6047,7 @@
       <c r="J87" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K87" s="22" t="s">
+      <c r="K87" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -6131,7 +6059,7 @@
         <v>122</v>
       </c>
       <c r="C88" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NY</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -6144,7 +6072,7 @@
         <v>1</v>
       </c>
       <c r="G88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H88" s="1">
@@ -6156,7 +6084,7 @@
       <c r="J88" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="K88" s="22" t="s">
+      <c r="K88" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -6168,7 +6096,7 @@
         <v>9</v>
       </c>
       <c r="C89" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NY</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -6181,7 +6109,7 @@
         <v>1</v>
       </c>
       <c r="G89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H89" s="1">
@@ -6193,7 +6121,7 @@
       <c r="J89" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K89" s="22" t="s">
+      <c r="K89" s="19" t="s">
         <v>244</v>
       </c>
     </row>
@@ -6205,7 +6133,7 @@
         <v>10</v>
       </c>
       <c r="C90" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>PA</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -6218,7 +6146,7 @@
         <v>1</v>
       </c>
       <c r="G90" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H90" s="1">
@@ -6230,7 +6158,7 @@
       <c r="J90" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K90" s="22" t="s">
+      <c r="K90" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6242,7 +6170,7 @@
         <v>12</v>
       </c>
       <c r="C91" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>PA</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -6255,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="G91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H91" s="1">
@@ -6267,7 +6195,7 @@
       <c r="J91" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K91" s="22" t="s">
+      <c r="K91" s="19" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6279,7 +6207,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>RI</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -6292,7 +6220,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H92" s="1">
@@ -6304,7 +6232,7 @@
       <c r="J92" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K92" s="22" t="s">
+      <c r="K92" s="19" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6316,7 +6244,7 @@
         <v>80</v>
       </c>
       <c r="C93" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>VA</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -6329,7 +6257,7 @@
         <v>1</v>
       </c>
       <c r="G93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H93" s="1">
@@ -6341,7 +6269,7 @@
       <c r="J93" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K93" s="22" t="s">
+      <c r="K93" s="19" t="s">
         <v>255</v>
       </c>
     </row>
@@ -6353,7 +6281,7 @@
         <v>82</v>
       </c>
       <c r="C94" s="2" t="str">
-        <f>RIGHT(B94,2)</f>
+        <f t="shared" ref="C94:C111" si="6">RIGHT(B94,2)</f>
         <v>VA</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -6366,7 +6294,7 @@
         <v>1</v>
       </c>
       <c r="G94" s="1">
-        <f>((1-E94)-(1-F94))+((1-F94)*2)</f>
+        <f t="shared" ref="G94:G111" si="7">((1-E94)-(1-F94))+((1-F94)*2)</f>
         <v>0</v>
       </c>
       <c r="H94" s="1">
@@ -6378,7 +6306,7 @@
       <c r="J94" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K94" s="22" t="s">
+      <c r="K94" s="19" t="s">
         <v>256</v>
       </c>
     </row>
@@ -6390,7 +6318,7 @@
         <v>81</v>
       </c>
       <c r="C95" s="2" t="str">
-        <f>RIGHT(B95,2)</f>
+        <f t="shared" si="6"/>
         <v>VA</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -6403,7 +6331,7 @@
         <v>1</v>
       </c>
       <c r="G95" s="1">
-        <f>((1-E95)-(1-F95))+((1-F95)*2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H95" s="1">
@@ -6415,7 +6343,7 @@
       <c r="J95" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K95" s="22" t="s">
+      <c r="K95" s="19" t="s">
         <v>245</v>
       </c>
     </row>
@@ -6427,7 +6355,7 @@
         <v>14</v>
       </c>
       <c r="C96" s="2" t="str">
-        <f>RIGHT(B96,2)</f>
+        <f t="shared" si="6"/>
         <v>VT</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -6440,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="G96" s="1">
-        <f>((1-E96)-(1-F96))+((1-F96)*2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H96" s="1">
@@ -6452,7 +6380,7 @@
       <c r="J96" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K96" s="22" t="s">
+      <c r="K96" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6464,7 +6392,7 @@
         <v>15</v>
       </c>
       <c r="C97" s="2" t="str">
-        <f>RIGHT(B97,2)</f>
+        <f t="shared" si="6"/>
         <v>VT</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -6477,7 +6405,7 @@
         <v>1</v>
       </c>
       <c r="G97" s="1">
-        <f>((1-E97)-(1-F97))+((1-F97)*2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H97" s="1">
@@ -6489,7 +6417,7 @@
       <c r="J97" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="K97" s="22" t="s">
+      <c r="K97" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6501,7 +6429,7 @@
         <v>104</v>
       </c>
       <c r="C98" s="2" t="str">
-        <f>RIGHT(B98,2)</f>
+        <f t="shared" si="6"/>
         <v>OR</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -6514,7 +6442,7 @@
         <v>0</v>
       </c>
       <c r="G98" s="1">
-        <f>((1-E98)-(1-F98))+((1-F98)*2)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H98" s="1">
@@ -6523,7 +6451,7 @@
       <c r="I98" s="1">
         <v>45.515231999999997</v>
       </c>
-      <c r="K98" s="22" t="s">
+      <c r="K98" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -6535,7 +6463,7 @@
         <v>103</v>
       </c>
       <c r="C99" s="2" t="str">
-        <f>RIGHT(B99,2)</f>
+        <f t="shared" si="6"/>
         <v>OR</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -6548,7 +6476,7 @@
         <v>0</v>
       </c>
       <c r="G99" s="1">
-        <f>((1-E99)-(1-F99))+((1-F99)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H99" s="1">
@@ -6557,7 +6485,7 @@
       <c r="I99" s="1">
         <v>44.942897500000001</v>
       </c>
-      <c r="K99" s="22" t="s">
+      <c r="K99" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6569,7 +6497,7 @@
         <v>107</v>
       </c>
       <c r="C100" s="2" t="str">
-        <f>RIGHT(B100,2)</f>
+        <f t="shared" si="6"/>
         <v>WA</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -6582,7 +6510,7 @@
         <v>0</v>
       </c>
       <c r="G100" s="1">
-        <f>((1-E100)-(1-F100))+((1-F100)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H100" s="1">
@@ -6592,7 +6520,7 @@
         <v>47.037874100000003</v>
       </c>
       <c r="J100" s="9"/>
-      <c r="K100" s="22" t="s">
+      <c r="K100" s="19" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6604,7 +6532,7 @@
         <v>108</v>
       </c>
       <c r="C101" s="2" t="str">
-        <f>RIGHT(B101,2)</f>
+        <f t="shared" si="6"/>
         <v>WA</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -6617,7 +6545,7 @@
         <v>0</v>
       </c>
       <c r="G101" s="1">
-        <f>((1-E101)-(1-F101))+((1-F101)*2)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H101" s="1">
@@ -6626,7 +6554,7 @@
       <c r="I101" s="1">
         <v>47.606209499999999</v>
       </c>
-      <c r="K101" s="22" t="s">
+      <c r="K101" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -6638,7 +6566,7 @@
         <v>120</v>
       </c>
       <c r="C102" s="11" t="str">
-        <f>RIGHT(B102,2)</f>
+        <f t="shared" si="6"/>
         <v>PR</v>
       </c>
       <c r="D102" s="5" t="s">
@@ -6651,7 +6579,7 @@
         <v>0</v>
       </c>
       <c r="G102" s="5">
-        <f>((1-E102)-(1-F102))+((1-F102)*2)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H102" s="5">
@@ -6661,7 +6589,7 @@
         <v>18.465539400000001</v>
       </c>
       <c r="J102" s="13"/>
-      <c r="K102" s="22" t="s">
+      <c r="K102" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -6673,7 +6601,7 @@
         <v>94</v>
       </c>
       <c r="C103" s="2" t="str">
-        <f>RIGHT(B103,2)</f>
+        <f t="shared" si="6"/>
         <v>CO</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -6686,7 +6614,7 @@
         <v>0</v>
       </c>
       <c r="G103" s="1">
-        <f>((1-E103)-(1-F103))+((1-F103)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H103" s="1">
@@ -6696,7 +6624,7 @@
         <v>39.739235800000003</v>
       </c>
       <c r="J103" s="12"/>
-      <c r="K103" s="22" t="s">
+      <c r="K103" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -6704,11 +6632,11 @@
       <c r="A104" s="2">
         <v>103</v>
       </c>
-      <c r="B104" s="23" t="s">
+      <c r="B104" s="20" t="s">
         <v>95</v>
       </c>
       <c r="C104" s="2" t="str">
-        <f>RIGHT(B104,2)</f>
+        <f t="shared" si="6"/>
         <v>CO</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -6721,7 +6649,7 @@
         <v>0</v>
       </c>
       <c r="G104" s="1">
-        <f>((1-E104)-(1-F104))+((1-F104)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H104" s="1">
@@ -6731,7 +6659,7 @@
         <v>39.0638705</v>
       </c>
       <c r="J104" s="12"/>
-      <c r="K104" s="22" t="s">
+      <c r="K104" s="19" t="s">
         <v>254</v>
       </c>
     </row>
@@ -6743,7 +6671,7 @@
         <v>96</v>
       </c>
       <c r="C105" s="2" t="str">
-        <f>RIGHT(B105,2)</f>
+        <f t="shared" si="6"/>
         <v>ID</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -6756,7 +6684,7 @@
         <v>0</v>
       </c>
       <c r="G105" s="1">
-        <f>((1-E105)-(1-F105))+((1-F105)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H105" s="1">
@@ -6766,10 +6694,10 @@
         <v>43.615018599999999</v>
       </c>
       <c r="J105" s="12"/>
-      <c r="K105" s="22" t="s">
+      <c r="K105" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="L105" s="31"/>
+      <c r="L105" s="27"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
@@ -6779,7 +6707,7 @@
         <v>98</v>
       </c>
       <c r="C106" s="2" t="str">
-        <f>RIGHT(B106,2)</f>
+        <f t="shared" si="6"/>
         <v>MT</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -6792,7 +6720,7 @@
         <v>0</v>
       </c>
       <c r="G106" s="1">
-        <f>((1-E106)-(1-F106))+((1-F106)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H106" s="1">
@@ -6802,7 +6730,7 @@
         <v>45.783285599999999</v>
       </c>
       <c r="J106" s="12"/>
-      <c r="K106" s="22" t="s">
+      <c r="K106" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6814,7 +6742,7 @@
         <v>99</v>
       </c>
       <c r="C107" s="2" t="str">
-        <f>RIGHT(B107,2)</f>
+        <f t="shared" si="6"/>
         <v>MT</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -6827,7 +6755,7 @@
         <v>0</v>
       </c>
       <c r="G107" s="1">
-        <f>((1-E107)-(1-F107))+((1-F107)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H107" s="1">
@@ -6837,7 +6765,7 @@
         <v>46.589145199999997</v>
       </c>
       <c r="J107" s="12"/>
-      <c r="K107" s="22" t="s">
+      <c r="K107" s="19" t="s">
         <v>241</v>
       </c>
       <c r="L107" s="3"/>
@@ -6850,7 +6778,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="2" t="str">
-        <f>RIGHT(B108,2)</f>
+        <f t="shared" si="6"/>
         <v>UT</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -6863,7 +6791,7 @@
         <v>0</v>
       </c>
       <c r="G108" s="1">
-        <f>((1-E108)-(1-F108))+((1-F108)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H108" s="1">
@@ -6873,7 +6801,7 @@
         <v>40.760779300000003</v>
       </c>
       <c r="J108" s="12"/>
-      <c r="K108" s="22" t="s">
+      <c r="K108" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -6881,11 +6809,11 @@
       <c r="A109" s="2">
         <v>108</v>
       </c>
-      <c r="B109" s="23" t="s">
+      <c r="B109" s="20" t="s">
         <v>109</v>
       </c>
       <c r="C109" s="2" t="str">
-        <f>RIGHT(B109,2)</f>
+        <f t="shared" si="6"/>
         <v>WY</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -6898,7 +6826,7 @@
         <v>0</v>
       </c>
       <c r="G109" s="1">
-        <f>((1-E109)-(1-F109))+((1-F109)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H109" s="1">
@@ -6908,7 +6836,7 @@
         <v>42.848708999999999</v>
       </c>
       <c r="J109" s="12"/>
-      <c r="K109" s="22" t="s">
+      <c r="K109" s="19" t="s">
         <v>254</v>
       </c>
       <c r="L109" s="3">
@@ -6923,7 +6851,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="2" t="str">
-        <f>RIGHT(B110,2)</f>
+        <f t="shared" si="6"/>
         <v>WY</v>
       </c>
       <c r="D110" s="1" t="s">
@@ -6936,7 +6864,7 @@
         <v>0</v>
       </c>
       <c r="G110" s="1">
-        <f>((1-E110)-(1-F110))+((1-F110)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H110" s="1">
@@ -6946,7 +6874,7 @@
         <v>41.139981400000003</v>
       </c>
       <c r="J110" s="12"/>
-      <c r="K110" s="22" t="s">
+      <c r="K110" s="19" t="s">
         <v>249</v>
       </c>
     </row>
@@ -6954,11 +6882,11 @@
       <c r="A111" s="2">
         <v>110</v>
       </c>
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="20" t="s">
         <v>97</v>
       </c>
       <c r="C111" s="2" t="str">
-        <f>RIGHT(B111,2)</f>
+        <f t="shared" si="6"/>
         <v>ID</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -6971,7 +6899,7 @@
         <v>0</v>
       </c>
       <c r="G111" s="1">
-        <f>((1-E111)-(1-F111))+((1-F111)*2)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H111" s="1">
@@ -6981,7 +6909,7 @@
         <v>43.492660700000002</v>
       </c>
       <c r="J111" s="12"/>
-      <c r="K111" s="22" t="s">
+      <c r="K111" s="19" t="s">
         <v>254</v>
       </c>
       <c r="L111" s="3">
@@ -7900,30 +7828,30 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="23" t="str">
+      <c r="B10" s="20" t="str">
         <f t="shared" ref="B10:B17" si="1">RIGHT(A10,2)</f>
         <v>TX</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="25">
-        <v>0</v>
-      </c>
-      <c r="E10" s="25">
-        <v>0</v>
-      </c>
-      <c r="F10" s="25">
+      <c r="D10" s="22">
+        <v>0</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22">
         <f t="shared" ref="F10:F17" si="2">((1-D10)-(1-E10))+((1-E10)*2)</f>
         <v>2</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="22">
         <v>-98.230012400000007</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="22">
         <v>26.2034071</v>
       </c>
       <c r="J10" s="8" t="s">
@@ -7934,30 +7862,30 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="B11" s="23" t="str">
+      <c r="B11" s="20" t="str">
         <f t="shared" si="1"/>
         <v>NC</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="25">
-        <v>1</v>
-      </c>
-      <c r="E11" s="25">
-        <v>1</v>
-      </c>
-      <c r="F11" s="25">
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="22">
         <v>-80.260491999999999</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="22">
         <v>36.102764000000001</v>
       </c>
       <c r="K11" s="3">
@@ -7965,30 +7893,30 @@
       </c>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="23" t="str">
+      <c r="B12" s="20" t="str">
         <f t="shared" si="1"/>
         <v>TX</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="25">
-        <v>0</v>
-      </c>
-      <c r="E12" s="25">
-        <v>0</v>
-      </c>
-      <c r="F12" s="25">
+      <c r="D12" s="22">
+        <v>0</v>
+      </c>
+      <c r="E12" s="22">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="22">
         <v>-101.8551665</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="22">
         <v>33.577863100000002</v>
       </c>
       <c r="J12" s="8" t="s">
@@ -7999,30 +7927,30 @@
       </c>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="23" t="str">
+      <c r="B13" s="20" t="str">
         <f t="shared" si="1"/>
         <v>CA</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="25">
-        <v>1</v>
-      </c>
-      <c r="E13" s="25">
-        <v>0</v>
-      </c>
-      <c r="F13" s="25">
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="22">
+        <v>0</v>
+      </c>
+      <c r="F13" s="22">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <v>-119.69819010000001</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="22">
         <v>34.420830500000001</v>
       </c>
       <c r="K13" s="3">
@@ -8030,41 +7958,41 @@
       </c>
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="23" t="str">
+      <c r="B14" s="20" t="str">
         <f t="shared" si="1"/>
         <v>WA</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="25">
-        <v>0</v>
-      </c>
-      <c r="E14" s="25">
-        <v>0</v>
-      </c>
-      <c r="F14" s="25">
+      <c r="D14" s="22">
+        <v>0</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="22">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <v>-117.42604660000001</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="22">
         <v>47.658780200000002</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="29">
         <v>597919</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="2" t="str">
@@ -8091,7 +8019,7 @@
         <v>36.066241900000001</v>
       </c>
       <c r="I15" s="8"/>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="19" t="s">
         <v>254</v>
       </c>
       <c r="K15" s="3">
@@ -8099,7 +8027,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="2" t="str">
@@ -8126,15 +8054,15 @@
         <v>30.3674198</v>
       </c>
       <c r="I16" s="9"/>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="28">
         <v>420782</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="20" t="s">
         <v>105</v>
       </c>
       <c r="B17" s="2" t="str">
@@ -8161,10 +8089,10 @@
         <v>37.096527799999997</v>
       </c>
       <c r="I17" s="8"/>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="K17" s="33">
+      <c r="K17" s="29">
         <v>197680</v>
       </c>
     </row>
@@ -8196,13 +8124,13 @@
         <v>46.188889000000003</v>
       </c>
       <c r="I18" s="8"/>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="19" t="s">
         <v>255</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="str">
@@ -8229,7 +8157,7 @@
         <v>46.786671900000002</v>
       </c>
       <c r="I19" s="8"/>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="19" t="s">
         <v>254</v>
       </c>
       <c r="K19" s="3">
@@ -8249,48 +8177,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="24"/>
+    <col min="1" max="1" width="13.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="21" t="s">
         <v>261</v>
       </c>
     </row>
@@ -8358,136 +8286,136 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="18">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="18">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="18">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="18">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="18">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="18">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="18">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="18">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17" s="18">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="18"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="B19" s="35">
+      <c r="B19" s="18">
         <v>110</v>
       </c>
     </row>

</xml_diff>